<commit_message>
guestbook einträge erstellen und ansehen
</commit_message>
<xml_diff>
--- a/documents/Zeitplanung.xlsx
+++ b/documents/Zeitplanung.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="DieseArbeitsmappe" showPivotChartFilter="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\jonas.schmid\_BLJ\Projekte\guestbook\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Projekte\guestbook\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -422,7 +422,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -492,6 +492,18 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="83">
     <border>
@@ -2015,6 +2027,51 @@
     <xf numFmtId="0" fontId="15" fillId="10" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="12" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="11" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="10" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="2" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="32" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="74" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="7" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="48" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="18" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="4" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="13" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="12" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="82" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2056,51 +2113,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="59" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="60" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="82" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="11" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="12" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="12" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="18" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="10" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="32" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="48" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="74" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20 % - Akzent4" xfId="6" builtinId="42"/>
@@ -2519,7 +2531,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -3023,10 +3035,10 @@
   <dimension ref="A1:AN44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="10" ySplit="4" topLeftCell="K5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="4" topLeftCell="K14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="N1" sqref="N1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AF9" sqref="AF9"/>
+      <selection pane="bottomRight" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3046,38 +3058,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="167" t="s">
+      <c r="A1" s="182" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="167"/>
-      <c r="C1" s="167"/>
-      <c r="D1" s="167"/>
-      <c r="E1" s="167"/>
-      <c r="F1" s="167"/>
-      <c r="G1" s="167"/>
-      <c r="H1" s="167"/>
-      <c r="I1" s="167"/>
-      <c r="J1" s="167"/>
-      <c r="K1" s="167"/>
-      <c r="L1" s="167"/>
-      <c r="M1" s="167"/>
-      <c r="N1" s="167"/>
-      <c r="O1" s="167"/>
-      <c r="P1" s="167"/>
-      <c r="Q1" s="167"/>
-      <c r="R1" s="167"/>
-      <c r="S1" s="167"/>
-      <c r="T1" s="167"/>
-      <c r="U1" s="167"/>
-      <c r="V1" s="167"/>
-      <c r="W1" s="167"/>
-      <c r="X1" s="167"/>
-      <c r="Y1" s="167"/>
-      <c r="Z1" s="167"/>
-      <c r="AA1" s="167"/>
-      <c r="AB1" s="167"/>
-      <c r="AC1" s="167"/>
-      <c r="AD1" s="167"/>
+      <c r="B1" s="182"/>
+      <c r="C1" s="182"/>
+      <c r="D1" s="182"/>
+      <c r="E1" s="182"/>
+      <c r="F1" s="182"/>
+      <c r="G1" s="182"/>
+      <c r="H1" s="182"/>
+      <c r="I1" s="182"/>
+      <c r="J1" s="182"/>
+      <c r="K1" s="182"/>
+      <c r="L1" s="182"/>
+      <c r="M1" s="182"/>
+      <c r="N1" s="182"/>
+      <c r="O1" s="182"/>
+      <c r="P1" s="182"/>
+      <c r="Q1" s="182"/>
+      <c r="R1" s="182"/>
+      <c r="S1" s="182"/>
+      <c r="T1" s="182"/>
+      <c r="U1" s="182"/>
+      <c r="V1" s="182"/>
+      <c r="W1" s="182"/>
+      <c r="X1" s="182"/>
+      <c r="Y1" s="182"/>
+      <c r="Z1" s="182"/>
+      <c r="AA1" s="182"/>
+      <c r="AB1" s="182"/>
+      <c r="AC1" s="182"/>
+      <c r="AD1" s="182"/>
     </row>
     <row r="2" spans="1:34" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10"/>
@@ -3094,36 +3106,36 @@
     <row r="3" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="84"/>
       <c r="B3" s="88"/>
-      <c r="C3" s="169" t="s">
+      <c r="C3" s="184" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="169"/>
+      <c r="D3" s="184"/>
       <c r="E3" s="23"/>
       <c r="F3" s="24"/>
       <c r="G3" s="26"/>
       <c r="H3" s="25"/>
       <c r="I3" s="26"/>
       <c r="J3" s="23"/>
-      <c r="K3" s="169"/>
-      <c r="L3" s="169"/>
-      <c r="M3" s="169"/>
-      <c r="N3" s="169"/>
-      <c r="O3" s="170"/>
-      <c r="P3" s="168"/>
-      <c r="Q3" s="169"/>
-      <c r="R3" s="169"/>
-      <c r="S3" s="169"/>
-      <c r="T3" s="170"/>
-      <c r="U3" s="168"/>
-      <c r="V3" s="169"/>
-      <c r="W3" s="169"/>
-      <c r="X3" s="169"/>
-      <c r="Y3" s="170"/>
-      <c r="Z3" s="168"/>
-      <c r="AA3" s="169"/>
-      <c r="AB3" s="169"/>
-      <c r="AC3" s="169"/>
-      <c r="AD3" s="170"/>
+      <c r="K3" s="184"/>
+      <c r="L3" s="184"/>
+      <c r="M3" s="184"/>
+      <c r="N3" s="184"/>
+      <c r="O3" s="185"/>
+      <c r="P3" s="183"/>
+      <c r="Q3" s="184"/>
+      <c r="R3" s="184"/>
+      <c r="S3" s="184"/>
+      <c r="T3" s="185"/>
+      <c r="U3" s="183"/>
+      <c r="V3" s="184"/>
+      <c r="W3" s="184"/>
+      <c r="X3" s="184"/>
+      <c r="Y3" s="185"/>
+      <c r="Z3" s="183"/>
+      <c r="AA3" s="184"/>
+      <c r="AB3" s="184"/>
+      <c r="AC3" s="184"/>
+      <c r="AD3" s="185"/>
       <c r="AE3" s="13"/>
       <c r="AF3" s="13"/>
       <c r="AG3" s="13"/>
@@ -3424,22 +3436,22 @@
       <c r="L9" s="152"/>
       <c r="M9" s="160"/>
       <c r="N9" s="160"/>
-      <c r="O9" s="179"/>
-      <c r="P9" s="188"/>
+      <c r="O9" s="166"/>
+      <c r="P9" s="167"/>
       <c r="Q9" s="161"/>
       <c r="R9" s="152"/>
-      <c r="S9" s="183"/>
+      <c r="S9" s="168"/>
       <c r="T9" s="162"/>
-      <c r="U9" s="188"/>
+      <c r="U9" s="167"/>
       <c r="V9" s="160"/>
       <c r="W9" s="152"/>
       <c r="X9" s="49"/>
-      <c r="Y9" s="189"/>
+      <c r="Y9" s="169"/>
       <c r="Z9" s="50"/>
       <c r="AA9" s="51"/>
       <c r="AB9" s="51"/>
       <c r="AC9" s="37"/>
-      <c r="AD9" s="192"/>
+      <c r="AD9" s="170"/>
     </row>
     <row r="10" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="85">
@@ -3652,7 +3664,7 @@
       </c>
       <c r="D15" s="116">
         <f>SUM(D16:D23)</f>
-        <v>0</v>
+        <v>10.5</v>
       </c>
       <c r="E15" s="117"/>
       <c r="F15" s="118"/>
@@ -3689,11 +3701,10 @@
         <v>40</v>
       </c>
       <c r="C16" s="36">
-        <v>5</v>
-      </c>
-      <c r="D16" s="72" t="str">
-        <f>IF(SUM(K16:AD16)=0," ",SUM(K16:AD16))</f>
-        <v xml:space="preserve"> </v>
+        <v>4</v>
+      </c>
+      <c r="D16" s="72">
+        <v>2.5</v>
       </c>
       <c r="E16" s="35"/>
       <c r="F16" s="36"/>
@@ -3702,23 +3713,23 @@
       <c r="I16" s="39"/>
       <c r="J16" s="150"/>
       <c r="K16" s="151"/>
-      <c r="L16" s="180"/>
-      <c r="M16" s="180"/>
-      <c r="N16" s="178"/>
-      <c r="O16" s="179"/>
+      <c r="L16" s="164"/>
+      <c r="M16" s="164"/>
+      <c r="N16" s="177"/>
+      <c r="O16" s="166"/>
       <c r="P16" s="154"/>
-      <c r="Q16" s="180"/>
-      <c r="R16" s="180"/>
+      <c r="Q16" s="164"/>
+      <c r="R16" s="164"/>
       <c r="S16" s="155"/>
       <c r="T16" s="156"/>
       <c r="U16" s="157"/>
-      <c r="V16" s="180"/>
-      <c r="W16" s="180"/>
+      <c r="V16" s="164"/>
+      <c r="W16" s="164"/>
       <c r="X16" s="152"/>
       <c r="Y16" s="158"/>
       <c r="Z16" s="154"/>
-      <c r="AA16" s="180"/>
-      <c r="AB16" s="180"/>
+      <c r="AA16" s="164"/>
+      <c r="AB16" s="164"/>
       <c r="AC16" s="72"/>
       <c r="AD16" s="96"/>
     </row>
@@ -3730,9 +3741,11 @@
         <v>41</v>
       </c>
       <c r="C17" s="36">
-        <v>4</v>
-      </c>
-      <c r="D17" s="72"/>
+        <v>5</v>
+      </c>
+      <c r="D17" s="72">
+        <v>8</v>
+      </c>
       <c r="E17" s="35"/>
       <c r="F17" s="36"/>
       <c r="G17" s="73"/>
@@ -3740,23 +3753,23 @@
       <c r="I17" s="39"/>
       <c r="J17" s="150"/>
       <c r="K17" s="151"/>
-      <c r="L17" s="180"/>
-      <c r="M17" s="180"/>
+      <c r="L17" s="164"/>
+      <c r="M17" s="164"/>
       <c r="N17" s="152"/>
-      <c r="O17" s="179"/>
-      <c r="P17" s="179"/>
-      <c r="Q17" s="180"/>
-      <c r="R17" s="180"/>
+      <c r="O17" s="166"/>
+      <c r="P17" s="166"/>
+      <c r="Q17" s="164"/>
+      <c r="R17" s="164"/>
       <c r="S17" s="155"/>
       <c r="T17" s="156"/>
       <c r="U17" s="157"/>
-      <c r="V17" s="180"/>
-      <c r="W17" s="180"/>
+      <c r="V17" s="164"/>
+      <c r="W17" s="164"/>
       <c r="X17" s="152"/>
       <c r="Y17" s="158"/>
       <c r="Z17" s="154"/>
-      <c r="AA17" s="180"/>
-      <c r="AB17" s="180"/>
+      <c r="AA17" s="164"/>
+      <c r="AB17" s="164"/>
       <c r="AC17" s="72"/>
       <c r="AD17" s="96"/>
     </row>
@@ -3778,23 +3791,23 @@
       <c r="I18" s="39"/>
       <c r="J18" s="150"/>
       <c r="K18" s="151"/>
-      <c r="L18" s="180"/>
-      <c r="M18" s="180"/>
+      <c r="L18" s="164"/>
+      <c r="M18" s="164"/>
       <c r="N18" s="152"/>
       <c r="O18" s="153"/>
-      <c r="P18" s="184"/>
-      <c r="Q18" s="180"/>
-      <c r="R18" s="180"/>
+      <c r="P18" s="175"/>
+      <c r="Q18" s="164"/>
+      <c r="R18" s="164"/>
       <c r="S18" s="155"/>
       <c r="T18" s="155"/>
       <c r="U18" s="157"/>
-      <c r="V18" s="180"/>
-      <c r="W18" s="180"/>
+      <c r="V18" s="164"/>
+      <c r="W18" s="164"/>
       <c r="X18" s="152"/>
       <c r="Y18" s="158"/>
       <c r="Z18" s="154"/>
-      <c r="AA18" s="180"/>
-      <c r="AB18" s="180"/>
+      <c r="AA18" s="164"/>
+      <c r="AB18" s="164"/>
       <c r="AC18" s="72"/>
       <c r="AD18" s="96"/>
     </row>
@@ -3816,23 +3829,23 @@
       <c r="I19" s="158"/>
       <c r="J19" s="154"/>
       <c r="K19" s="151"/>
-      <c r="L19" s="180"/>
-      <c r="M19" s="180"/>
+      <c r="L19" s="164"/>
+      <c r="M19" s="164"/>
       <c r="N19" s="36"/>
       <c r="O19" s="73"/>
       <c r="P19" s="154"/>
-      <c r="Q19" s="180"/>
-      <c r="R19" s="180"/>
-      <c r="S19" s="184"/>
+      <c r="Q19" s="164"/>
+      <c r="R19" s="164"/>
+      <c r="S19" s="175"/>
       <c r="T19" s="156"/>
       <c r="U19" s="157"/>
-      <c r="V19" s="180"/>
-      <c r="W19" s="180"/>
+      <c r="V19" s="164"/>
+      <c r="W19" s="164"/>
       <c r="X19" s="152"/>
       <c r="Y19" s="158"/>
       <c r="Z19" s="154"/>
-      <c r="AA19" s="180"/>
-      <c r="AB19" s="180"/>
+      <c r="AA19" s="164"/>
+      <c r="AB19" s="164"/>
       <c r="AC19" s="72"/>
       <c r="AD19" s="96"/>
     </row>
@@ -3854,23 +3867,23 @@
       <c r="I20" s="158"/>
       <c r="J20" s="154"/>
       <c r="K20" s="155"/>
-      <c r="L20" s="180"/>
-      <c r="M20" s="180"/>
+      <c r="L20" s="164"/>
+      <c r="M20" s="164"/>
       <c r="N20" s="36"/>
       <c r="O20" s="73"/>
       <c r="P20" s="154"/>
-      <c r="Q20" s="180"/>
-      <c r="R20" s="180"/>
-      <c r="S20" s="182"/>
-      <c r="T20" s="182"/>
+      <c r="Q20" s="164"/>
+      <c r="R20" s="164"/>
+      <c r="S20" s="176"/>
+      <c r="T20" s="176"/>
       <c r="U20" s="73"/>
-      <c r="V20" s="180"/>
-      <c r="W20" s="180"/>
+      <c r="V20" s="164"/>
+      <c r="W20" s="164"/>
       <c r="X20" s="42"/>
       <c r="Y20" s="158"/>
       <c r="Z20" s="154"/>
-      <c r="AA20" s="180"/>
-      <c r="AB20" s="180"/>
+      <c r="AA20" s="164"/>
+      <c r="AB20" s="164"/>
       <c r="AC20" s="72"/>
       <c r="AD20" s="96"/>
     </row>
@@ -3892,23 +3905,23 @@
       <c r="I21" s="158"/>
       <c r="J21" s="154"/>
       <c r="K21" s="151"/>
-      <c r="L21" s="180"/>
-      <c r="M21" s="180"/>
+      <c r="L21" s="164"/>
+      <c r="M21" s="164"/>
       <c r="N21" s="36"/>
       <c r="O21" s="73"/>
       <c r="P21" s="154"/>
-      <c r="Q21" s="180"/>
-      <c r="R21" s="180"/>
-      <c r="S21" s="191"/>
-      <c r="T21" s="182"/>
-      <c r="U21" s="182"/>
-      <c r="V21" s="180"/>
-      <c r="W21" s="180"/>
-      <c r="X21" s="187"/>
+      <c r="Q21" s="164"/>
+      <c r="R21" s="164"/>
+      <c r="S21" s="163"/>
+      <c r="T21" s="176"/>
+      <c r="U21" s="176"/>
+      <c r="V21" s="164"/>
+      <c r="W21" s="164"/>
+      <c r="X21" s="173"/>
       <c r="Y21" s="158"/>
       <c r="Z21" s="154"/>
-      <c r="AA21" s="180"/>
-      <c r="AB21" s="180"/>
+      <c r="AA21" s="164"/>
+      <c r="AB21" s="164"/>
       <c r="AC21" s="72"/>
       <c r="AD21" s="96"/>
     </row>
@@ -3930,24 +3943,24 @@
       <c r="I22" s="158"/>
       <c r="J22" s="154"/>
       <c r="K22" s="151"/>
-      <c r="L22" s="180"/>
-      <c r="M22" s="180"/>
+      <c r="L22" s="164"/>
+      <c r="M22" s="164"/>
       <c r="N22" s="36"/>
       <c r="O22" s="73"/>
       <c r="P22" s="154"/>
-      <c r="Q22" s="180"/>
-      <c r="R22" s="180"/>
-      <c r="S22" s="191"/>
-      <c r="T22" s="191"/>
+      <c r="Q22" s="164"/>
+      <c r="R22" s="164"/>
+      <c r="S22" s="163"/>
+      <c r="T22" s="163"/>
       <c r="U22" s="36"/>
-      <c r="V22" s="180"/>
-      <c r="W22" s="180"/>
-      <c r="X22" s="187"/>
-      <c r="Y22" s="186"/>
-      <c r="Z22" s="184"/>
-      <c r="AA22" s="180"/>
-      <c r="AB22" s="180"/>
-      <c r="AC22" s="190"/>
+      <c r="V22" s="164"/>
+      <c r="W22" s="164"/>
+      <c r="X22" s="173"/>
+      <c r="Y22" s="174"/>
+      <c r="Z22" s="175"/>
+      <c r="AA22" s="164"/>
+      <c r="AB22" s="164"/>
+      <c r="AC22" s="172"/>
       <c r="AD22" s="96"/>
     </row>
     <row r="23" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3971,25 +3984,25 @@
       <c r="I23" s="39"/>
       <c r="J23" s="150"/>
       <c r="K23" s="159"/>
-      <c r="L23" s="181"/>
-      <c r="M23" s="181"/>
+      <c r="L23" s="165"/>
+      <c r="M23" s="165"/>
       <c r="N23" s="36"/>
       <c r="O23" s="73"/>
       <c r="P23" s="154"/>
-      <c r="Q23" s="181"/>
-      <c r="R23" s="180"/>
+      <c r="Q23" s="165"/>
+      <c r="R23" s="164"/>
       <c r="S23" s="161"/>
       <c r="T23" s="162"/>
       <c r="U23" s="36"/>
-      <c r="V23" s="181"/>
-      <c r="W23" s="180"/>
+      <c r="V23" s="165"/>
+      <c r="W23" s="164"/>
       <c r="X23" s="158"/>
       <c r="Y23" s="158"/>
       <c r="Z23" s="158"/>
-      <c r="AA23" s="181"/>
-      <c r="AB23" s="181"/>
-      <c r="AC23" s="185"/>
-      <c r="AD23" s="192"/>
+      <c r="AA23" s="165"/>
+      <c r="AB23" s="165"/>
+      <c r="AC23" s="171"/>
+      <c r="AD23" s="170"/>
     </row>
     <row r="24" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="112">
@@ -4509,15 +4522,15 @@
     </row>
     <row r="35" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="137"/>
-      <c r="B35" s="166"/>
-      <c r="C35" s="166"/>
-      <c r="D35" s="166"/>
-      <c r="E35" s="166"/>
-      <c r="F35" s="166"/>
-      <c r="G35" s="166"/>
-      <c r="H35" s="166"/>
-      <c r="I35" s="166"/>
-      <c r="J35" s="166"/>
+      <c r="B35" s="181"/>
+      <c r="C35" s="181"/>
+      <c r="D35" s="181"/>
+      <c r="E35" s="181"/>
+      <c r="F35" s="181"/>
+      <c r="G35" s="181"/>
+      <c r="H35" s="181"/>
+      <c r="I35" s="181"/>
+      <c r="J35" s="181"/>
     </row>
     <row r="36" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="138"/>
@@ -4532,26 +4545,26 @@
       <c r="H36" s="15"/>
       <c r="I36" s="15"/>
       <c r="J36" s="15"/>
-      <c r="K36" s="164"/>
-      <c r="L36" s="165"/>
-      <c r="M36" s="165"/>
-      <c r="N36" s="165"/>
-      <c r="O36" s="165"/>
-      <c r="P36" s="165"/>
-      <c r="Q36" s="165"/>
-      <c r="R36" s="165"/>
-      <c r="S36" s="165"/>
-      <c r="T36" s="165"/>
-      <c r="U36" s="165"/>
-      <c r="V36" s="165"/>
-      <c r="W36" s="165"/>
-      <c r="X36" s="165"/>
-      <c r="Y36" s="165"/>
-      <c r="Z36" s="165"/>
-      <c r="AA36" s="165"/>
-      <c r="AB36" s="165"/>
-      <c r="AC36" s="165"/>
-      <c r="AD36" s="165"/>
+      <c r="K36" s="179"/>
+      <c r="L36" s="180"/>
+      <c r="M36" s="180"/>
+      <c r="N36" s="180"/>
+      <c r="O36" s="180"/>
+      <c r="P36" s="180"/>
+      <c r="Q36" s="180"/>
+      <c r="R36" s="180"/>
+      <c r="S36" s="180"/>
+      <c r="T36" s="180"/>
+      <c r="U36" s="180"/>
+      <c r="V36" s="180"/>
+      <c r="W36" s="180"/>
+      <c r="X36" s="180"/>
+      <c r="Y36" s="180"/>
+      <c r="Z36" s="180"/>
+      <c r="AA36" s="180"/>
+      <c r="AB36" s="180"/>
+      <c r="AC36" s="180"/>
+      <c r="AD36" s="180"/>
     </row>
     <row r="37" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="17"/>
@@ -4564,26 +4577,26 @@
       <c r="H37" s="18"/>
       <c r="I37" s="18"/>
       <c r="J37" s="18"/>
-      <c r="K37" s="163"/>
-      <c r="L37" s="163"/>
-      <c r="M37" s="163"/>
-      <c r="N37" s="163"/>
-      <c r="O37" s="163"/>
-      <c r="P37" s="163"/>
-      <c r="Q37" s="163"/>
-      <c r="R37" s="163"/>
-      <c r="S37" s="163"/>
-      <c r="T37" s="163"/>
-      <c r="U37" s="163"/>
-      <c r="V37" s="163"/>
-      <c r="W37" s="163"/>
-      <c r="X37" s="163"/>
-      <c r="Y37" s="163"/>
-      <c r="Z37" s="163"/>
-      <c r="AA37" s="163"/>
-      <c r="AB37" s="163"/>
-      <c r="AC37" s="163"/>
-      <c r="AD37" s="163"/>
+      <c r="K37" s="178"/>
+      <c r="L37" s="178"/>
+      <c r="M37" s="178"/>
+      <c r="N37" s="178"/>
+      <c r="O37" s="178"/>
+      <c r="P37" s="178"/>
+      <c r="Q37" s="178"/>
+      <c r="R37" s="178"/>
+      <c r="S37" s="178"/>
+      <c r="T37" s="178"/>
+      <c r="U37" s="178"/>
+      <c r="V37" s="178"/>
+      <c r="W37" s="178"/>
+      <c r="X37" s="178"/>
+      <c r="Y37" s="178"/>
+      <c r="Z37" s="178"/>
+      <c r="AA37" s="178"/>
+      <c r="AB37" s="178"/>
+      <c r="AC37" s="178"/>
+      <c r="AD37" s="178"/>
     </row>
     <row r="38" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="17"/>
@@ -4596,26 +4609,26 @@
       <c r="H38" s="18"/>
       <c r="I38" s="18"/>
       <c r="J38" s="18"/>
-      <c r="K38" s="163"/>
-      <c r="L38" s="163"/>
-      <c r="M38" s="163"/>
-      <c r="N38" s="163"/>
-      <c r="O38" s="163"/>
-      <c r="P38" s="163"/>
-      <c r="Q38" s="163"/>
-      <c r="R38" s="163"/>
-      <c r="S38" s="163"/>
-      <c r="T38" s="163"/>
-      <c r="U38" s="163"/>
-      <c r="V38" s="163"/>
-      <c r="W38" s="163"/>
-      <c r="X38" s="163"/>
-      <c r="Y38" s="163"/>
-      <c r="Z38" s="163"/>
-      <c r="AA38" s="163"/>
-      <c r="AB38" s="163"/>
-      <c r="AC38" s="163"/>
-      <c r="AD38" s="163"/>
+      <c r="K38" s="178"/>
+      <c r="L38" s="178"/>
+      <c r="M38" s="178"/>
+      <c r="N38" s="178"/>
+      <c r="O38" s="178"/>
+      <c r="P38" s="178"/>
+      <c r="Q38" s="178"/>
+      <c r="R38" s="178"/>
+      <c r="S38" s="178"/>
+      <c r="T38" s="178"/>
+      <c r="U38" s="178"/>
+      <c r="V38" s="178"/>
+      <c r="W38" s="178"/>
+      <c r="X38" s="178"/>
+      <c r="Y38" s="178"/>
+      <c r="Z38" s="178"/>
+      <c r="AA38" s="178"/>
+      <c r="AB38" s="178"/>
+      <c r="AC38" s="178"/>
+      <c r="AD38" s="178"/>
     </row>
     <row r="39" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20"/>
@@ -4685,21 +4698,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="173"/>
-      <c r="B1" s="173"/>
-      <c r="C1" s="173"/>
-      <c r="D1" s="173"/>
-      <c r="E1" s="173"/>
-      <c r="F1" s="173"/>
-      <c r="G1" s="173"/>
-      <c r="H1" s="173"/>
-      <c r="I1" s="173"/>
-      <c r="J1" s="173"/>
-      <c r="K1" s="173"/>
-      <c r="L1" s="173"/>
-      <c r="M1" s="173"/>
-      <c r="N1" s="173"/>
-      <c r="O1" s="173"/>
+      <c r="A1" s="188"/>
+      <c r="B1" s="188"/>
+      <c r="C1" s="188"/>
+      <c r="D1" s="188"/>
+      <c r="E1" s="188"/>
+      <c r="F1" s="188"/>
+      <c r="G1" s="188"/>
+      <c r="H1" s="188"/>
+      <c r="I1" s="188"/>
+      <c r="J1" s="188"/>
+      <c r="K1" s="188"/>
+      <c r="L1" s="188"/>
+      <c r="M1" s="188"/>
+      <c r="N1" s="188"/>
+      <c r="O1" s="188"/>
     </row>
     <row r="2" spans="1:15" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -5005,10 +5018,10 @@
     <row r="25" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="174" t="s">
+      <c r="A27" s="189" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="175"/>
+      <c r="B27" s="190"/>
       <c r="C27" s="4" t="s">
         <v>29</v>
       </c>
@@ -5017,10 +5030,10 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="171" t="s">
+      <c r="A28" s="186" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="172"/>
+      <c r="B28" s="187"/>
       <c r="C28" s="5">
         <f>'IPA Zeitplanung'!C5</f>
         <v>0</v>
@@ -5031,10 +5044,10 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="176" t="s">
+      <c r="A29" s="191" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="177"/>
+      <c r="B29" s="192"/>
       <c r="C29" s="5">
         <f>'IPA Zeitplanung'!C11</f>
         <v>0</v>
@@ -5045,24 +5058,24 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="171" t="s">
+      <c r="A30" s="186" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="172"/>
+      <c r="B30" s="187"/>
       <c r="C30" s="5">
         <f>'IPA Zeitplanung'!C15</f>
         <v>54</v>
       </c>
       <c r="D30" s="5">
         <f>'IPA Zeitplanung'!D15</f>
-        <v>0</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="176" t="s">
+      <c r="A31" s="191" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="177"/>
+      <c r="B31" s="192"/>
       <c r="C31" s="5">
         <f>'IPA Zeitplanung'!C24</f>
         <v>0</v>
@@ -5073,10 +5086,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="171" t="s">
+      <c r="A32" s="186" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="172"/>
+      <c r="B32" s="187"/>
       <c r="C32" s="5">
         <f>'IPA Zeitplanung'!C29</f>
         <v>10.8</v>
@@ -5087,10 +5100,10 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="171" t="s">
+      <c r="A33" s="186" t="s">
         <v>10</v>
       </c>
-      <c r="B33" s="172"/>
+      <c r="B33" s="187"/>
       <c r="C33" s="5">
         <f>'IPA Zeitplanung'!C31</f>
         <v>0</v>

</xml_diff>

<commit_message>
Wochenplan verbessert datum und text sowie "" hinzugefügt
</commit_message>
<xml_diff>
--- a/documents/Zeitplanung.xlsx
+++ b/documents/Zeitplanung.xlsx
@@ -16,8 +16,8 @@
     <sheet name="Ist Arbeitszeit - Übersicht" sheetId="7" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'IPA Zeitplanung'!$A$3:$AD$34</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'IPA Zeitplanung'!$A$1:$AD$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'IPA Zeitplanung'!$A$3:$AD$38</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'IPA Zeitplanung'!$A$1:$AD$45</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Ist Arbeitszeit - Übersicht'!$A$1:$O$47</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
@@ -135,7 +135,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
   <si>
     <t>Nr.</t>
   </si>
@@ -280,6 +280,33 @@
   </si>
   <si>
     <t>F.006</t>
+  </si>
+  <si>
+    <t>Abwesend: Sonstiges</t>
+  </si>
+  <si>
+    <t>Sephir</t>
+  </si>
+  <si>
+    <t>Zeitplanung für nächste Woche erstellen und nachführen</t>
+  </si>
+  <si>
+    <t>Release 1</t>
+  </si>
+  <si>
+    <t>Release 2</t>
+  </si>
+  <si>
+    <t>Woche 1</t>
+  </si>
+  <si>
+    <t>Woche 2</t>
+  </si>
+  <si>
+    <t>Woche 3</t>
+  </si>
+  <si>
+    <t>Woche 4</t>
   </si>
 </sst>
 </file>
@@ -422,7 +449,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -504,6 +531,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="83">
     <border>
@@ -1549,7 +1582,7 @@
     <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="193">
+  <cellXfs count="197">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2006,12 +2039,6 @@
     <xf numFmtId="0" fontId="15" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="17" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2051,12 +2078,6 @@
     <xf numFmtId="0" fontId="20" fillId="14" borderId="74" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="7" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="48" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="14" borderId="18" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2070,6 +2091,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="14" borderId="82" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="50" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2113,6 +2155,9 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="59" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="60" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20 % - Akzent4" xfId="6" builtinId="42"/>
@@ -2457,13 +2502,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>54</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.8</c:v>
+                  <c:v>12.200000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2531,7 +2576,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.5</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -3032,13 +3077,13 @@
   <sheetPr codeName="Tabelle1">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:AN44"/>
+  <dimension ref="A1:AN66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="10" ySplit="4" topLeftCell="K14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="4" topLeftCell="K17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="N1" sqref="N1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomRight" activeCell="AG32" sqref="AG32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3058,38 +3103,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="182" t="s">
+      <c r="A1" s="185" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="182"/>
-      <c r="C1" s="182"/>
-      <c r="D1" s="182"/>
-      <c r="E1" s="182"/>
-      <c r="F1" s="182"/>
-      <c r="G1" s="182"/>
-      <c r="H1" s="182"/>
-      <c r="I1" s="182"/>
-      <c r="J1" s="182"/>
-      <c r="K1" s="182"/>
-      <c r="L1" s="182"/>
-      <c r="M1" s="182"/>
-      <c r="N1" s="182"/>
-      <c r="O1" s="182"/>
-      <c r="P1" s="182"/>
-      <c r="Q1" s="182"/>
-      <c r="R1" s="182"/>
-      <c r="S1" s="182"/>
-      <c r="T1" s="182"/>
-      <c r="U1" s="182"/>
-      <c r="V1" s="182"/>
-      <c r="W1" s="182"/>
-      <c r="X1" s="182"/>
-      <c r="Y1" s="182"/>
-      <c r="Z1" s="182"/>
-      <c r="AA1" s="182"/>
-      <c r="AB1" s="182"/>
-      <c r="AC1" s="182"/>
-      <c r="AD1" s="182"/>
+      <c r="B1" s="185"/>
+      <c r="C1" s="185"/>
+      <c r="D1" s="185"/>
+      <c r="E1" s="185"/>
+      <c r="F1" s="185"/>
+      <c r="G1" s="185"/>
+      <c r="H1" s="185"/>
+      <c r="I1" s="185"/>
+      <c r="J1" s="185"/>
+      <c r="K1" s="185"/>
+      <c r="L1" s="185"/>
+      <c r="M1" s="185"/>
+      <c r="N1" s="185"/>
+      <c r="O1" s="185"/>
+      <c r="P1" s="185"/>
+      <c r="Q1" s="185"/>
+      <c r="R1" s="185"/>
+      <c r="S1" s="185"/>
+      <c r="T1" s="185"/>
+      <c r="U1" s="185"/>
+      <c r="V1" s="185"/>
+      <c r="W1" s="185"/>
+      <c r="X1" s="185"/>
+      <c r="Y1" s="185"/>
+      <c r="Z1" s="185"/>
+      <c r="AA1" s="185"/>
+      <c r="AB1" s="185"/>
+      <c r="AC1" s="185"/>
+      <c r="AD1" s="185"/>
     </row>
     <row r="2" spans="1:34" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10"/>
@@ -3106,36 +3151,44 @@
     <row r="3" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="84"/>
       <c r="B3" s="88"/>
-      <c r="C3" s="184" t="s">
+      <c r="C3" s="187" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="184"/>
+      <c r="D3" s="187"/>
       <c r="E3" s="23"/>
       <c r="F3" s="24"/>
       <c r="G3" s="26"/>
       <c r="H3" s="25"/>
       <c r="I3" s="26"/>
       <c r="J3" s="23"/>
-      <c r="K3" s="184"/>
-      <c r="L3" s="184"/>
-      <c r="M3" s="184"/>
-      <c r="N3" s="184"/>
-      <c r="O3" s="185"/>
-      <c r="P3" s="183"/>
-      <c r="Q3" s="184"/>
-      <c r="R3" s="184"/>
-      <c r="S3" s="184"/>
-      <c r="T3" s="185"/>
-      <c r="U3" s="183"/>
-      <c r="V3" s="184"/>
-      <c r="W3" s="184"/>
-      <c r="X3" s="184"/>
-      <c r="Y3" s="185"/>
-      <c r="Z3" s="183"/>
-      <c r="AA3" s="184"/>
-      <c r="AB3" s="184"/>
-      <c r="AC3" s="184"/>
-      <c r="AD3" s="185"/>
+      <c r="K3" s="187" t="s">
+        <v>53</v>
+      </c>
+      <c r="L3" s="187"/>
+      <c r="M3" s="187"/>
+      <c r="N3" s="187"/>
+      <c r="O3" s="188"/>
+      <c r="P3" s="186" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q3" s="187"/>
+      <c r="R3" s="187"/>
+      <c r="S3" s="187"/>
+      <c r="T3" s="188"/>
+      <c r="U3" s="187" t="s">
+        <v>55</v>
+      </c>
+      <c r="V3" s="187"/>
+      <c r="W3" s="187"/>
+      <c r="X3" s="187"/>
+      <c r="Y3" s="188"/>
+      <c r="Z3" s="186" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA3" s="187"/>
+      <c r="AB3" s="187"/>
+      <c r="AC3" s="187"/>
+      <c r="AD3" s="188"/>
       <c r="AE3" s="13"/>
       <c r="AF3" s="13"/>
       <c r="AG3" s="13"/>
@@ -3434,24 +3487,24 @@
       <c r="J9" s="105"/>
       <c r="K9" s="129"/>
       <c r="L9" s="152"/>
-      <c r="M9" s="160"/>
-      <c r="N9" s="160"/>
-      <c r="O9" s="166"/>
-      <c r="P9" s="167"/>
-      <c r="Q9" s="161"/>
+      <c r="M9" s="158"/>
+      <c r="N9" s="158"/>
+      <c r="O9" s="164"/>
+      <c r="P9" s="165"/>
+      <c r="Q9" s="159"/>
       <c r="R9" s="152"/>
-      <c r="S9" s="168"/>
-      <c r="T9" s="162"/>
-      <c r="U9" s="167"/>
-      <c r="V9" s="160"/>
+      <c r="S9" s="166"/>
+      <c r="T9" s="160"/>
+      <c r="U9" s="165"/>
+      <c r="V9" s="158"/>
       <c r="W9" s="152"/>
       <c r="X9" s="49"/>
-      <c r="Y9" s="169"/>
+      <c r="Y9" s="167"/>
       <c r="Z9" s="50"/>
       <c r="AA9" s="51"/>
       <c r="AB9" s="51"/>
       <c r="AC9" s="37"/>
-      <c r="AD9" s="170"/>
+      <c r="AD9" s="168"/>
     </row>
     <row r="10" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="85">
@@ -3622,9 +3675,7 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E14" s="35">
-        <v>1</v>
-      </c>
+      <c r="E14" s="35"/>
       <c r="F14" s="36"/>
       <c r="G14" s="73"/>
       <c r="H14" s="38"/>
@@ -3660,11 +3711,11 @@
       </c>
       <c r="C15" s="115">
         <f>SUM(C16:C23)</f>
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="D15" s="116">
         <f>SUM(D16:D23)</f>
-        <v>10.5</v>
+        <v>24</v>
       </c>
       <c r="E15" s="117"/>
       <c r="F15" s="118"/>
@@ -3704,36 +3755,38 @@
         <v>4</v>
       </c>
       <c r="D16" s="72">
-        <v>2.5</v>
-      </c>
-      <c r="E16" s="35"/>
+        <v>6</v>
+      </c>
+      <c r="E16" s="35">
+        <v>1</v>
+      </c>
       <c r="F16" s="36"/>
       <c r="G16" s="73"/>
       <c r="H16" s="38"/>
       <c r="I16" s="39"/>
       <c r="J16" s="150"/>
       <c r="K16" s="151"/>
-      <c r="L16" s="164"/>
-      <c r="M16" s="164"/>
-      <c r="N16" s="177"/>
-      <c r="O16" s="166"/>
-      <c r="P16" s="154"/>
-      <c r="Q16" s="164"/>
-      <c r="R16" s="164"/>
-      <c r="S16" s="155"/>
-      <c r="T16" s="156"/>
-      <c r="U16" s="157"/>
-      <c r="V16" s="164"/>
-      <c r="W16" s="164"/>
-      <c r="X16" s="152"/>
-      <c r="Y16" s="158"/>
+      <c r="L16" s="162"/>
+      <c r="M16" s="162"/>
+      <c r="N16" s="173"/>
+      <c r="O16" s="164"/>
+      <c r="P16" s="171"/>
+      <c r="Q16" s="162"/>
+      <c r="R16" s="162"/>
+      <c r="S16" s="171"/>
+      <c r="T16" s="174"/>
+      <c r="U16" s="172"/>
+      <c r="V16" s="162"/>
+      <c r="W16" s="162"/>
+      <c r="X16" s="169"/>
+      <c r="Y16" s="156"/>
       <c r="Z16" s="154"/>
-      <c r="AA16" s="164"/>
-      <c r="AB16" s="164"/>
+      <c r="AA16" s="162"/>
+      <c r="AB16" s="162"/>
       <c r="AC16" s="72"/>
       <c r="AD16" s="96"/>
     </row>
-    <row r="17" spans="1:30" ht="14.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" ht="14.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A17" s="86">
         <v>32</v>
       </c>
@@ -3741,39 +3794,41 @@
         <v>41</v>
       </c>
       <c r="C17" s="36">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D17" s="72">
-        <v>8</v>
-      </c>
-      <c r="E17" s="35"/>
+        <v>18</v>
+      </c>
+      <c r="E17" s="35">
+        <v>1</v>
+      </c>
       <c r="F17" s="36"/>
       <c r="G17" s="73"/>
       <c r="H17" s="38"/>
       <c r="I17" s="39"/>
       <c r="J17" s="150"/>
       <c r="K17" s="151"/>
-      <c r="L17" s="164"/>
-      <c r="M17" s="164"/>
+      <c r="L17" s="162"/>
+      <c r="M17" s="162"/>
       <c r="N17" s="152"/>
-      <c r="O17" s="166"/>
-      <c r="P17" s="166"/>
-      <c r="Q17" s="164"/>
-      <c r="R17" s="164"/>
-      <c r="S17" s="155"/>
-      <c r="T17" s="156"/>
-      <c r="U17" s="157"/>
-      <c r="V17" s="164"/>
-      <c r="W17" s="164"/>
-      <c r="X17" s="152"/>
-      <c r="Y17" s="158"/>
-      <c r="Z17" s="154"/>
-      <c r="AA17" s="164"/>
-      <c r="AB17" s="164"/>
+      <c r="O17" s="164"/>
+      <c r="P17" s="164"/>
+      <c r="Q17" s="162"/>
+      <c r="R17" s="162"/>
+      <c r="S17" s="172"/>
+      <c r="T17" s="174"/>
+      <c r="U17" s="169"/>
+      <c r="V17" s="162"/>
+      <c r="W17" s="162"/>
+      <c r="X17" s="170"/>
+      <c r="Y17" s="169"/>
+      <c r="Z17" s="169"/>
+      <c r="AA17" s="162"/>
+      <c r="AB17" s="162"/>
       <c r="AC17" s="72"/>
       <c r="AD17" s="96"/>
     </row>
-    <row r="18" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="86">
         <v>33</v>
       </c>
@@ -3781,7 +3836,7 @@
         <v>42</v>
       </c>
       <c r="C18" s="36">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D18" s="72"/>
       <c r="E18" s="35"/>
@@ -3791,27 +3846,27 @@
       <c r="I18" s="39"/>
       <c r="J18" s="150"/>
       <c r="K18" s="151"/>
-      <c r="L18" s="164"/>
-      <c r="M18" s="164"/>
+      <c r="L18" s="162"/>
+      <c r="M18" s="162"/>
       <c r="N18" s="152"/>
       <c r="O18" s="153"/>
-      <c r="P18" s="175"/>
-      <c r="Q18" s="164"/>
-      <c r="R18" s="164"/>
+      <c r="P18" s="51"/>
+      <c r="Q18" s="162"/>
+      <c r="R18" s="162"/>
       <c r="S18" s="155"/>
-      <c r="T18" s="155"/>
-      <c r="U18" s="157"/>
-      <c r="V18" s="164"/>
-      <c r="W18" s="164"/>
+      <c r="T18" s="174"/>
+      <c r="U18" s="154"/>
+      <c r="V18" s="162"/>
+      <c r="W18" s="162"/>
       <c r="X18" s="152"/>
-      <c r="Y18" s="158"/>
-      <c r="Z18" s="154"/>
-      <c r="AA18" s="164"/>
-      <c r="AB18" s="164"/>
-      <c r="AC18" s="72"/>
+      <c r="Y18" s="156"/>
+      <c r="Z18" s="169"/>
+      <c r="AA18" s="162"/>
+      <c r="AB18" s="162"/>
+      <c r="AC18" s="169"/>
       <c r="AD18" s="96"/>
     </row>
-    <row r="19" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="86">
         <v>34</v>
       </c>
@@ -3826,30 +3881,29 @@
       <c r="F19" s="36"/>
       <c r="G19" s="73"/>
       <c r="H19" s="38"/>
-      <c r="I19" s="158"/>
+      <c r="I19" s="156"/>
       <c r="J19" s="154"/>
       <c r="K19" s="151"/>
-      <c r="L19" s="164"/>
-      <c r="M19" s="164"/>
+      <c r="L19" s="162"/>
+      <c r="M19" s="162"/>
       <c r="N19" s="36"/>
       <c r="O19" s="73"/>
       <c r="P19" s="154"/>
-      <c r="Q19" s="164"/>
-      <c r="R19" s="164"/>
-      <c r="S19" s="175"/>
-      <c r="T19" s="156"/>
-      <c r="U19" s="157"/>
-      <c r="V19" s="164"/>
-      <c r="W19" s="164"/>
+      <c r="Q19" s="162"/>
+      <c r="R19" s="162"/>
+      <c r="T19" s="174"/>
+      <c r="U19" s="154"/>
+      <c r="V19" s="162"/>
+      <c r="W19" s="162"/>
       <c r="X19" s="152"/>
-      <c r="Y19" s="158"/>
+      <c r="Y19" s="156"/>
       <c r="Z19" s="154"/>
-      <c r="AA19" s="164"/>
-      <c r="AB19" s="164"/>
+      <c r="AA19" s="162"/>
+      <c r="AB19" s="162"/>
       <c r="AC19" s="72"/>
       <c r="AD19" s="96"/>
     </row>
-    <row r="20" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="86">
         <v>35</v>
       </c>
@@ -3864,30 +3918,31 @@
       <c r="F20" s="36"/>
       <c r="G20" s="73"/>
       <c r="H20" s="38"/>
-      <c r="I20" s="158"/>
+      <c r="I20" s="156"/>
       <c r="J20" s="154"/>
       <c r="K20" s="155"/>
-      <c r="L20" s="164"/>
-      <c r="M20" s="164"/>
+      <c r="L20" s="162"/>
+      <c r="M20" s="162"/>
       <c r="N20" s="36"/>
       <c r="O20" s="73"/>
       <c r="P20" s="154"/>
-      <c r="Q20" s="164"/>
-      <c r="R20" s="164"/>
-      <c r="S20" s="176"/>
-      <c r="T20" s="176"/>
-      <c r="U20" s="73"/>
-      <c r="V20" s="164"/>
-      <c r="W20" s="164"/>
-      <c r="X20" s="42"/>
-      <c r="Y20" s="158"/>
+      <c r="Q20" s="162"/>
+      <c r="R20" s="162"/>
+      <c r="S20" s="51"/>
+      <c r="T20" s="174"/>
+      <c r="U20" s="154"/>
+      <c r="V20" s="162"/>
+      <c r="W20" s="162"/>
+      <c r="X20" s="43"/>
+      <c r="Y20" s="156"/>
       <c r="Z20" s="154"/>
-      <c r="AA20" s="164"/>
-      <c r="AB20" s="164"/>
+      <c r="AA20" s="162"/>
+      <c r="AB20" s="162"/>
       <c r="AC20" s="72"/>
       <c r="AD20" s="96"/>
-    </row>
-    <row r="21" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH20" s="73"/>
+    </row>
+    <row r="21" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="86">
         <v>36</v>
       </c>
@@ -3902,30 +3957,30 @@
       <c r="F21" s="36"/>
       <c r="G21" s="73"/>
       <c r="H21" s="38"/>
-      <c r="I21" s="158"/>
+      <c r="I21" s="156"/>
       <c r="J21" s="154"/>
       <c r="K21" s="151"/>
-      <c r="L21" s="164"/>
-      <c r="M21" s="164"/>
+      <c r="L21" s="162"/>
+      <c r="M21" s="162"/>
       <c r="N21" s="36"/>
       <c r="O21" s="73"/>
       <c r="P21" s="154"/>
-      <c r="Q21" s="164"/>
-      <c r="R21" s="164"/>
-      <c r="S21" s="163"/>
-      <c r="T21" s="176"/>
-      <c r="U21" s="176"/>
-      <c r="V21" s="164"/>
-      <c r="W21" s="164"/>
-      <c r="X21" s="173"/>
-      <c r="Y21" s="158"/>
-      <c r="Z21" s="154"/>
-      <c r="AA21" s="164"/>
-      <c r="AB21" s="164"/>
+      <c r="Q21" s="162"/>
+      <c r="R21" s="162"/>
+      <c r="S21" s="51"/>
+      <c r="T21" s="174"/>
+      <c r="U21" s="154"/>
+      <c r="V21" s="162"/>
+      <c r="W21" s="162"/>
+      <c r="X21" s="43"/>
+      <c r="Y21" s="43"/>
+      <c r="Z21" s="42"/>
+      <c r="AA21" s="162"/>
+      <c r="AB21" s="162"/>
       <c r="AC21" s="72"/>
       <c r="AD21" s="96"/>
     </row>
-    <row r="22" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="86">
         <v>37</v>
       </c>
@@ -3940,30 +3995,30 @@
       <c r="F22" s="36"/>
       <c r="G22" s="73"/>
       <c r="H22" s="38"/>
-      <c r="I22" s="158"/>
+      <c r="I22" s="156"/>
       <c r="J22" s="154"/>
       <c r="K22" s="151"/>
-      <c r="L22" s="164"/>
-      <c r="M22" s="164"/>
+      <c r="L22" s="162"/>
+      <c r="M22" s="162"/>
       <c r="N22" s="36"/>
       <c r="O22" s="73"/>
       <c r="P22" s="154"/>
-      <c r="Q22" s="164"/>
-      <c r="R22" s="164"/>
-      <c r="S22" s="163"/>
-      <c r="T22" s="163"/>
-      <c r="U22" s="36"/>
-      <c r="V22" s="164"/>
-      <c r="W22" s="164"/>
-      <c r="X22" s="173"/>
-      <c r="Y22" s="174"/>
-      <c r="Z22" s="175"/>
-      <c r="AA22" s="164"/>
-      <c r="AB22" s="164"/>
-      <c r="AC22" s="172"/>
+      <c r="Q22" s="162"/>
+      <c r="R22" s="162"/>
+      <c r="S22" s="161"/>
+      <c r="T22" s="174"/>
+      <c r="U22" s="154"/>
+      <c r="V22" s="162"/>
+      <c r="W22" s="162"/>
+      <c r="X22" s="43"/>
+      <c r="Y22" s="43"/>
+      <c r="Z22" s="42"/>
+      <c r="AA22" s="162"/>
+      <c r="AB22" s="162"/>
+      <c r="AC22" s="43"/>
       <c r="AD22" s="96"/>
     </row>
-    <row r="23" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="86">
         <v>38</v>
       </c>
@@ -3979,336 +4034,327 @@
       </c>
       <c r="E23" s="46"/>
       <c r="F23" s="36"/>
-      <c r="G23" s="73"/>
+      <c r="G23" s="36"/>
       <c r="H23" s="38"/>
       <c r="I23" s="39"/>
       <c r="J23" s="150"/>
-      <c r="K23" s="159"/>
-      <c r="L23" s="165"/>
-      <c r="M23" s="165"/>
+      <c r="K23" s="157"/>
+      <c r="L23" s="163"/>
+      <c r="M23" s="163"/>
       <c r="N23" s="36"/>
       <c r="O23" s="73"/>
       <c r="P23" s="154"/>
-      <c r="Q23" s="165"/>
-      <c r="R23" s="164"/>
-      <c r="S23" s="161"/>
-      <c r="T23" s="162"/>
-      <c r="U23" s="36"/>
-      <c r="V23" s="165"/>
-      <c r="W23" s="164"/>
-      <c r="X23" s="158"/>
-      <c r="Y23" s="158"/>
-      <c r="Z23" s="158"/>
-      <c r="AA23" s="165"/>
-      <c r="AB23" s="165"/>
-      <c r="AC23" s="171"/>
-      <c r="AD23" s="170"/>
-    </row>
-    <row r="24" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="112">
-        <v>40</v>
-      </c>
-      <c r="B24" s="113" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="115">
-        <f>SUM(C25:C28)</f>
-        <v>0</v>
-      </c>
-      <c r="D24" s="116">
-        <f>SUM(D25:D28)</f>
-        <v>0</v>
-      </c>
-      <c r="E24" s="122"/>
-      <c r="F24" s="118"/>
-      <c r="G24" s="122"/>
-      <c r="H24" s="119"/>
-      <c r="I24" s="120"/>
-      <c r="J24" s="121"/>
-      <c r="K24" s="118"/>
-      <c r="L24" s="122"/>
-      <c r="M24" s="123"/>
-      <c r="N24" s="124"/>
-      <c r="O24" s="117"/>
-      <c r="P24" s="114"/>
-      <c r="Q24" s="123"/>
-      <c r="R24" s="124"/>
-      <c r="S24" s="122"/>
-      <c r="T24" s="119"/>
-      <c r="U24" s="114"/>
-      <c r="V24" s="123"/>
-      <c r="W24" s="123"/>
-      <c r="X24" s="123"/>
-      <c r="Y24" s="119"/>
-      <c r="Z24" s="114"/>
-      <c r="AA24" s="123"/>
-      <c r="AB24" s="123"/>
-      <c r="AC24" s="124"/>
-      <c r="AD24" s="125"/>
-    </row>
-    <row r="25" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="86">
-        <v>30</v>
-      </c>
-      <c r="B25" s="98" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="36"/>
-      <c r="D25" s="72" t="str">
+      <c r="Q23" s="163"/>
+      <c r="R23" s="162"/>
+      <c r="S23" s="159"/>
+      <c r="T23" s="174"/>
+      <c r="U23" s="154"/>
+      <c r="V23" s="163"/>
+      <c r="W23" s="162"/>
+      <c r="X23" s="156"/>
+      <c r="Y23" s="43"/>
+      <c r="Z23" s="42"/>
+      <c r="AA23" s="163"/>
+      <c r="AB23" s="163"/>
+      <c r="AC23" s="43"/>
+      <c r="AD23" s="96"/>
+    </row>
+    <row r="24" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="86"/>
+      <c r="B24" s="97" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="47"/>
+      <c r="D24" s="37" t="str">
+        <f>IF(SUM(K24:AD24)=0," ",SUM(K24:AD24))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E24" s="46"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="156"/>
+      <c r="J24" s="150"/>
+      <c r="K24" s="157"/>
+      <c r="L24" s="163"/>
+      <c r="M24" s="163"/>
+      <c r="N24" s="36"/>
+      <c r="O24" s="36"/>
+      <c r="P24" s="154"/>
+      <c r="Q24" s="163"/>
+      <c r="R24" s="163"/>
+      <c r="S24" s="36"/>
+      <c r="T24" s="174"/>
+      <c r="U24" s="154"/>
+      <c r="V24" s="163"/>
+      <c r="W24" s="163"/>
+      <c r="X24" s="170"/>
+      <c r="Y24" s="43"/>
+      <c r="Z24" s="42"/>
+      <c r="AA24" s="163"/>
+      <c r="AB24" s="163"/>
+      <c r="AC24" s="43"/>
+      <c r="AD24" s="96"/>
+    </row>
+    <row r="25" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="86"/>
+      <c r="B25" s="97" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="47"/>
+      <c r="D25" s="37" t="str">
         <f>IF(SUM(K25:AD25)=0," ",SUM(K25:AD25))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E25" s="35">
-        <v>1</v>
-      </c>
+      <c r="E25" s="46"/>
       <c r="F25" s="36"/>
-      <c r="G25" s="73"/>
-      <c r="H25" s="38"/>
-      <c r="I25" s="39"/>
-      <c r="J25" s="106"/>
-      <c r="K25" s="73"/>
-      <c r="L25" s="41"/>
-      <c r="M25" s="41"/>
-      <c r="N25" s="41"/>
-      <c r="O25" s="74"/>
-      <c r="P25" s="45"/>
-      <c r="Q25" s="43"/>
-      <c r="R25" s="41"/>
-      <c r="S25" s="43"/>
-      <c r="T25" s="44"/>
-      <c r="U25" s="72"/>
-      <c r="V25" s="41"/>
-      <c r="W25" s="41"/>
-      <c r="X25" s="41"/>
-      <c r="Y25" s="36"/>
-      <c r="Z25" s="45"/>
-      <c r="AA25" s="43"/>
-      <c r="AB25" s="43"/>
+      <c r="G25" s="80"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="156"/>
+      <c r="J25" s="150"/>
+      <c r="K25" s="157"/>
+      <c r="L25" s="163"/>
+      <c r="M25" s="163"/>
+      <c r="N25" s="36"/>
+      <c r="O25" s="36"/>
+      <c r="P25" s="154"/>
+      <c r="Q25" s="163"/>
+      <c r="R25" s="163"/>
+      <c r="S25" s="36"/>
+      <c r="T25" s="174"/>
+      <c r="U25" s="154"/>
+      <c r="V25" s="163"/>
+      <c r="W25" s="163"/>
+      <c r="X25" s="43"/>
+      <c r="Y25" s="170"/>
+      <c r="Z25" s="42"/>
+      <c r="AA25" s="163"/>
+      <c r="AB25" s="163"/>
       <c r="AC25" s="43"/>
-      <c r="AD25" s="99"/>
-    </row>
-    <row r="26" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="86">
-        <v>31</v>
-      </c>
-      <c r="B26" s="98" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26" s="36"/>
-      <c r="D26" s="72" t="str">
-        <f>IF(SUM(K26:AD26)=0," ",SUM(K26:AD26))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E26" s="35">
-        <v>1</v>
-      </c>
-      <c r="F26" s="36"/>
-      <c r="G26" s="73"/>
-      <c r="H26" s="38"/>
-      <c r="I26" s="39"/>
-      <c r="J26" s="106"/>
-      <c r="K26" s="73"/>
-      <c r="L26" s="41"/>
-      <c r="M26" s="41"/>
-      <c r="N26" s="41"/>
-      <c r="O26" s="74"/>
-      <c r="P26" s="45"/>
-      <c r="Q26" s="43"/>
-      <c r="R26" s="41"/>
-      <c r="S26" s="43"/>
-      <c r="T26" s="44"/>
-      <c r="U26" s="72"/>
-      <c r="V26" s="41"/>
-      <c r="W26" s="41"/>
-      <c r="X26" s="41"/>
-      <c r="Y26" s="36"/>
-      <c r="Z26" s="45"/>
-      <c r="AA26" s="51"/>
-      <c r="AB26" s="51"/>
-      <c r="AC26" s="51"/>
-      <c r="AD26" s="100"/>
-    </row>
-    <row r="27" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD25" s="96"/>
+    </row>
+    <row r="26" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="112">
+        <v>40</v>
+      </c>
+      <c r="B26" s="113" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="115">
+        <f>SUM(C27:C30)</f>
+        <v>0</v>
+      </c>
+      <c r="D26" s="116">
+        <f>SUM(D27:D30)</f>
+        <v>0</v>
+      </c>
+      <c r="E26" s="122"/>
+      <c r="F26" s="118"/>
+      <c r="G26" s="122"/>
+      <c r="H26" s="119"/>
+      <c r="I26" s="120"/>
+      <c r="J26" s="121"/>
+      <c r="K26" s="118"/>
+      <c r="L26" s="122"/>
+      <c r="M26" s="123"/>
+      <c r="N26" s="124"/>
+      <c r="O26" s="117"/>
+      <c r="P26" s="114"/>
+      <c r="Q26" s="123"/>
+      <c r="R26" s="124"/>
+      <c r="S26" s="122"/>
+      <c r="T26" s="119"/>
+      <c r="U26" s="114"/>
+      <c r="V26" s="123"/>
+      <c r="W26" s="123"/>
+      <c r="X26" s="123"/>
+      <c r="Y26" s="119"/>
+      <c r="Z26" s="114"/>
+      <c r="AA26" s="123"/>
+      <c r="AB26" s="123"/>
+      <c r="AC26" s="124"/>
+      <c r="AD26" s="125"/>
+    </row>
+    <row r="27" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="86">
-        <v>32</v>
-      </c>
-      <c r="B27" s="101" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="68"/>
+        <v>30</v>
+      </c>
+      <c r="B27" s="98" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="36"/>
       <c r="D27" s="72" t="str">
         <f>IF(SUM(K27:AD27)=0," ",SUM(K27:AD27))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E27" s="76">
+      <c r="E27" s="35">
         <v>1</v>
       </c>
-      <c r="F27" s="48"/>
-      <c r="G27" s="56"/>
-      <c r="H27" s="53"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="73"/>
+      <c r="H27" s="38"/>
       <c r="I27" s="39"/>
       <c r="J27" s="106"/>
-      <c r="K27" s="56"/>
-      <c r="L27" s="49"/>
-      <c r="M27" s="49"/>
-      <c r="N27" s="49"/>
-      <c r="O27" s="109"/>
-      <c r="P27" s="77"/>
-      <c r="Q27" s="78"/>
-      <c r="R27" s="49"/>
-      <c r="S27" s="78"/>
-      <c r="T27" s="55"/>
-      <c r="U27" s="79"/>
-      <c r="V27" s="61"/>
-      <c r="W27" s="61"/>
-      <c r="X27" s="61"/>
-      <c r="Y27" s="80"/>
-      <c r="Z27" s="77"/>
+      <c r="K27" s="73"/>
+      <c r="L27" s="41"/>
+      <c r="M27" s="41"/>
+      <c r="N27" s="41"/>
+      <c r="O27" s="74"/>
+      <c r="P27" s="45"/>
+      <c r="Q27" s="43"/>
+      <c r="R27" s="41"/>
+      <c r="S27" s="43"/>
+      <c r="T27" s="44"/>
+      <c r="U27" s="72"/>
+      <c r="V27" s="41"/>
+      <c r="W27" s="41"/>
+      <c r="X27" s="41"/>
+      <c r="Y27" s="36"/>
+      <c r="Z27" s="45"/>
       <c r="AA27" s="43"/>
       <c r="AB27" s="43"/>
       <c r="AC27" s="43"/>
-      <c r="AD27" s="93"/>
-    </row>
-    <row r="28" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="85">
-        <v>33</v>
-      </c>
-      <c r="B28" s="101" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" s="58"/>
-      <c r="D28" s="67" t="str">
+      <c r="AD27" s="99"/>
+    </row>
+    <row r="28" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="86">
+        <v>31</v>
+      </c>
+      <c r="B28" s="98" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="36"/>
+      <c r="D28" s="72" t="str">
         <f>IF(SUM(K28:AD28)=0," ",SUM(K28:AD28))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E28" s="57">
-        <v>2</v>
-      </c>
-      <c r="F28" s="68"/>
-      <c r="G28" s="80"/>
-      <c r="H28" s="69"/>
+      <c r="E28" s="35">
+        <v>1</v>
+      </c>
+      <c r="F28" s="36"/>
+      <c r="G28" s="73"/>
+      <c r="H28" s="38"/>
       <c r="I28" s="39"/>
-      <c r="J28" s="107"/>
-      <c r="K28" s="65"/>
-      <c r="L28" s="60"/>
-      <c r="M28" s="60"/>
-      <c r="N28" s="60"/>
-      <c r="O28" s="70"/>
-      <c r="P28" s="66"/>
-      <c r="Q28" s="63"/>
-      <c r="R28" s="61"/>
-      <c r="S28" s="63"/>
-      <c r="T28" s="64"/>
-      <c r="U28" s="67"/>
-      <c r="V28" s="60"/>
-      <c r="W28" s="71"/>
-      <c r="X28" s="60"/>
-      <c r="Y28" s="65"/>
-      <c r="Z28" s="66"/>
-      <c r="AA28" s="63"/>
-      <c r="AB28" s="63"/>
-      <c r="AC28" s="63"/>
-      <c r="AD28" s="102"/>
-    </row>
-    <row r="29" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="112">
-        <v>50</v>
-      </c>
-      <c r="B29" s="113" t="s">
-        <v>13</v>
-      </c>
-      <c r="C29" s="115">
-        <f>SUM(C30)</f>
-        <v>10.8</v>
-      </c>
-      <c r="D29" s="116">
-        <f>SUM(D30)</f>
-        <v>0</v>
-      </c>
-      <c r="E29" s="117"/>
-      <c r="F29" s="118"/>
-      <c r="G29" s="122"/>
-      <c r="H29" s="119"/>
-      <c r="I29" s="120"/>
-      <c r="J29" s="121"/>
-      <c r="K29" s="118"/>
-      <c r="L29" s="122"/>
-      <c r="M29" s="123"/>
-      <c r="N29" s="124"/>
-      <c r="O29" s="117"/>
-      <c r="P29" s="114"/>
-      <c r="Q29" s="123"/>
-      <c r="R29" s="124"/>
-      <c r="S29" s="122"/>
-      <c r="T29" s="119"/>
-      <c r="U29" s="114"/>
-      <c r="V29" s="123"/>
-      <c r="W29" s="123"/>
-      <c r="X29" s="123"/>
-      <c r="Y29" s="119"/>
-      <c r="Z29" s="114"/>
-      <c r="AA29" s="123"/>
-      <c r="AB29" s="123"/>
-      <c r="AC29" s="124"/>
-      <c r="AD29" s="125"/>
-    </row>
-    <row r="30" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="87">
-        <v>51</v>
+      <c r="J28" s="106"/>
+      <c r="K28" s="73"/>
+      <c r="L28" s="41"/>
+      <c r="M28" s="41"/>
+      <c r="N28" s="41"/>
+      <c r="O28" s="74"/>
+      <c r="P28" s="45"/>
+      <c r="Q28" s="43"/>
+      <c r="R28" s="41"/>
+      <c r="S28" s="43"/>
+      <c r="T28" s="44"/>
+      <c r="U28" s="72"/>
+      <c r="V28" s="41"/>
+      <c r="W28" s="41"/>
+      <c r="X28" s="41"/>
+      <c r="Y28" s="36"/>
+      <c r="Z28" s="45"/>
+      <c r="AA28" s="51"/>
+      <c r="AB28" s="51"/>
+      <c r="AC28" s="51"/>
+      <c r="AD28" s="100"/>
+    </row>
+    <row r="29" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="86">
+        <v>32</v>
+      </c>
+      <c r="B29" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="68"/>
+      <c r="D29" s="72" t="str">
+        <f>IF(SUM(K29:AD29)=0," ",SUM(K29:AD29))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E29" s="76">
+        <v>1</v>
+      </c>
+      <c r="F29" s="48"/>
+      <c r="G29" s="56"/>
+      <c r="H29" s="53"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="106"/>
+      <c r="K29" s="56"/>
+      <c r="L29" s="49"/>
+      <c r="M29" s="49"/>
+      <c r="N29" s="49"/>
+      <c r="O29" s="109"/>
+      <c r="P29" s="77"/>
+      <c r="Q29" s="78"/>
+      <c r="R29" s="49"/>
+      <c r="S29" s="78"/>
+      <c r="T29" s="55"/>
+      <c r="U29" s="79"/>
+      <c r="V29" s="61"/>
+      <c r="W29" s="61"/>
+      <c r="X29" s="61"/>
+      <c r="Y29" s="80"/>
+      <c r="Z29" s="77"/>
+      <c r="AA29" s="43"/>
+      <c r="AB29" s="43"/>
+      <c r="AC29" s="43"/>
+      <c r="AD29" s="93"/>
+      <c r="AI29" s="196" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="85">
+        <v>33</v>
       </c>
       <c r="B30" s="101" t="s">
-        <v>6</v>
-      </c>
-      <c r="C30" s="68">
-        <f>(C5+C11+C15+C24)*0.2</f>
-        <v>10.8</v>
-      </c>
-      <c r="D30" s="79" t="str">
+        <v>27</v>
+      </c>
+      <c r="C30" s="58"/>
+      <c r="D30" s="67" t="str">
         <f>IF(SUM(K30:AD30)=0," ",SUM(K30:AD30))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E30" s="76">
-        <v>3</v>
+      <c r="E30" s="57">
+        <v>2</v>
       </c>
       <c r="F30" s="68"/>
       <c r="G30" s="80"/>
       <c r="H30" s="69"/>
       <c r="I30" s="39"/>
-      <c r="J30" s="105"/>
-      <c r="K30" s="80"/>
-      <c r="L30" s="61"/>
-      <c r="M30" s="61"/>
-      <c r="N30" s="61"/>
-      <c r="O30" s="109"/>
-      <c r="P30" s="77"/>
-      <c r="Q30" s="78"/>
+      <c r="J30" s="107"/>
+      <c r="K30" s="65"/>
+      <c r="L30" s="60"/>
+      <c r="M30" s="60"/>
+      <c r="N30" s="60"/>
+      <c r="O30" s="70"/>
+      <c r="P30" s="66"/>
+      <c r="Q30" s="63"/>
       <c r="R30" s="61"/>
-      <c r="S30" s="78"/>
-      <c r="T30" s="55"/>
-      <c r="U30" s="79"/>
-      <c r="V30" s="61"/>
-      <c r="W30" s="61"/>
-      <c r="X30" s="61"/>
-      <c r="Y30" s="69"/>
-      <c r="Z30" s="81"/>
-      <c r="AA30" s="78"/>
-      <c r="AB30" s="78"/>
-      <c r="AC30" s="78"/>
-      <c r="AD30" s="93"/>
-    </row>
-    <row r="31" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S30" s="63"/>
+      <c r="T30" s="64"/>
+      <c r="U30" s="67"/>
+      <c r="V30" s="60"/>
+      <c r="W30" s="71"/>
+      <c r="X30" s="60"/>
+      <c r="Y30" s="65"/>
+      <c r="Z30" s="66"/>
+      <c r="AA30" s="63"/>
+      <c r="AB30" s="63"/>
+      <c r="AC30" s="63"/>
+      <c r="AD30" s="102"/>
+    </row>
+    <row r="31" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="112">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B31" s="113" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C31" s="115">
-        <f>SUM(C32:C33)</f>
-        <v>0</v>
+        <f>SUM(C32)</f>
+        <v>12.200000000000001</v>
       </c>
       <c r="D31" s="116">
-        <f>SUM(D32:D33)</f>
+        <f>SUM(D32)</f>
         <v>0</v>
       </c>
       <c r="E31" s="117"/>
@@ -4338,326 +4384,566 @@
       <c r="AC31" s="124"/>
       <c r="AD31" s="125"/>
     </row>
-    <row r="32" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="86">
-        <v>61</v>
-      </c>
-      <c r="B32" s="97" t="s">
-        <v>35</v>
-      </c>
-      <c r="C32" s="36"/>
-      <c r="D32" s="72" t="str">
+    <row r="32" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="87">
+        <v>51</v>
+      </c>
+      <c r="B32" s="101" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="68">
+        <f>(C5+C11+C15+C26)*0.2</f>
+        <v>12.200000000000001</v>
+      </c>
+      <c r="D32" s="79" t="str">
         <f>IF(SUM(K32:AD32)=0," ",SUM(K32:AD32))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E32" s="35">
-        <v>2</v>
-      </c>
-      <c r="F32" s="36"/>
-      <c r="G32" s="73"/>
-      <c r="H32" s="38"/>
+      <c r="E32" s="76">
+        <v>3</v>
+      </c>
+      <c r="F32" s="68"/>
+      <c r="G32" s="80"/>
+      <c r="H32" s="69"/>
       <c r="I32" s="39"/>
-      <c r="J32" s="110"/>
-      <c r="K32" s="73"/>
-      <c r="L32" s="41"/>
-      <c r="M32" s="41"/>
-      <c r="N32" s="41"/>
-      <c r="O32" s="74"/>
-      <c r="P32" s="45"/>
-      <c r="Q32" s="43"/>
-      <c r="R32" s="41"/>
-      <c r="S32" s="43"/>
-      <c r="T32" s="44"/>
-      <c r="U32" s="72"/>
-      <c r="V32" s="41"/>
-      <c r="W32" s="41"/>
-      <c r="X32" s="41"/>
-      <c r="Y32" s="73"/>
-      <c r="Z32" s="42"/>
-      <c r="AA32" s="43"/>
-      <c r="AB32" s="43"/>
-      <c r="AC32" s="43"/>
-      <c r="AD32" s="100"/>
+      <c r="J32" s="105"/>
+      <c r="K32" s="80"/>
+      <c r="L32" s="61"/>
+      <c r="M32" s="61"/>
+      <c r="N32" s="61"/>
+      <c r="O32" s="109"/>
+      <c r="P32" s="77"/>
+      <c r="Q32" s="78"/>
+      <c r="R32" s="61"/>
+      <c r="S32" s="78"/>
+      <c r="T32" s="55"/>
+      <c r="U32" s="79"/>
+      <c r="V32" s="61"/>
+      <c r="W32" s="61"/>
+      <c r="X32" s="61"/>
+      <c r="Y32" s="69"/>
+      <c r="Z32" s="81"/>
+      <c r="AA32" s="78"/>
+      <c r="AB32" s="78"/>
+      <c r="AC32" s="78"/>
+      <c r="AD32" s="93"/>
     </row>
     <row r="33" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="85">
-        <v>62</v>
-      </c>
-      <c r="B33" s="98" t="s">
-        <v>36</v>
-      </c>
-      <c r="C33" s="47"/>
-      <c r="D33" s="37" t="str">
+      <c r="A33" s="87">
+        <v>52</v>
+      </c>
+      <c r="B33" s="175" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="80">
+        <v>0.5</v>
+      </c>
+      <c r="D33" s="79" t="str">
         <f>IF(SUM(K33:AD33)=0," ",SUM(K33:AD33))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E33" s="46">
-        <v>1</v>
-      </c>
-      <c r="F33" s="82"/>
-      <c r="G33" s="139"/>
-      <c r="H33" s="83"/>
-      <c r="I33" s="39"/>
-      <c r="J33" s="108"/>
-      <c r="K33" s="56"/>
-      <c r="L33" s="49"/>
-      <c r="M33" s="49"/>
-      <c r="N33" s="49"/>
-      <c r="O33" s="74"/>
-      <c r="P33" s="75"/>
-      <c r="Q33" s="51"/>
-      <c r="R33" s="41"/>
-      <c r="S33" s="51"/>
-      <c r="T33" s="52"/>
-      <c r="U33" s="37"/>
-      <c r="V33" s="49"/>
-      <c r="W33" s="41"/>
-      <c r="X33" s="49"/>
-      <c r="Y33" s="56"/>
-      <c r="Z33" s="50"/>
-      <c r="AA33" s="51"/>
-      <c r="AB33" s="51"/>
-      <c r="AC33" s="51"/>
-      <c r="AD33" s="100"/>
-    </row>
-    <row r="34" spans="1:30" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="111"/>
-      <c r="B34" s="130" t="s">
-        <v>7</v>
-      </c>
-      <c r="C34" s="131">
-        <f>SUM(C5+C11+C15+C24+C31)</f>
-        <v>54</v>
-      </c>
-      <c r="D34" s="131" t="str">
+      <c r="E33" s="76"/>
+      <c r="F33" s="68"/>
+      <c r="G33" s="80"/>
+      <c r="H33" s="69"/>
+      <c r="I33" s="176"/>
+      <c r="J33" s="177"/>
+      <c r="K33" s="80"/>
+      <c r="L33" s="178"/>
+      <c r="M33" s="179"/>
+      <c r="N33" s="61"/>
+      <c r="O33" s="55"/>
+      <c r="P33" s="77"/>
+      <c r="Q33" s="79"/>
+      <c r="R33" s="61"/>
+      <c r="S33" s="80"/>
+      <c r="T33" s="55"/>
+      <c r="U33" s="80"/>
+      <c r="V33" s="179"/>
+      <c r="W33" s="179"/>
+      <c r="X33" s="41"/>
+      <c r="Y33" s="170"/>
+      <c r="Z33" s="77"/>
+      <c r="AA33" s="79"/>
+      <c r="AB33" s="79"/>
+      <c r="AC33" s="43"/>
+      <c r="AD33" s="170"/>
+    </row>
+    <row r="34" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="87"/>
+      <c r="B34" s="175" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34" s="80">
+        <v>0.5</v>
+      </c>
+      <c r="D34" s="79" t="str">
         <f>IF(SUM(K34:AD34)=0," ",SUM(K34:AD34))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E34" s="131"/>
-      <c r="F34" s="131"/>
-      <c r="G34" s="131"/>
-      <c r="H34" s="131"/>
-      <c r="I34" s="132"/>
-      <c r="J34" s="133"/>
-      <c r="K34" s="134">
-        <f t="shared" ref="K34:AD34" si="3">SUM(K5:K33)</f>
-        <v>0</v>
-      </c>
-      <c r="L34" s="131">
+      <c r="E34" s="76"/>
+      <c r="F34" s="68"/>
+      <c r="G34" s="80"/>
+      <c r="H34" s="69"/>
+      <c r="I34" s="176"/>
+      <c r="J34" s="177"/>
+      <c r="K34" s="80"/>
+      <c r="L34" s="178"/>
+      <c r="M34" s="179"/>
+      <c r="N34" s="61"/>
+      <c r="O34" s="55"/>
+      <c r="P34" s="77"/>
+      <c r="Q34" s="79"/>
+      <c r="R34" s="61"/>
+      <c r="S34" s="80"/>
+      <c r="T34" s="55"/>
+      <c r="U34" s="80"/>
+      <c r="V34" s="179"/>
+      <c r="W34" s="179"/>
+      <c r="X34" s="41"/>
+      <c r="Y34" s="180"/>
+      <c r="Z34" s="77"/>
+      <c r="AA34" s="79"/>
+      <c r="AB34" s="79"/>
+      <c r="AC34" s="78"/>
+      <c r="AD34" s="170"/>
+    </row>
+    <row r="35" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="112">
+        <v>60</v>
+      </c>
+      <c r="B35" s="113" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="115">
+        <f>SUM(C36:C37)</f>
+        <v>0</v>
+      </c>
+      <c r="D35" s="116">
+        <f>SUM(D36:D37)</f>
+        <v>0</v>
+      </c>
+      <c r="E35" s="117"/>
+      <c r="F35" s="118"/>
+      <c r="G35" s="122"/>
+      <c r="H35" s="119"/>
+      <c r="I35" s="120"/>
+      <c r="J35" s="121"/>
+      <c r="K35" s="118"/>
+      <c r="L35" s="122"/>
+      <c r="M35" s="123"/>
+      <c r="N35" s="124"/>
+      <c r="O35" s="117"/>
+      <c r="P35" s="114"/>
+      <c r="Q35" s="123"/>
+      <c r="R35" s="124"/>
+      <c r="S35" s="122"/>
+      <c r="T35" s="119"/>
+      <c r="U35" s="114"/>
+      <c r="V35" s="123"/>
+      <c r="W35" s="123"/>
+      <c r="X35" s="123"/>
+      <c r="Y35" s="119"/>
+      <c r="Z35" s="114"/>
+      <c r="AA35" s="123"/>
+      <c r="AB35" s="123"/>
+      <c r="AC35" s="124"/>
+      <c r="AD35" s="125"/>
+    </row>
+    <row r="36" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="86">
+        <v>61</v>
+      </c>
+      <c r="B36" s="97" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" s="36"/>
+      <c r="D36" s="72" t="str">
+        <f>IF(SUM(K36:AD36)=0," ",SUM(K36:AD36))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E36" s="35">
+        <v>2</v>
+      </c>
+      <c r="F36" s="36"/>
+      <c r="G36" s="73"/>
+      <c r="H36" s="38"/>
+      <c r="I36" s="39"/>
+      <c r="J36" s="110"/>
+      <c r="K36" s="73"/>
+      <c r="L36" s="41"/>
+      <c r="M36" s="41"/>
+      <c r="N36" s="41"/>
+      <c r="O36" s="74"/>
+      <c r="P36" s="45"/>
+      <c r="Q36" s="43"/>
+      <c r="R36" s="41"/>
+      <c r="S36" s="43"/>
+      <c r="T36" s="44"/>
+      <c r="U36" s="72"/>
+      <c r="V36" s="41"/>
+      <c r="W36" s="41"/>
+      <c r="X36" s="41"/>
+      <c r="Y36" s="73"/>
+      <c r="Z36" s="42"/>
+      <c r="AA36" s="43"/>
+      <c r="AB36" s="43"/>
+      <c r="AC36" s="43"/>
+      <c r="AD36" s="100"/>
+    </row>
+    <row r="37" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="85">
+        <v>62</v>
+      </c>
+      <c r="B37" s="98" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" s="47"/>
+      <c r="D37" s="37" t="str">
+        <f>IF(SUM(K37:AD37)=0," ",SUM(K37:AD37))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E37" s="46">
+        <v>1</v>
+      </c>
+      <c r="F37" s="82"/>
+      <c r="G37" s="139"/>
+      <c r="H37" s="83"/>
+      <c r="I37" s="39"/>
+      <c r="J37" s="108"/>
+      <c r="K37" s="56"/>
+      <c r="L37" s="49"/>
+      <c r="M37" s="49"/>
+      <c r="N37" s="49"/>
+      <c r="O37" s="74"/>
+      <c r="P37" s="75"/>
+      <c r="Q37" s="51"/>
+      <c r="R37" s="41"/>
+      <c r="S37" s="51"/>
+      <c r="T37" s="52"/>
+      <c r="U37" s="37"/>
+      <c r="V37" s="49"/>
+      <c r="W37" s="41"/>
+      <c r="X37" s="49"/>
+      <c r="Y37" s="56"/>
+      <c r="Z37" s="50"/>
+      <c r="AA37" s="51"/>
+      <c r="AB37" s="51"/>
+      <c r="AC37" s="51"/>
+      <c r="AD37" s="100"/>
+    </row>
+    <row r="38" spans="1:30" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="111"/>
+      <c r="B38" s="130" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="131">
+        <f>SUM(C5+C11+C15+C26+C35)</f>
+        <v>61</v>
+      </c>
+      <c r="D38" s="131" t="str">
+        <f>IF(SUM(K38:AD38)=0," ",SUM(K38:AD38))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E38" s="131"/>
+      <c r="F38" s="131"/>
+      <c r="G38" s="131"/>
+      <c r="H38" s="131"/>
+      <c r="I38" s="132"/>
+      <c r="J38" s="133"/>
+      <c r="K38" s="134">
+        <f t="shared" ref="K38:AD38" si="3">SUM(K5:K37)</f>
+        <v>0</v>
+      </c>
+      <c r="L38" s="131">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M34" s="135">
+      <c r="M38" s="135">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N34" s="135">
+      <c r="N38" s="135">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O34" s="135">
+      <c r="O38" s="135">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P34" s="135">
+      <c r="P38" s="135">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="Q34" s="131">
+      <c r="Q38" s="131">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R34" s="135">
+      <c r="R38" s="135">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S34" s="131">
+      <c r="S38" s="131">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="T34" s="135">
+      <c r="T38" s="135">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="U34" s="135">
+      <c r="U38" s="135">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="V34" s="131">
+      <c r="V38" s="131">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W34" s="135">
+      <c r="W38" s="135">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="X34" s="131">
+      <c r="X38" s="131">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="Y34" s="135">
+      <c r="Y38" s="135">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="Z34" s="135">
+      <c r="Z38" s="135">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AA34" s="131">
+      <c r="AA38" s="131">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AB34" s="135">
+      <c r="AB38" s="135">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AC34" s="131">
+      <c r="AC38" s="131">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AD34" s="136">
+      <c r="AD38" s="136">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="137"/>
-      <c r="B35" s="181"/>
-      <c r="C35" s="181"/>
-      <c r="D35" s="181"/>
-      <c r="E35" s="181"/>
-      <c r="F35" s="181"/>
-      <c r="G35" s="181"/>
-      <c r="H35" s="181"/>
-      <c r="I35" s="181"/>
-      <c r="J35" s="181"/>
-    </row>
-    <row r="36" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="138"/>
-      <c r="B36" s="15" t="s">
+    <row r="39" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="137"/>
+      <c r="B39" s="184"/>
+      <c r="C39" s="184"/>
+      <c r="D39" s="184"/>
+      <c r="E39" s="184"/>
+      <c r="F39" s="184"/>
+      <c r="G39" s="184"/>
+      <c r="H39" s="184"/>
+      <c r="I39" s="184"/>
+      <c r="J39" s="184"/>
+    </row>
+    <row r="40" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="138"/>
+      <c r="B40" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="15"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15"/>
-      <c r="H36" s="15"/>
-      <c r="I36" s="15"/>
-      <c r="J36" s="15"/>
-      <c r="K36" s="179"/>
-      <c r="L36" s="180"/>
-      <c r="M36" s="180"/>
-      <c r="N36" s="180"/>
-      <c r="O36" s="180"/>
-      <c r="P36" s="180"/>
-      <c r="Q36" s="180"/>
-      <c r="R36" s="180"/>
-      <c r="S36" s="180"/>
-      <c r="T36" s="180"/>
-      <c r="U36" s="180"/>
-      <c r="V36" s="180"/>
-      <c r="W36" s="180"/>
-      <c r="X36" s="180"/>
-      <c r="Y36" s="180"/>
-      <c r="Z36" s="180"/>
-      <c r="AA36" s="180"/>
-      <c r="AB36" s="180"/>
-      <c r="AC36" s="180"/>
-      <c r="AD36" s="180"/>
-    </row>
-    <row r="37" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="17"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
-      <c r="H37" s="18"/>
-      <c r="I37" s="18"/>
-      <c r="J37" s="18"/>
-      <c r="K37" s="178"/>
-      <c r="L37" s="178"/>
-      <c r="M37" s="178"/>
-      <c r="N37" s="178"/>
-      <c r="O37" s="178"/>
-      <c r="P37" s="178"/>
-      <c r="Q37" s="178"/>
-      <c r="R37" s="178"/>
-      <c r="S37" s="178"/>
-      <c r="T37" s="178"/>
-      <c r="U37" s="178"/>
-      <c r="V37" s="178"/>
-      <c r="W37" s="178"/>
-      <c r="X37" s="178"/>
-      <c r="Y37" s="178"/>
-      <c r="Z37" s="178"/>
-      <c r="AA37" s="178"/>
-      <c r="AB37" s="178"/>
-      <c r="AC37" s="178"/>
-      <c r="AD37" s="178"/>
-    </row>
-    <row r="38" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="17"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="18"/>
-      <c r="I38" s="18"/>
-      <c r="J38" s="18"/>
-      <c r="K38" s="178"/>
-      <c r="L38" s="178"/>
-      <c r="M38" s="178"/>
-      <c r="N38" s="178"/>
-      <c r="O38" s="178"/>
-      <c r="P38" s="178"/>
-      <c r="Q38" s="178"/>
-      <c r="R38" s="178"/>
-      <c r="S38" s="178"/>
-      <c r="T38" s="178"/>
-      <c r="U38" s="178"/>
-      <c r="V38" s="178"/>
-      <c r="W38" s="178"/>
-      <c r="X38" s="178"/>
-      <c r="Y38" s="178"/>
-      <c r="Z38" s="178"/>
-      <c r="AA38" s="178"/>
-      <c r="AB38" s="178"/>
-      <c r="AC38" s="178"/>
-      <c r="AD38" s="178"/>
-    </row>
-    <row r="39" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="20"/>
-      <c r="B39" s="18"/>
-      <c r="J39" s="9"/>
-    </row>
-    <row r="40" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="20"/>
-      <c r="B40" s="18"/>
-      <c r="J40" s="9"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="15"/>
+      <c r="J40" s="15"/>
+      <c r="K40" s="182"/>
+      <c r="L40" s="183"/>
+      <c r="M40" s="183"/>
+      <c r="N40" s="183"/>
+      <c r="O40" s="183"/>
+      <c r="P40" s="183"/>
+      <c r="Q40" s="183"/>
+      <c r="R40" s="183"/>
+      <c r="S40" s="183"/>
+      <c r="T40" s="183"/>
+      <c r="U40" s="183"/>
+      <c r="V40" s="183"/>
+      <c r="W40" s="183"/>
+      <c r="X40" s="183"/>
+      <c r="Y40" s="183"/>
+      <c r="Z40" s="183"/>
+      <c r="AA40" s="183"/>
+      <c r="AB40" s="183"/>
+      <c r="AC40" s="183"/>
+      <c r="AD40" s="183"/>
     </row>
     <row r="41" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J41" s="9"/>
+      <c r="A41" s="174"/>
+      <c r="B41" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C41" s="18"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="18"/>
+      <c r="I41" s="18"/>
+      <c r="J41" s="18"/>
+      <c r="K41" s="181"/>
+      <c r="L41" s="181"/>
+      <c r="M41" s="181"/>
+      <c r="N41" s="181"/>
+      <c r="O41" s="181"/>
+      <c r="P41" s="181"/>
+      <c r="Q41" s="181"/>
+      <c r="R41" s="181"/>
+      <c r="S41" s="181"/>
+      <c r="T41" s="181"/>
+      <c r="U41" s="181"/>
+      <c r="V41" s="181"/>
+      <c r="W41" s="181"/>
+      <c r="X41" s="181"/>
+      <c r="Y41" s="181"/>
+      <c r="Z41" s="181"/>
+      <c r="AA41" s="181"/>
+      <c r="AB41" s="181"/>
+      <c r="AC41" s="181"/>
+      <c r="AD41" s="181"/>
     </row>
     <row r="42" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="20"/>
-      <c r="J42" s="9"/>
+      <c r="A42" s="17"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="18"/>
+      <c r="I42" s="18"/>
+      <c r="J42" s="18"/>
+      <c r="K42" s="181"/>
+      <c r="L42" s="181"/>
+      <c r="M42" s="181"/>
+      <c r="N42" s="181"/>
+      <c r="O42" s="181"/>
+      <c r="P42" s="181"/>
+      <c r="Q42" s="181"/>
+      <c r="R42" s="181"/>
+      <c r="S42" s="181"/>
+      <c r="T42" s="181"/>
+      <c r="U42" s="181"/>
+      <c r="V42" s="181"/>
+      <c r="W42" s="181"/>
+      <c r="X42" s="181"/>
+      <c r="Y42" s="181"/>
+      <c r="Z42" s="181"/>
+      <c r="AA42" s="181"/>
+      <c r="AB42" s="181"/>
+      <c r="AC42" s="181"/>
+      <c r="AD42" s="181"/>
     </row>
     <row r="43" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="20"/>
+      <c r="B43" s="18"/>
       <c r="J43" s="9"/>
     </row>
     <row r="44" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="20"/>
+      <c r="B44" s="18"/>
       <c r="J44" s="9"/>
+    </row>
+    <row r="45" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J45" s="9"/>
+    </row>
+    <row r="46" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="20"/>
+      <c r="J46" s="9"/>
+    </row>
+    <row r="47" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J47" s="9"/>
+    </row>
+    <row r="48" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J48" s="9"/>
+    </row>
+    <row r="59" spans="34:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH59" s="9"/>
+      <c r="AI59" s="9"/>
+      <c r="AJ59" s="9"/>
+      <c r="AK59" s="9"/>
+      <c r="AL59" s="9"/>
+      <c r="AM59" s="9"/>
+      <c r="AN59" s="9"/>
+    </row>
+    <row r="60" spans="34:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH60" s="9"/>
+      <c r="AI60" s="9"/>
+      <c r="AJ60" s="9"/>
+      <c r="AK60" s="9"/>
+      <c r="AL60" s="9"/>
+      <c r="AM60" s="9"/>
+      <c r="AN60" s="9"/>
+    </row>
+    <row r="61" spans="34:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH61" s="9"/>
+      <c r="AI61" s="9"/>
+      <c r="AJ61" s="9"/>
+      <c r="AK61" s="9"/>
+      <c r="AL61" s="9"/>
+      <c r="AM61" s="9"/>
+      <c r="AN61" s="9"/>
+    </row>
+    <row r="62" spans="34:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH62" s="9"/>
+      <c r="AI62" s="9"/>
+      <c r="AJ62" s="9"/>
+      <c r="AK62" s="9"/>
+      <c r="AL62" s="9"/>
+      <c r="AM62" s="9"/>
+      <c r="AN62" s="9"/>
+    </row>
+    <row r="63" spans="34:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH63" s="9"/>
+      <c r="AI63" s="9"/>
+      <c r="AJ63" s="9"/>
+      <c r="AK63" s="9"/>
+      <c r="AL63" s="9"/>
+      <c r="AM63" s="9"/>
+      <c r="AN63" s="9"/>
+    </row>
+    <row r="64" spans="34:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH64" s="9"/>
+      <c r="AI64" s="9"/>
+      <c r="AJ64" s="9"/>
+      <c r="AK64" s="9"/>
+      <c r="AL64" s="9"/>
+      <c r="AM64" s="9"/>
+      <c r="AN64" s="9"/>
+    </row>
+    <row r="65" spans="34:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH65" s="9"/>
+      <c r="AI65" s="9"/>
+      <c r="AJ65" s="9"/>
+      <c r="AK65" s="9"/>
+      <c r="AL65" s="9"/>
+      <c r="AM65" s="9"/>
+      <c r="AN65" s="9"/>
+    </row>
+    <row r="66" spans="34:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH66" s="9"/>
+      <c r="AI66" s="9"/>
+      <c r="AJ66" s="9"/>
+      <c r="AK66" s="9"/>
+      <c r="AL66" s="9"/>
+      <c r="AM66" s="9"/>
+      <c r="AN66" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="K37:AD38"/>
-    <mergeCell ref="K36:AD36"/>
-    <mergeCell ref="B35:J35"/>
+    <mergeCell ref="K41:AD42"/>
+    <mergeCell ref="K40:AD40"/>
+    <mergeCell ref="B39:J39"/>
     <mergeCell ref="A1:AD1"/>
     <mergeCell ref="U3:Y3"/>
     <mergeCell ref="Z3:AD3"/>
@@ -4698,21 +4984,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="188"/>
-      <c r="B1" s="188"/>
-      <c r="C1" s="188"/>
-      <c r="D1" s="188"/>
-      <c r="E1" s="188"/>
-      <c r="F1" s="188"/>
-      <c r="G1" s="188"/>
-      <c r="H1" s="188"/>
-      <c r="I1" s="188"/>
-      <c r="J1" s="188"/>
-      <c r="K1" s="188"/>
-      <c r="L1" s="188"/>
-      <c r="M1" s="188"/>
-      <c r="N1" s="188"/>
-      <c r="O1" s="188"/>
+      <c r="A1" s="191"/>
+      <c r="B1" s="191"/>
+      <c r="C1" s="191"/>
+      <c r="D1" s="191"/>
+      <c r="E1" s="191"/>
+      <c r="F1" s="191"/>
+      <c r="G1" s="191"/>
+      <c r="H1" s="191"/>
+      <c r="I1" s="191"/>
+      <c r="J1" s="191"/>
+      <c r="K1" s="191"/>
+      <c r="L1" s="191"/>
+      <c r="M1" s="191"/>
+      <c r="N1" s="191"/>
+      <c r="O1" s="191"/>
     </row>
     <row r="2" spans="1:15" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -4751,7 +5037,7 @@
         <v>42702</v>
       </c>
       <c r="C4" s="5">
-        <f>'IPA Zeitplanung'!K34</f>
+        <f>'IPA Zeitplanung'!K38</f>
         <v>0</v>
       </c>
     </row>
@@ -4764,7 +5050,7 @@
         <v>42703</v>
       </c>
       <c r="C5" s="5">
-        <f>'IPA Zeitplanung'!L34</f>
+        <f>'IPA Zeitplanung'!L38</f>
         <v>0</v>
       </c>
     </row>
@@ -4777,7 +5063,7 @@
         <v>42704</v>
       </c>
       <c r="C6" s="5">
-        <f>'IPA Zeitplanung'!M34</f>
+        <f>'IPA Zeitplanung'!M38</f>
         <v>0</v>
       </c>
     </row>
@@ -4790,7 +5076,7 @@
         <v>42705</v>
       </c>
       <c r="C7" s="5">
-        <f>'IPA Zeitplanung'!N34</f>
+        <f>'IPA Zeitplanung'!N38</f>
         <v>0</v>
       </c>
     </row>
@@ -4803,7 +5089,7 @@
         <v>42706</v>
       </c>
       <c r="C8" s="5">
-        <f>'IPA Zeitplanung'!O34</f>
+        <f>'IPA Zeitplanung'!O38</f>
         <v>0</v>
       </c>
     </row>
@@ -4816,7 +5102,7 @@
         <v>42709</v>
       </c>
       <c r="C9" s="5">
-        <f>'IPA Zeitplanung'!P34</f>
+        <f>'IPA Zeitplanung'!P38</f>
         <v>0</v>
       </c>
     </row>
@@ -4829,7 +5115,7 @@
         <v>42710</v>
       </c>
       <c r="C10" s="5">
-        <f>'IPA Zeitplanung'!Q34</f>
+        <f>'IPA Zeitplanung'!Q38</f>
         <v>0</v>
       </c>
     </row>
@@ -4842,7 +5128,7 @@
         <v>42711</v>
       </c>
       <c r="C11" s="5">
-        <f>'IPA Zeitplanung'!R34</f>
+        <f>'IPA Zeitplanung'!R38</f>
         <v>0</v>
       </c>
     </row>
@@ -4855,7 +5141,7 @@
         <v>42712</v>
       </c>
       <c r="C12" s="5">
-        <f>'IPA Zeitplanung'!S34</f>
+        <f>'IPA Zeitplanung'!S38</f>
         <v>0</v>
       </c>
     </row>
@@ -4868,7 +5154,7 @@
         <v>42713</v>
       </c>
       <c r="C13" s="5">
-        <f>'IPA Zeitplanung'!T34</f>
+        <f>'IPA Zeitplanung'!T38</f>
         <v>0</v>
       </c>
     </row>
@@ -4881,7 +5167,7 @@
         <v>42716</v>
       </c>
       <c r="C14" s="5">
-        <f>'IPA Zeitplanung'!U34</f>
+        <f>'IPA Zeitplanung'!U38</f>
         <v>0</v>
       </c>
     </row>
@@ -4894,7 +5180,7 @@
         <v>42717</v>
       </c>
       <c r="C15" s="5">
-        <f>'IPA Zeitplanung'!V34</f>
+        <f>'IPA Zeitplanung'!V38</f>
         <v>0</v>
       </c>
     </row>
@@ -4907,7 +5193,7 @@
         <v>42718</v>
       </c>
       <c r="C16" s="5">
-        <f>'IPA Zeitplanung'!W34</f>
+        <f>'IPA Zeitplanung'!W38</f>
         <v>0</v>
       </c>
     </row>
@@ -4920,7 +5206,7 @@
         <v>42719</v>
       </c>
       <c r="C17" s="5">
-        <f>'IPA Zeitplanung'!X34</f>
+        <f>'IPA Zeitplanung'!X38</f>
         <v>0</v>
       </c>
     </row>
@@ -4933,7 +5219,7 @@
         <v>42720</v>
       </c>
       <c r="C18" s="5">
-        <f>'IPA Zeitplanung'!Y34</f>
+        <f>'IPA Zeitplanung'!Y38</f>
         <v>0</v>
       </c>
     </row>
@@ -4946,7 +5232,7 @@
         <v>42723</v>
       </c>
       <c r="C19" s="5">
-        <f>'IPA Zeitplanung'!Z34</f>
+        <f>'IPA Zeitplanung'!Z38</f>
         <v>0</v>
       </c>
     </row>
@@ -4959,7 +5245,7 @@
         <v>42724</v>
       </c>
       <c r="C20" s="5">
-        <f>'IPA Zeitplanung'!AA34</f>
+        <f>'IPA Zeitplanung'!AA38</f>
         <v>0</v>
       </c>
     </row>
@@ -4972,7 +5258,7 @@
         <v>42725</v>
       </c>
       <c r="C21" s="5">
-        <f>'IPA Zeitplanung'!AB34</f>
+        <f>'IPA Zeitplanung'!AB38</f>
         <v>0</v>
       </c>
     </row>
@@ -4985,7 +5271,7 @@
         <v>42726</v>
       </c>
       <c r="C22" s="5">
-        <f>'IPA Zeitplanung'!AC34</f>
+        <f>'IPA Zeitplanung'!AC38</f>
         <v>0</v>
       </c>
     </row>
@@ -4998,7 +5284,7 @@
         <v>42727</v>
       </c>
       <c r="C23" s="5">
-        <f>'IPA Zeitplanung'!AD34</f>
+        <f>'IPA Zeitplanung'!AD38</f>
         <v>0</v>
       </c>
     </row>
@@ -5018,10 +5304,10 @@
     <row r="25" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="189" t="s">
+      <c r="A27" s="192" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="190"/>
+      <c r="B27" s="193"/>
       <c r="C27" s="4" t="s">
         <v>29</v>
       </c>
@@ -5030,10 +5316,10 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="186" t="s">
+      <c r="A28" s="189" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="187"/>
+      <c r="B28" s="190"/>
       <c r="C28" s="5">
         <f>'IPA Zeitplanung'!C5</f>
         <v>0</v>
@@ -5044,10 +5330,10 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="191" t="s">
+      <c r="A29" s="194" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="192"/>
+      <c r="B29" s="195"/>
       <c r="C29" s="5">
         <f>'IPA Zeitplanung'!C11</f>
         <v>0</v>
@@ -5058,58 +5344,58 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="186" t="s">
+      <c r="A30" s="189" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="187"/>
+      <c r="B30" s="190"/>
       <c r="C30" s="5">
         <f>'IPA Zeitplanung'!C15</f>
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="D30" s="5">
         <f>'IPA Zeitplanung'!D15</f>
-        <v>10.5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="191" t="s">
+      <c r="A31" s="194" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="192"/>
+      <c r="B31" s="195"/>
       <c r="C31" s="5">
-        <f>'IPA Zeitplanung'!C24</f>
+        <f>'IPA Zeitplanung'!C26</f>
         <v>0</v>
       </c>
       <c r="D31" s="5">
-        <f>'IPA Zeitplanung'!D24</f>
+        <f>'IPA Zeitplanung'!D26</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="186" t="s">
+      <c r="A32" s="189" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="187"/>
+      <c r="B32" s="190"/>
       <c r="C32" s="5">
-        <f>'IPA Zeitplanung'!C29</f>
-        <v>10.8</v>
+        <f>'IPA Zeitplanung'!C31</f>
+        <v>12.200000000000001</v>
       </c>
       <c r="D32" s="5">
-        <f>SUM('IPA Zeitplanung'!D29)</f>
+        <f>SUM('IPA Zeitplanung'!D31)</f>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="186" t="s">
+      <c r="A33" s="189" t="s">
         <v>10</v>
       </c>
-      <c r="B33" s="187"/>
+      <c r="B33" s="190"/>
       <c r="C33" s="5">
-        <f>'IPA Zeitplanung'!C31</f>
+        <f>'IPA Zeitplanung'!C35</f>
         <v>0</v>
       </c>
       <c r="D33" s="5">
-        <f>'IPA Zeitplanung'!D31</f>
+        <f>'IPA Zeitplanung'!D35</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Durcheinander vor neujahr packe im moment alles in Funktionen
</commit_message>
<xml_diff>
--- a/documents/Zeitplanung.xlsx
+++ b/documents/Zeitplanung.xlsx
@@ -3098,10 +3098,10 @@
   <dimension ref="A1:AN67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="10" ySplit="4" topLeftCell="K23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="4" topLeftCell="K5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="N1" sqref="N1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AG31" sqref="AG31"/>
+      <selection pane="bottomRight" activeCell="AG18" sqref="AG18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4162,7 +4162,7 @@
         <v>16</v>
       </c>
       <c r="D26" s="79">
-        <v>11</v>
+        <v>19.5</v>
       </c>
       <c r="E26" s="46">
         <v>2</v>

</xml_diff>

<commit_message>
05.01.2017 Views und Controller start.
</commit_message>
<xml_diff>
--- a/documents/Zeitplanung.xlsx
+++ b/documents/Zeitplanung.xlsx
@@ -16,8 +16,8 @@
     <sheet name="Ist Arbeitszeit - Übersicht" sheetId="7" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'IPA Zeitplanung'!$A$3:$AD$39</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'IPA Zeitplanung'!$A$1:$AD$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'IPA Zeitplanung'!$A$3:$AD$40</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'IPA Zeitplanung'!$A$1:$AN$47</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Ist Arbeitszeit - Übersicht'!$A$1:$O$47</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
@@ -135,7 +135,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="61">
   <si>
     <t>Nr.</t>
   </si>
@@ -150,9 +150,6 @@
   </si>
   <si>
     <t>Priorität</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Reserve</t>
@@ -311,6 +308,18 @@
   <si>
     <t>Release 3</t>
   </si>
+  <si>
+    <t>Abwesend: Ferien</t>
+  </si>
+  <si>
+    <t>Code Ordnung machen.</t>
+  </si>
+  <si>
+    <t>Woche 5</t>
+  </si>
+  <si>
+    <t>Woche 6</t>
+  </si>
 </sst>
 </file>
 
@@ -452,7 +461,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -540,8 +549,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="83">
+  <borders count="85">
     <border>
       <left/>
       <right/>
@@ -1571,6 +1586,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0"/>
@@ -1585,7 +1622,7 @@
     <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="202">
+  <cellXfs count="222">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1625,9 +1662,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2176,6 +2210,69 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="59" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="60" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="54" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="54" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="48" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="32" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="52" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="84" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20 % - Akzent4" xfId="6" builtinId="42"/>
@@ -3095,13 +3192,13 @@
   <sheetPr codeName="Tabelle1">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:AN67"/>
+  <dimension ref="A1:AX68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="10" ySplit="4" topLeftCell="K5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="4" topLeftCell="R5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="N1" sqref="N1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AG18" sqref="AG18"/>
+      <selection pane="bottomRight" activeCell="AP13" sqref="AP13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3109,52 +3206,62 @@
     <col min="1" max="1" width="3.625" style="9" customWidth="1"/>
     <col min="2" max="2" width="44.25" style="9" customWidth="1"/>
     <col min="3" max="3" width="5" style="9" customWidth="1"/>
-    <col min="4" max="4" width="5" style="21" customWidth="1"/>
+    <col min="4" max="4" width="5" style="20" customWidth="1"/>
     <col min="5" max="5" width="5" style="9" customWidth="1"/>
     <col min="6" max="8" width="3.125" style="9" customWidth="1"/>
     <col min="9" max="9" width="7.625" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.25" style="22" customWidth="1"/>
-    <col min="11" max="30" width="3.125" style="9" customWidth="1"/>
-    <col min="31" max="31" width="4.25" style="8" customWidth="1"/>
-    <col min="32" max="40" width="12.5" style="8" customWidth="1"/>
-    <col min="41" max="16384" width="12.5" style="9"/>
+    <col min="10" max="10" width="4.25" style="21" customWidth="1"/>
+    <col min="11" max="40" width="3.125" style="9" customWidth="1"/>
+    <col min="41" max="41" width="4.25" style="8" customWidth="1"/>
+    <col min="42" max="50" width="12.5" style="8" customWidth="1"/>
+    <col min="51" max="16384" width="12.5" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="191" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="191"/>
-      <c r="C1" s="191"/>
-      <c r="D1" s="191"/>
-      <c r="E1" s="191"/>
-      <c r="F1" s="191"/>
-      <c r="G1" s="191"/>
-      <c r="H1" s="191"/>
-      <c r="I1" s="191"/>
-      <c r="J1" s="191"/>
-      <c r="K1" s="191"/>
-      <c r="L1" s="191"/>
-      <c r="M1" s="191"/>
-      <c r="N1" s="191"/>
-      <c r="O1" s="191"/>
-      <c r="P1" s="191"/>
-      <c r="Q1" s="191"/>
-      <c r="R1" s="191"/>
-      <c r="S1" s="191"/>
-      <c r="T1" s="191"/>
-      <c r="U1" s="191"/>
-      <c r="V1" s="191"/>
-      <c r="W1" s="191"/>
-      <c r="X1" s="191"/>
-      <c r="Y1" s="191"/>
-      <c r="Z1" s="191"/>
-      <c r="AA1" s="191"/>
-      <c r="AB1" s="191"/>
-      <c r="AC1" s="191"/>
-      <c r="AD1" s="191"/>
-    </row>
-    <row r="2" spans="1:34" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:41" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="190" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="190"/>
+      <c r="C1" s="190"/>
+      <c r="D1" s="190"/>
+      <c r="E1" s="190"/>
+      <c r="F1" s="190"/>
+      <c r="G1" s="190"/>
+      <c r="H1" s="190"/>
+      <c r="I1" s="190"/>
+      <c r="J1" s="190"/>
+      <c r="K1" s="190"/>
+      <c r="L1" s="190"/>
+      <c r="M1" s="190"/>
+      <c r="N1" s="190"/>
+      <c r="O1" s="190"/>
+      <c r="P1" s="190"/>
+      <c r="Q1" s="190"/>
+      <c r="R1" s="190"/>
+      <c r="S1" s="190"/>
+      <c r="T1" s="190"/>
+      <c r="U1" s="190"/>
+      <c r="V1" s="190"/>
+      <c r="W1" s="190"/>
+      <c r="X1" s="190"/>
+      <c r="Y1" s="190"/>
+      <c r="Z1" s="190"/>
+      <c r="AA1" s="190"/>
+      <c r="AB1" s="190"/>
+      <c r="AC1" s="190"/>
+      <c r="AD1" s="190"/>
+      <c r="AE1" s="190"/>
+      <c r="AF1" s="190"/>
+      <c r="AG1" s="190"/>
+      <c r="AH1" s="190"/>
+      <c r="AI1" s="190"/>
+      <c r="AJ1" s="190"/>
+      <c r="AK1" s="190"/>
+      <c r="AL1" s="190"/>
+      <c r="AM1" s="190"/>
+      <c r="AN1" s="190"/>
+    </row>
+    <row r="2" spans="1:41" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -3166,1846 +3273,2311 @@
       <c r="I2" s="8"/>
       <c r="J2" s="12"/>
     </row>
-    <row r="3" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="84"/>
-      <c r="B3" s="88"/>
-      <c r="C3" s="192" t="s">
+    <row r="3" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="83"/>
+      <c r="B3" s="87"/>
+      <c r="C3" s="191" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="192"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="192" t="s">
+      <c r="D3" s="191"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="191" t="s">
+        <v>52</v>
+      </c>
+      <c r="L3" s="191"/>
+      <c r="M3" s="191"/>
+      <c r="N3" s="191"/>
+      <c r="O3" s="192"/>
+      <c r="P3" s="193" t="s">
         <v>53</v>
       </c>
-      <c r="L3" s="192"/>
-      <c r="M3" s="192"/>
-      <c r="N3" s="192"/>
-      <c r="O3" s="193"/>
-      <c r="P3" s="194" t="s">
+      <c r="Q3" s="191"/>
+      <c r="R3" s="191"/>
+      <c r="S3" s="191"/>
+      <c r="T3" s="192"/>
+      <c r="U3" s="191" t="s">
         <v>54</v>
       </c>
-      <c r="Q3" s="192"/>
-      <c r="R3" s="192"/>
-      <c r="S3" s="192"/>
-      <c r="T3" s="193"/>
-      <c r="U3" s="192" t="s">
+      <c r="V3" s="191"/>
+      <c r="W3" s="191"/>
+      <c r="X3" s="191"/>
+      <c r="Y3" s="192"/>
+      <c r="Z3" s="193" t="s">
         <v>55</v>
       </c>
-      <c r="V3" s="192"/>
-      <c r="W3" s="192"/>
-      <c r="X3" s="192"/>
-      <c r="Y3" s="193"/>
-      <c r="Z3" s="194" t="s">
-        <v>56</v>
-      </c>
-      <c r="AA3" s="192"/>
-      <c r="AB3" s="192"/>
-      <c r="AC3" s="192"/>
-      <c r="AD3" s="193"/>
-      <c r="AE3" s="13"/>
-      <c r="AF3" s="13"/>
-      <c r="AG3" s="13"/>
-      <c r="AH3" s="13"/>
-    </row>
-    <row r="4" spans="1:34" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="127" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="89"/>
-      <c r="C4" s="28" t="s">
+      <c r="AA3" s="191"/>
+      <c r="AB3" s="191"/>
+      <c r="AC3" s="191"/>
+      <c r="AD3" s="192"/>
+      <c r="AE3" s="193" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF3" s="191"/>
+      <c r="AG3" s="191"/>
+      <c r="AH3" s="191"/>
+      <c r="AI3" s="192"/>
+      <c r="AJ3" s="193" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK3" s="191"/>
+      <c r="AL3" s="191"/>
+      <c r="AM3" s="191"/>
+      <c r="AN3" s="192"/>
+      <c r="AO3" s="13"/>
+    </row>
+    <row r="4" spans="1:41" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="126" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="88"/>
+      <c r="C4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4" s="140" t="s">
+      <c r="F4" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="141" t="s">
-        <v>37</v>
-      </c>
-      <c r="I4" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="103" t="s">
-        <v>8</v>
-      </c>
-      <c r="K4" s="128">
+      <c r="G4" s="139" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="140" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="102" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="127">
         <v>42702</v>
       </c>
-      <c r="L4" s="32">
+      <c r="L4" s="31">
         <v>42703</v>
       </c>
-      <c r="M4" s="32">
+      <c r="M4" s="31">
         <v>42704</v>
       </c>
-      <c r="N4" s="33">
+      <c r="N4" s="32">
         <v>42705</v>
       </c>
-      <c r="O4" s="34">
+      <c r="O4" s="33">
         <f>N4+1</f>
         <v>42706</v>
       </c>
-      <c r="P4" s="34">
+      <c r="P4" s="33">
         <v>42709</v>
       </c>
-      <c r="Q4" s="34">
-        <f t="shared" ref="Q4:AD4" si="0">P4+1</f>
+      <c r="Q4" s="33">
+        <f t="shared" ref="Q4:Y4" si="0">P4+1</f>
         <v>42710</v>
       </c>
-      <c r="R4" s="34">
+      <c r="R4" s="33">
         <f t="shared" si="0"/>
         <v>42711</v>
       </c>
-      <c r="S4" s="34">
+      <c r="S4" s="33">
         <f t="shared" si="0"/>
         <v>42712</v>
       </c>
-      <c r="T4" s="34">
+      <c r="T4" s="33">
         <f t="shared" si="0"/>
         <v>42713</v>
       </c>
-      <c r="U4" s="34">
+      <c r="U4" s="33">
         <v>42716</v>
       </c>
-      <c r="V4" s="34">
+      <c r="V4" s="33">
         <f t="shared" si="0"/>
         <v>42717</v>
       </c>
-      <c r="W4" s="34">
+      <c r="W4" s="33">
         <f t="shared" si="0"/>
         <v>42718</v>
       </c>
-      <c r="X4" s="34">
+      <c r="X4" s="33">
         <f t="shared" si="0"/>
         <v>42719</v>
       </c>
-      <c r="Y4" s="34">
+      <c r="Y4" s="33">
         <f t="shared" si="0"/>
         <v>42720</v>
       </c>
-      <c r="Z4" s="34">
+      <c r="Z4" s="33">
         <v>42723</v>
       </c>
-      <c r="AA4" s="34">
-        <f t="shared" si="0"/>
+      <c r="AA4" s="33">
+        <f>Z4+1</f>
         <v>42724</v>
       </c>
-      <c r="AB4" s="34">
-        <f t="shared" si="0"/>
+      <c r="AB4" s="33">
+        <f>AA4+1</f>
         <v>42725</v>
       </c>
-      <c r="AC4" s="34">
-        <f t="shared" si="0"/>
+      <c r="AC4" s="33">
+        <f>AB4+1</f>
         <v>42726</v>
       </c>
-      <c r="AD4" s="34">
-        <f t="shared" si="0"/>
+      <c r="AD4" s="33">
+        <f>AC4+1</f>
         <v>42727</v>
       </c>
-    </row>
-    <row r="5" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="112">
+      <c r="AE4" s="33">
+        <v>42737</v>
+      </c>
+      <c r="AF4" s="33">
+        <v>42738</v>
+      </c>
+      <c r="AG4" s="33">
+        <v>42739</v>
+      </c>
+      <c r="AH4" s="33">
+        <v>42740</v>
+      </c>
+      <c r="AI4" s="33">
+        <v>42741</v>
+      </c>
+      <c r="AJ4" s="33">
+        <v>42744</v>
+      </c>
+      <c r="AK4" s="33">
+        <v>42745</v>
+      </c>
+      <c r="AL4" s="33">
+        <v>42746</v>
+      </c>
+      <c r="AM4" s="33">
+        <v>42747</v>
+      </c>
+      <c r="AN4" s="33">
+        <v>42748</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="111">
         <v>10</v>
       </c>
-      <c r="B5" s="113" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="115">
+      <c r="B5" s="112" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="114">
         <f>SUM(C6:C10)</f>
         <v>0</v>
       </c>
-      <c r="D5" s="116">
+      <c r="D5" s="115">
         <f>SUM(D6:D10)</f>
         <v>0</v>
       </c>
-      <c r="E5" s="117"/>
-      <c r="F5" s="118"/>
-      <c r="G5" s="122"/>
-      <c r="H5" s="119"/>
-      <c r="I5" s="120"/>
-      <c r="J5" s="121"/>
-      <c r="K5" s="118"/>
-      <c r="L5" s="122"/>
-      <c r="M5" s="123"/>
-      <c r="N5" s="124"/>
-      <c r="O5" s="117"/>
-      <c r="P5" s="114"/>
-      <c r="Q5" s="123"/>
-      <c r="R5" s="124"/>
-      <c r="S5" s="122"/>
-      <c r="T5" s="119"/>
-      <c r="U5" s="114"/>
-      <c r="V5" s="123"/>
-      <c r="W5" s="123"/>
-      <c r="X5" s="123"/>
-      <c r="Y5" s="119"/>
-      <c r="Z5" s="114"/>
-      <c r="AA5" s="123"/>
-      <c r="AB5" s="123"/>
-      <c r="AC5" s="124"/>
-      <c r="AD5" s="125"/>
-    </row>
-    <row r="6" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="85">
+      <c r="E5" s="116"/>
+      <c r="F5" s="117"/>
+      <c r="G5" s="121"/>
+      <c r="H5" s="118"/>
+      <c r="I5" s="119"/>
+      <c r="J5" s="120"/>
+      <c r="K5" s="117"/>
+      <c r="L5" s="121"/>
+      <c r="M5" s="122"/>
+      <c r="N5" s="123"/>
+      <c r="O5" s="116"/>
+      <c r="P5" s="113"/>
+      <c r="Q5" s="122"/>
+      <c r="R5" s="123"/>
+      <c r="S5" s="121"/>
+      <c r="T5" s="118"/>
+      <c r="U5" s="113"/>
+      <c r="V5" s="122"/>
+      <c r="W5" s="122"/>
+      <c r="X5" s="122"/>
+      <c r="Y5" s="118"/>
+      <c r="Z5" s="113"/>
+      <c r="AA5" s="122"/>
+      <c r="AB5" s="122"/>
+      <c r="AC5" s="123"/>
+      <c r="AD5" s="124"/>
+      <c r="AE5" s="121"/>
+      <c r="AF5" s="121"/>
+      <c r="AG5" s="121"/>
+      <c r="AH5" s="121"/>
+      <c r="AI5" s="116"/>
+      <c r="AJ5" s="121"/>
+      <c r="AK5" s="121"/>
+      <c r="AL5" s="121"/>
+      <c r="AM5" s="121"/>
+      <c r="AN5" s="121"/>
+    </row>
+    <row r="6" spans="1:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="84">
         <v>11</v>
       </c>
-      <c r="B6" s="90" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="37" t="str">
+      <c r="B6" s="89" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="35"/>
+      <c r="D6" s="36" t="str">
         <f>IF(SUM(K6:AD6)=0," ",SUM(K6:AD6))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E6" s="35">
+      <c r="E6" s="34">
         <v>1</v>
       </c>
-      <c r="F6" s="36"/>
-      <c r="G6" s="73"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="104"/>
-      <c r="K6" s="129"/>
-      <c r="L6" s="41"/>
-      <c r="M6" s="41"/>
-      <c r="N6" s="41"/>
-      <c r="O6" s="74"/>
-      <c r="P6" s="42"/>
-      <c r="Q6" s="43"/>
-      <c r="R6" s="41"/>
-      <c r="S6" s="43"/>
-      <c r="T6" s="44"/>
-      <c r="U6" s="40"/>
-      <c r="V6" s="41"/>
-      <c r="W6" s="41"/>
-      <c r="X6" s="41"/>
-      <c r="Y6" s="36"/>
-      <c r="Z6" s="45"/>
-      <c r="AA6" s="43"/>
-      <c r="AB6" s="43"/>
-      <c r="AC6" s="43"/>
-      <c r="AD6" s="91"/>
-    </row>
-    <row r="7" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="85">
+      <c r="F6" s="35"/>
+      <c r="G6" s="72"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="103"/>
+      <c r="K6" s="128"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="73"/>
+      <c r="P6" s="41"/>
+      <c r="Q6" s="42"/>
+      <c r="R6" s="40"/>
+      <c r="S6" s="42"/>
+      <c r="T6" s="43"/>
+      <c r="U6" s="39"/>
+      <c r="V6" s="40"/>
+      <c r="W6" s="40"/>
+      <c r="X6" s="40"/>
+      <c r="Y6" s="35"/>
+      <c r="Z6" s="44"/>
+      <c r="AA6" s="42"/>
+      <c r="AB6" s="42"/>
+      <c r="AC6" s="42"/>
+      <c r="AD6" s="90"/>
+      <c r="AE6" s="72"/>
+      <c r="AF6" s="72"/>
+      <c r="AG6" s="72"/>
+      <c r="AH6" s="72"/>
+      <c r="AI6" s="202"/>
+      <c r="AJ6" s="218"/>
+      <c r="AK6" s="218"/>
+      <c r="AL6" s="218"/>
+      <c r="AM6" s="218"/>
+      <c r="AN6" s="218"/>
+    </row>
+    <row r="7" spans="1:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="84">
         <v>12</v>
       </c>
-      <c r="B7" s="92" t="s">
+      <c r="B7" s="91" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="46"/>
+      <c r="D7" s="36" t="str">
+        <f>IF(SUM(K7:AD7)=0," ",SUM(K7:AD7))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E7" s="45">
+        <v>1</v>
+      </c>
+      <c r="F7" s="35"/>
+      <c r="G7" s="72"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="104"/>
+      <c r="K7" s="128"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="48"/>
+      <c r="N7" s="48"/>
+      <c r="O7" s="73"/>
+      <c r="P7" s="49"/>
+      <c r="Q7" s="50"/>
+      <c r="R7" s="40"/>
+      <c r="S7" s="50"/>
+      <c r="T7" s="51"/>
+      <c r="U7" s="47"/>
+      <c r="V7" s="48"/>
+      <c r="W7" s="40"/>
+      <c r="X7" s="48"/>
+      <c r="Y7" s="52"/>
+      <c r="Z7" s="53"/>
+      <c r="AA7" s="50"/>
+      <c r="AB7" s="50"/>
+      <c r="AC7" s="50"/>
+      <c r="AD7" s="92"/>
+      <c r="AE7" s="55"/>
+      <c r="AF7" s="55"/>
+      <c r="AG7" s="55"/>
+      <c r="AH7" s="55"/>
+      <c r="AI7" s="203"/>
+      <c r="AJ7" s="176"/>
+      <c r="AK7" s="176"/>
+      <c r="AL7" s="176"/>
+      <c r="AM7" s="176"/>
+      <c r="AN7" s="176"/>
+    </row>
+    <row r="8" spans="1:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="84">
+        <v>13</v>
+      </c>
+      <c r="B8" s="91" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="46"/>
+      <c r="D8" s="36" t="str">
+        <f>IF(SUM(K8:AD8)=0," ",SUM(K8:AD8))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E8" s="45">
+        <v>1</v>
+      </c>
+      <c r="F8" s="35"/>
+      <c r="G8" s="72"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="104"/>
+      <c r="K8" s="128"/>
+      <c r="L8" s="40"/>
+      <c r="M8" s="48"/>
+      <c r="N8" s="48"/>
+      <c r="O8" s="73"/>
+      <c r="P8" s="49"/>
+      <c r="Q8" s="141"/>
+      <c r="R8" s="142"/>
+      <c r="S8" s="141"/>
+      <c r="T8" s="143"/>
+      <c r="U8" s="144"/>
+      <c r="V8" s="145"/>
+      <c r="W8" s="142"/>
+      <c r="X8" s="48"/>
+      <c r="Y8" s="52"/>
+      <c r="Z8" s="53"/>
+      <c r="AA8" s="50"/>
+      <c r="AB8" s="50"/>
+      <c r="AC8" s="36"/>
+      <c r="AD8" s="93"/>
+      <c r="AE8" s="55"/>
+      <c r="AF8" s="55"/>
+      <c r="AG8" s="55"/>
+      <c r="AH8" s="55"/>
+      <c r="AI8" s="203"/>
+      <c r="AJ8" s="219"/>
+      <c r="AK8" s="219"/>
+      <c r="AL8" s="219"/>
+      <c r="AM8" s="219"/>
+      <c r="AN8" s="219"/>
+    </row>
+    <row r="9" spans="1:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="84">
+        <v>14</v>
+      </c>
+      <c r="B9" s="94" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="46"/>
+      <c r="D9" s="36" t="str">
+        <f>IF(SUM(K9:AD9)=0," ",SUM(K9:AD9))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E9" s="45">
+        <v>1</v>
+      </c>
+      <c r="F9" s="35"/>
+      <c r="G9" s="72"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="104"/>
+      <c r="K9" s="128"/>
+      <c r="L9" s="151"/>
+      <c r="M9" s="157"/>
+      <c r="N9" s="157"/>
+      <c r="O9" s="163"/>
+      <c r="P9" s="164"/>
+      <c r="Q9" s="158"/>
+      <c r="R9" s="151"/>
+      <c r="S9" s="165"/>
+      <c r="T9" s="159"/>
+      <c r="U9" s="164"/>
+      <c r="V9" s="157"/>
+      <c r="W9" s="151"/>
+      <c r="X9" s="48"/>
+      <c r="Z9" s="49"/>
+      <c r="AA9" s="50"/>
+      <c r="AB9" s="50"/>
+      <c r="AC9" s="36"/>
+      <c r="AD9" s="166"/>
+      <c r="AI9" s="204"/>
+      <c r="AJ9" s="176"/>
+      <c r="AK9" s="176"/>
+      <c r="AL9" s="176"/>
+      <c r="AM9" s="176"/>
+      <c r="AN9" s="176"/>
+    </row>
+    <row r="10" spans="1:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="84">
         <v>15</v>
       </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="37" t="str">
-        <f t="shared" ref="D7:D10" si="1">IF(SUM(K7:AD7)=0," ",SUM(K7:AD7))</f>
+      <c r="B10" s="94" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="57"/>
+      <c r="D10" s="36" t="str">
+        <f>IF(SUM(K10:AD10)=0," ",SUM(K10:AD10))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E7" s="46">
+      <c r="E10" s="56">
         <v>1</v>
       </c>
-      <c r="F7" s="36"/>
-      <c r="G7" s="73"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="105"/>
-      <c r="K7" s="129"/>
-      <c r="L7" s="41"/>
-      <c r="M7" s="49"/>
-      <c r="N7" s="49"/>
-      <c r="O7" s="74"/>
-      <c r="P7" s="50"/>
-      <c r="Q7" s="51"/>
-      <c r="R7" s="41"/>
-      <c r="S7" s="51"/>
-      <c r="T7" s="52"/>
-      <c r="U7" s="48"/>
-      <c r="V7" s="49"/>
-      <c r="W7" s="41"/>
-      <c r="X7" s="49"/>
-      <c r="Y7" s="53"/>
-      <c r="Z7" s="54"/>
-      <c r="AA7" s="51"/>
-      <c r="AB7" s="51"/>
-      <c r="AC7" s="51"/>
-      <c r="AD7" s="93"/>
-    </row>
-    <row r="8" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="85">
-        <v>13</v>
-      </c>
-      <c r="B8" s="92" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="47"/>
-      <c r="D8" s="37" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E8" s="46">
-        <v>1</v>
-      </c>
-      <c r="F8" s="36"/>
-      <c r="G8" s="73"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="105"/>
-      <c r="K8" s="129"/>
-      <c r="L8" s="41"/>
-      <c r="M8" s="49"/>
-      <c r="N8" s="49"/>
-      <c r="O8" s="74"/>
-      <c r="P8" s="50"/>
-      <c r="Q8" s="142"/>
-      <c r="R8" s="143"/>
-      <c r="S8" s="142"/>
-      <c r="T8" s="144"/>
-      <c r="U8" s="145"/>
-      <c r="V8" s="146"/>
-      <c r="W8" s="143"/>
-      <c r="X8" s="49"/>
-      <c r="Y8" s="53"/>
-      <c r="Z8" s="54"/>
-      <c r="AA8" s="51"/>
-      <c r="AB8" s="51"/>
-      <c r="AC8" s="37"/>
-      <c r="AD8" s="94"/>
-      <c r="AF8" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="85">
-        <v>14</v>
-      </c>
-      <c r="B9" s="95" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="47"/>
-      <c r="D9" s="37" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E9" s="46">
-        <v>1</v>
-      </c>
-      <c r="F9" s="36"/>
-      <c r="G9" s="73"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="105"/>
-      <c r="K9" s="129"/>
-      <c r="L9" s="152"/>
-      <c r="M9" s="158"/>
-      <c r="N9" s="158"/>
-      <c r="O9" s="164"/>
-      <c r="P9" s="165"/>
-      <c r="Q9" s="159"/>
-      <c r="R9" s="152"/>
-      <c r="S9" s="166"/>
-      <c r="T9" s="160"/>
-      <c r="U9" s="165"/>
-      <c r="V9" s="158"/>
-      <c r="W9" s="152"/>
-      <c r="X9" s="49"/>
-      <c r="Z9" s="50"/>
-      <c r="AA9" s="51"/>
-      <c r="AB9" s="51"/>
-      <c r="AC9" s="37"/>
-      <c r="AD9" s="167"/>
-    </row>
-    <row r="10" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="85">
-        <v>15</v>
-      </c>
-      <c r="B10" s="95" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="58"/>
-      <c r="D10" s="37" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E10" s="57">
-        <v>1</v>
-      </c>
-      <c r="F10" s="48"/>
-      <c r="G10" s="56"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="105"/>
-      <c r="K10" s="129"/>
-      <c r="L10" s="41"/>
-      <c r="M10" s="60"/>
-      <c r="N10" s="60"/>
-      <c r="O10" s="109"/>
-      <c r="P10" s="62"/>
-      <c r="Q10" s="63"/>
-      <c r="R10" s="61"/>
-      <c r="S10" s="63"/>
-      <c r="T10" s="64"/>
-      <c r="U10" s="59"/>
-      <c r="V10" s="60"/>
-      <c r="W10" s="61"/>
-      <c r="X10" s="60"/>
-      <c r="Y10" s="65"/>
-      <c r="Z10" s="66"/>
-      <c r="AA10" s="63"/>
-      <c r="AB10" s="63"/>
-      <c r="AC10" s="67"/>
-      <c r="AD10" s="94"/>
-    </row>
-    <row r="11" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="112">
+      <c r="F10" s="47"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="104"/>
+      <c r="K10" s="128"/>
+      <c r="L10" s="40"/>
+      <c r="M10" s="59"/>
+      <c r="N10" s="59"/>
+      <c r="O10" s="108"/>
+      <c r="P10" s="61"/>
+      <c r="Q10" s="62"/>
+      <c r="R10" s="60"/>
+      <c r="S10" s="62"/>
+      <c r="T10" s="63"/>
+      <c r="U10" s="58"/>
+      <c r="V10" s="59"/>
+      <c r="W10" s="60"/>
+      <c r="X10" s="59"/>
+      <c r="Y10" s="64"/>
+      <c r="Z10" s="65"/>
+      <c r="AA10" s="62"/>
+      <c r="AB10" s="62"/>
+      <c r="AC10" s="66"/>
+      <c r="AD10" s="93"/>
+      <c r="AE10" s="64"/>
+      <c r="AF10" s="64"/>
+      <c r="AG10" s="64"/>
+      <c r="AH10" s="64"/>
+      <c r="AI10" s="205"/>
+      <c r="AJ10" s="220"/>
+      <c r="AK10" s="220"/>
+      <c r="AL10" s="220"/>
+      <c r="AM10" s="220"/>
+      <c r="AN10" s="220"/>
+    </row>
+    <row r="11" spans="1:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="111">
         <v>20</v>
       </c>
-      <c r="B11" s="113" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="126">
+      <c r="B11" s="112" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="125">
         <f>SUM(C12:C14)</f>
         <v>0</v>
       </c>
-      <c r="D11" s="115">
+      <c r="D11" s="114">
         <f>SUM(D12:D14)</f>
         <v>0</v>
       </c>
-      <c r="E11" s="117"/>
-      <c r="F11" s="118"/>
-      <c r="G11" s="122"/>
-      <c r="H11" s="119"/>
-      <c r="I11" s="120"/>
-      <c r="J11" s="121"/>
-      <c r="K11" s="118"/>
-      <c r="L11" s="122"/>
-      <c r="M11" s="123"/>
-      <c r="N11" s="124"/>
-      <c r="O11" s="117"/>
-      <c r="P11" s="114"/>
-      <c r="Q11" s="116"/>
-      <c r="R11" s="147"/>
-      <c r="S11" s="115"/>
-      <c r="T11" s="148"/>
-      <c r="U11" s="149"/>
-      <c r="V11" s="116"/>
-      <c r="W11" s="116"/>
-      <c r="X11" s="123"/>
-      <c r="Y11" s="119"/>
-      <c r="Z11" s="114"/>
-      <c r="AA11" s="123"/>
-      <c r="AB11" s="123"/>
-      <c r="AC11" s="124"/>
-      <c r="AD11" s="125"/>
-    </row>
-    <row r="12" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="86">
+      <c r="E11" s="116"/>
+      <c r="F11" s="117"/>
+      <c r="G11" s="121"/>
+      <c r="H11" s="118"/>
+      <c r="I11" s="119"/>
+      <c r="J11" s="120"/>
+      <c r="K11" s="117"/>
+      <c r="L11" s="121"/>
+      <c r="M11" s="122"/>
+      <c r="N11" s="123"/>
+      <c r="O11" s="116"/>
+      <c r="P11" s="113"/>
+      <c r="Q11" s="115"/>
+      <c r="R11" s="146"/>
+      <c r="S11" s="114"/>
+      <c r="T11" s="147"/>
+      <c r="U11" s="148"/>
+      <c r="V11" s="115"/>
+      <c r="W11" s="115"/>
+      <c r="X11" s="122"/>
+      <c r="Y11" s="118"/>
+      <c r="Z11" s="113"/>
+      <c r="AA11" s="122"/>
+      <c r="AB11" s="122"/>
+      <c r="AC11" s="123"/>
+      <c r="AD11" s="124"/>
+      <c r="AE11" s="121"/>
+      <c r="AF11" s="121"/>
+      <c r="AG11" s="121"/>
+      <c r="AH11" s="121"/>
+      <c r="AI11" s="116"/>
+      <c r="AJ11" s="121"/>
+      <c r="AK11" s="121"/>
+      <c r="AL11" s="121"/>
+      <c r="AM11" s="121"/>
+      <c r="AN11" s="121"/>
+    </row>
+    <row r="12" spans="1:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="85">
         <v>21</v>
       </c>
-      <c r="B12" s="90" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="72" t="str">
+      <c r="B12" s="89" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="35"/>
+      <c r="D12" s="71" t="str">
         <f>IF(SUM(K12:AD12)=0," ",SUM(K12:AD12))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E12" s="35"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="73"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="150"/>
-      <c r="K12" s="36"/>
-      <c r="L12" s="41"/>
-      <c r="M12" s="49"/>
-      <c r="N12" s="41"/>
-      <c r="O12" s="74"/>
-      <c r="P12" s="42"/>
-      <c r="Q12" s="43"/>
-      <c r="R12" s="41"/>
-      <c r="S12" s="43"/>
-      <c r="T12" s="43"/>
-      <c r="U12" s="40"/>
-      <c r="V12" s="41"/>
-      <c r="W12" s="41"/>
-      <c r="X12" s="41"/>
-      <c r="Y12" s="73"/>
-      <c r="Z12" s="45"/>
-      <c r="AA12" s="43"/>
-      <c r="AB12" s="43"/>
-      <c r="AC12" s="72"/>
-      <c r="AD12" s="96"/>
-    </row>
-    <row r="13" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="86">
+      <c r="E12" s="34"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="72"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="149"/>
+      <c r="K12" s="35"/>
+      <c r="L12" s="40"/>
+      <c r="M12" s="48"/>
+      <c r="N12" s="40"/>
+      <c r="O12" s="73"/>
+      <c r="P12" s="41"/>
+      <c r="Q12" s="42"/>
+      <c r="R12" s="40"/>
+      <c r="S12" s="42"/>
+      <c r="T12" s="42"/>
+      <c r="U12" s="39"/>
+      <c r="V12" s="40"/>
+      <c r="W12" s="40"/>
+      <c r="X12" s="40"/>
+      <c r="Y12" s="72"/>
+      <c r="Z12" s="44"/>
+      <c r="AA12" s="42"/>
+      <c r="AB12" s="42"/>
+      <c r="AC12" s="71"/>
+      <c r="AD12" s="95"/>
+      <c r="AE12" s="72"/>
+      <c r="AF12" s="72"/>
+      <c r="AG12" s="72"/>
+      <c r="AH12" s="72"/>
+      <c r="AI12" s="202"/>
+      <c r="AJ12" s="218"/>
+      <c r="AK12" s="218"/>
+      <c r="AL12" s="218"/>
+      <c r="AM12" s="218"/>
+      <c r="AN12" s="218"/>
+    </row>
+    <row r="13" spans="1:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="85">
         <v>22</v>
       </c>
-      <c r="B13" s="90"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="72" t="str">
-        <f t="shared" ref="D13:D14" si="2">IF(SUM(K13:AD13)=0," ",SUM(K13:AD13))</f>
+      <c r="B13" s="89"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="71" t="str">
+        <f>IF(SUM(K13:AD13)=0," ",SUM(K13:AD13))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E13" s="35"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="73"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="105"/>
-      <c r="K13" s="36"/>
-      <c r="L13" s="41"/>
-      <c r="M13" s="49"/>
-      <c r="N13" s="41"/>
-      <c r="O13" s="74"/>
-      <c r="P13" s="42"/>
-      <c r="Q13" s="43"/>
-      <c r="R13" s="41"/>
-      <c r="S13" s="43"/>
-      <c r="T13" s="43"/>
-      <c r="U13" s="40"/>
-      <c r="V13" s="41"/>
-      <c r="W13" s="41"/>
-      <c r="X13" s="41"/>
-      <c r="Y13" s="73"/>
-      <c r="Z13" s="45"/>
-      <c r="AA13" s="43"/>
-      <c r="AB13" s="43"/>
-      <c r="AC13" s="72"/>
-      <c r="AD13" s="96"/>
-    </row>
-    <row r="14" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="86">
+      <c r="E13" s="34"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="72"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="104"/>
+      <c r="K13" s="35"/>
+      <c r="L13" s="40"/>
+      <c r="M13" s="48"/>
+      <c r="N13" s="40"/>
+      <c r="O13" s="73"/>
+      <c r="P13" s="41"/>
+      <c r="Q13" s="42"/>
+      <c r="R13" s="40"/>
+      <c r="S13" s="42"/>
+      <c r="T13" s="42"/>
+      <c r="U13" s="39"/>
+      <c r="V13" s="40"/>
+      <c r="W13" s="40"/>
+      <c r="X13" s="40"/>
+      <c r="Y13" s="72"/>
+      <c r="Z13" s="44"/>
+      <c r="AA13" s="42"/>
+      <c r="AB13" s="42"/>
+      <c r="AC13" s="71"/>
+      <c r="AD13" s="95"/>
+      <c r="AE13" s="72"/>
+      <c r="AF13" s="72"/>
+      <c r="AG13" s="72"/>
+      <c r="AH13" s="72"/>
+      <c r="AI13" s="202"/>
+      <c r="AJ13" s="218"/>
+      <c r="AK13" s="218"/>
+      <c r="AL13" s="218"/>
+      <c r="AM13" s="218"/>
+      <c r="AN13" s="218"/>
+    </row>
+    <row r="14" spans="1:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="85">
         <v>23</v>
       </c>
-      <c r="B14" s="90"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="72" t="str">
-        <f t="shared" si="2"/>
+      <c r="B14" s="89"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="71" t="str">
+        <f>IF(SUM(K14:AD14)=0," ",SUM(K14:AD14))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E14" s="35"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="73"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="105"/>
-      <c r="K14" s="36"/>
-      <c r="L14" s="41"/>
-      <c r="M14" s="49"/>
-      <c r="N14" s="41"/>
-      <c r="O14" s="74"/>
-      <c r="P14" s="42"/>
-      <c r="Q14" s="43"/>
-      <c r="R14" s="41"/>
-      <c r="S14" s="43"/>
-      <c r="T14" s="43"/>
-      <c r="U14" s="40"/>
-      <c r="V14" s="41"/>
-      <c r="W14" s="41"/>
-      <c r="X14" s="41"/>
-      <c r="Y14" s="73"/>
-      <c r="Z14" s="45"/>
-      <c r="AA14" s="43"/>
-      <c r="AB14" s="43"/>
-      <c r="AC14" s="72"/>
-      <c r="AD14" s="96"/>
-    </row>
-    <row r="15" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="112">
+      <c r="E14" s="34"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="72"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="104"/>
+      <c r="K14" s="35"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="48"/>
+      <c r="N14" s="40"/>
+      <c r="O14" s="73"/>
+      <c r="P14" s="41"/>
+      <c r="Q14" s="42"/>
+      <c r="R14" s="40"/>
+      <c r="S14" s="42"/>
+      <c r="T14" s="42"/>
+      <c r="U14" s="39"/>
+      <c r="V14" s="40"/>
+      <c r="W14" s="40"/>
+      <c r="X14" s="40"/>
+      <c r="Y14" s="72"/>
+      <c r="Z14" s="44"/>
+      <c r="AA14" s="42"/>
+      <c r="AB14" s="42"/>
+      <c r="AC14" s="71"/>
+      <c r="AD14" s="95"/>
+      <c r="AE14" s="72"/>
+      <c r="AF14" s="72"/>
+      <c r="AG14" s="72"/>
+      <c r="AH14" s="72"/>
+      <c r="AI14" s="202"/>
+      <c r="AJ14" s="218"/>
+      <c r="AK14" s="218"/>
+      <c r="AL14" s="218"/>
+      <c r="AM14" s="218"/>
+      <c r="AN14" s="218"/>
+    </row>
+    <row r="15" spans="1:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="111">
         <v>30</v>
       </c>
-      <c r="B15" s="113" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="115">
+      <c r="B15" s="112" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="114">
         <f>SUM(C16:C23)</f>
         <v>81</v>
       </c>
-      <c r="D15" s="116">
+      <c r="D15" s="115">
         <f>SUM(D16:D23)</f>
         <v>30</v>
       </c>
-      <c r="E15" s="117"/>
-      <c r="F15" s="118"/>
-      <c r="G15" s="122"/>
-      <c r="H15" s="119"/>
-      <c r="I15" s="120"/>
-      <c r="J15" s="121"/>
-      <c r="K15" s="118"/>
-      <c r="L15" s="122"/>
-      <c r="M15" s="123"/>
-      <c r="N15" s="124"/>
-      <c r="O15" s="117"/>
-      <c r="P15" s="114"/>
-      <c r="Q15" s="116"/>
-      <c r="R15" s="147"/>
-      <c r="S15" s="115"/>
-      <c r="T15" s="148"/>
-      <c r="U15" s="149"/>
-      <c r="V15" s="116"/>
-      <c r="W15" s="116"/>
-      <c r="X15" s="123"/>
-      <c r="Y15" s="119"/>
-      <c r="Z15" s="114"/>
-      <c r="AA15" s="123"/>
-      <c r="AB15" s="123"/>
-      <c r="AC15" s="124"/>
-      <c r="AD15" s="125"/>
-    </row>
-    <row r="16" spans="1:34" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="86">
+      <c r="E15" s="116"/>
+      <c r="F15" s="117"/>
+      <c r="G15" s="121"/>
+      <c r="H15" s="118"/>
+      <c r="I15" s="119"/>
+      <c r="J15" s="120"/>
+      <c r="K15" s="117"/>
+      <c r="L15" s="121"/>
+      <c r="M15" s="122"/>
+      <c r="N15" s="123"/>
+      <c r="O15" s="116"/>
+      <c r="P15" s="113"/>
+      <c r="Q15" s="115"/>
+      <c r="R15" s="146"/>
+      <c r="S15" s="114"/>
+      <c r="T15" s="147"/>
+      <c r="U15" s="148"/>
+      <c r="V15" s="115"/>
+      <c r="W15" s="115"/>
+      <c r="X15" s="122"/>
+      <c r="Y15" s="118"/>
+      <c r="Z15" s="113"/>
+      <c r="AA15" s="122"/>
+      <c r="AB15" s="122"/>
+      <c r="AC15" s="123"/>
+      <c r="AD15" s="124"/>
+      <c r="AE15" s="214"/>
+      <c r="AF15" s="214"/>
+      <c r="AG15" s="214"/>
+      <c r="AH15" s="121"/>
+      <c r="AI15" s="116"/>
+      <c r="AJ15" s="214"/>
+      <c r="AK15" s="214"/>
+      <c r="AL15" s="214"/>
+      <c r="AM15" s="214"/>
+      <c r="AN15" s="214"/>
+    </row>
+    <row r="16" spans="1:41" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="85">
         <v>31</v>
       </c>
-      <c r="B16" s="97" t="s">
+      <c r="B16" s="96" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="35">
+        <v>4</v>
+      </c>
+      <c r="D16" s="71">
+        <v>6</v>
+      </c>
+      <c r="E16" s="34">
+        <v>1</v>
+      </c>
+      <c r="F16" s="35"/>
+      <c r="G16" s="72"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="149"/>
+      <c r="K16" s="150"/>
+      <c r="L16" s="161"/>
+      <c r="M16" s="161"/>
+      <c r="N16" s="171"/>
+      <c r="O16" s="163"/>
+      <c r="P16" s="169"/>
+      <c r="Q16" s="161"/>
+      <c r="R16" s="161"/>
+      <c r="S16" s="169"/>
+      <c r="T16" s="172"/>
+      <c r="U16" s="170"/>
+      <c r="V16" s="161"/>
+      <c r="W16" s="161"/>
+      <c r="X16" s="167"/>
+      <c r="Y16" s="155"/>
+      <c r="Z16" s="153"/>
+      <c r="AA16" s="161"/>
+      <c r="AB16" s="161"/>
+      <c r="AC16" s="71"/>
+      <c r="AD16" s="213"/>
+      <c r="AE16" s="216"/>
+      <c r="AF16" s="216"/>
+      <c r="AG16" s="216"/>
+      <c r="AH16" s="150"/>
+      <c r="AI16" s="206"/>
+      <c r="AJ16" s="176"/>
+      <c r="AK16" s="176"/>
+      <c r="AL16" s="176"/>
+      <c r="AM16" s="176"/>
+      <c r="AN16" s="176"/>
+    </row>
+    <row r="17" spans="1:40" ht="14.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="85">
+        <v>32</v>
+      </c>
+      <c r="B17" s="96" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="36">
-        <v>4</v>
-      </c>
-      <c r="D16" s="72">
-        <v>6</v>
-      </c>
-      <c r="E16" s="35">
+      <c r="C17" s="35">
+        <v>17</v>
+      </c>
+      <c r="D17" s="71">
+        <v>24</v>
+      </c>
+      <c r="E17" s="34">
         <v>1</v>
       </c>
-      <c r="F16" s="36"/>
-      <c r="G16" s="73"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="150"/>
-      <c r="K16" s="151"/>
-      <c r="L16" s="162"/>
-      <c r="M16" s="162"/>
-      <c r="N16" s="172"/>
-      <c r="O16" s="164"/>
-      <c r="P16" s="170"/>
-      <c r="Q16" s="162"/>
-      <c r="R16" s="162"/>
-      <c r="S16" s="170"/>
-      <c r="T16" s="173"/>
-      <c r="U16" s="171"/>
-      <c r="V16" s="162"/>
-      <c r="W16" s="162"/>
-      <c r="X16" s="168"/>
-      <c r="Y16" s="156"/>
-      <c r="Z16" s="154"/>
-      <c r="AA16" s="162"/>
-      <c r="AB16" s="162"/>
-      <c r="AC16" s="72"/>
-      <c r="AD16" s="96"/>
-    </row>
-    <row r="17" spans="1:34" ht="14.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="86">
-        <v>32</v>
-      </c>
-      <c r="B17" s="97" t="s">
+      <c r="F17" s="35"/>
+      <c r="G17" s="72"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="149"/>
+      <c r="K17" s="150"/>
+      <c r="L17" s="161"/>
+      <c r="M17" s="161"/>
+      <c r="N17" s="151"/>
+      <c r="O17" s="163"/>
+      <c r="P17" s="163"/>
+      <c r="Q17" s="161"/>
+      <c r="R17" s="161"/>
+      <c r="S17" s="170"/>
+      <c r="T17" s="172"/>
+      <c r="U17" s="167"/>
+      <c r="V17" s="161"/>
+      <c r="W17" s="161"/>
+      <c r="X17" s="168"/>
+      <c r="Y17" s="167"/>
+      <c r="Z17" s="153"/>
+      <c r="AA17" s="161"/>
+      <c r="AB17" s="161"/>
+      <c r="AC17" s="71"/>
+      <c r="AD17" s="213"/>
+      <c r="AE17" s="212"/>
+      <c r="AF17" s="212"/>
+      <c r="AG17" s="212"/>
+      <c r="AH17" s="35"/>
+      <c r="AI17" s="202"/>
+      <c r="AJ17" s="176"/>
+      <c r="AK17" s="176"/>
+      <c r="AL17" s="176"/>
+      <c r="AM17" s="176"/>
+      <c r="AN17" s="176"/>
+    </row>
+    <row r="18" spans="1:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="85">
+        <v>33</v>
+      </c>
+      <c r="B18" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="36">
-        <v>17</v>
-      </c>
-      <c r="D17" s="72">
-        <v>24</v>
-      </c>
-      <c r="E17" s="35">
-        <v>1</v>
-      </c>
-      <c r="F17" s="36"/>
-      <c r="G17" s="73"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="39"/>
-      <c r="J17" s="150"/>
-      <c r="K17" s="151"/>
-      <c r="L17" s="162"/>
-      <c r="M17" s="162"/>
-      <c r="N17" s="152"/>
-      <c r="O17" s="164"/>
-      <c r="P17" s="164"/>
-      <c r="Q17" s="162"/>
-      <c r="R17" s="162"/>
-      <c r="S17" s="171"/>
-      <c r="T17" s="173"/>
-      <c r="U17" s="168"/>
-      <c r="V17" s="162"/>
-      <c r="W17" s="162"/>
-      <c r="X17" s="169"/>
-      <c r="Y17" s="168"/>
-      <c r="Z17" s="154"/>
-      <c r="AA17" s="162"/>
-      <c r="AB17" s="162"/>
-      <c r="AC17" s="72"/>
-      <c r="AD17" s="96"/>
-    </row>
-    <row r="18" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="86">
-        <v>33</v>
-      </c>
-      <c r="B18" s="97" t="s">
+      <c r="C18" s="35">
+        <v>9</v>
+      </c>
+      <c r="D18" s="71"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="72"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="149"/>
+      <c r="K18" s="150"/>
+      <c r="L18" s="161"/>
+      <c r="M18" s="161"/>
+      <c r="N18" s="151"/>
+      <c r="O18" s="152"/>
+      <c r="P18" s="50"/>
+      <c r="Q18" s="161"/>
+      <c r="R18" s="161"/>
+      <c r="S18" s="154"/>
+      <c r="T18" s="172"/>
+      <c r="U18" s="153"/>
+      <c r="V18" s="161"/>
+      <c r="W18" s="161"/>
+      <c r="X18" s="151"/>
+      <c r="Y18" s="155"/>
+      <c r="Z18" s="153"/>
+      <c r="AA18" s="161"/>
+      <c r="AB18" s="161"/>
+      <c r="AD18" s="213"/>
+      <c r="AE18" s="216"/>
+      <c r="AF18" s="216"/>
+      <c r="AG18" s="216"/>
+      <c r="AH18" s="150"/>
+      <c r="AI18" s="206"/>
+      <c r="AJ18" s="176"/>
+      <c r="AK18" s="176"/>
+      <c r="AL18" s="176"/>
+      <c r="AM18" s="176"/>
+      <c r="AN18" s="176"/>
+    </row>
+    <row r="19" spans="1:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="85">
+        <v>34</v>
+      </c>
+      <c r="B19" s="96" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="36">
-        <v>9</v>
-      </c>
-      <c r="D18" s="72"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="73"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="150"/>
-      <c r="K18" s="151"/>
-      <c r="L18" s="162"/>
-      <c r="M18" s="162"/>
-      <c r="N18" s="152"/>
-      <c r="O18" s="153"/>
-      <c r="P18" s="51"/>
-      <c r="Q18" s="162"/>
-      <c r="R18" s="162"/>
-      <c r="S18" s="155"/>
-      <c r="T18" s="173"/>
-      <c r="U18" s="154"/>
-      <c r="V18" s="162"/>
-      <c r="W18" s="162"/>
-      <c r="X18" s="152"/>
-      <c r="Y18" s="156"/>
-      <c r="Z18" s="154"/>
-      <c r="AA18" s="162"/>
-      <c r="AB18" s="162"/>
-      <c r="AD18" s="96"/>
-    </row>
-    <row r="19" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="86">
-        <v>34</v>
-      </c>
-      <c r="B19" s="97" t="s">
+      <c r="C19" s="35">
+        <v>15</v>
+      </c>
+      <c r="D19" s="71"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="72"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="155"/>
+      <c r="J19" s="153"/>
+      <c r="K19" s="150"/>
+      <c r="L19" s="161"/>
+      <c r="M19" s="161"/>
+      <c r="N19" s="35"/>
+      <c r="O19" s="72"/>
+      <c r="P19" s="153"/>
+      <c r="Q19" s="161"/>
+      <c r="R19" s="161"/>
+      <c r="T19" s="172"/>
+      <c r="U19" s="153"/>
+      <c r="V19" s="161"/>
+      <c r="W19" s="161"/>
+      <c r="X19" s="151"/>
+      <c r="Y19" s="155"/>
+      <c r="Z19" s="167"/>
+      <c r="AA19" s="161"/>
+      <c r="AB19" s="161"/>
+      <c r="AC19" s="167"/>
+      <c r="AD19" s="169"/>
+      <c r="AE19" s="216"/>
+      <c r="AF19" s="216"/>
+      <c r="AG19" s="216"/>
+      <c r="AH19" s="155"/>
+      <c r="AI19" s="206"/>
+      <c r="AJ19" s="176"/>
+      <c r="AK19" s="176"/>
+      <c r="AL19" s="176"/>
+      <c r="AM19" s="176"/>
+      <c r="AN19" s="176"/>
+    </row>
+    <row r="20" spans="1:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="85">
+        <v>35</v>
+      </c>
+      <c r="B20" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="36">
+      <c r="C20" s="35">
+        <v>8</v>
+      </c>
+      <c r="D20" s="71"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="72"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="155"/>
+      <c r="J20" s="153"/>
+      <c r="K20" s="154"/>
+      <c r="L20" s="161"/>
+      <c r="M20" s="161"/>
+      <c r="N20" s="35"/>
+      <c r="O20" s="72"/>
+      <c r="P20" s="153"/>
+      <c r="Q20" s="161"/>
+      <c r="R20" s="161"/>
+      <c r="S20" s="50"/>
+      <c r="T20" s="172"/>
+      <c r="U20" s="153"/>
+      <c r="V20" s="161"/>
+      <c r="W20" s="161"/>
+      <c r="X20" s="151"/>
+      <c r="Y20" s="151"/>
+      <c r="AA20" s="161"/>
+      <c r="AB20" s="161"/>
+      <c r="AC20" s="71"/>
+      <c r="AD20" s="213"/>
+      <c r="AE20" s="211"/>
+      <c r="AF20" s="211"/>
+      <c r="AG20" s="211"/>
+      <c r="AH20" s="201"/>
+      <c r="AI20" s="207"/>
+      <c r="AJ20" s="176"/>
+      <c r="AK20" s="176"/>
+      <c r="AL20" s="176"/>
+      <c r="AM20" s="176"/>
+      <c r="AN20" s="176"/>
+    </row>
+    <row r="21" spans="1:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="85">
+        <v>36</v>
+      </c>
+      <c r="B21" s="96" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="35">
+        <v>10</v>
+      </c>
+      <c r="D21" s="71"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="72"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="155"/>
+      <c r="J21" s="153"/>
+      <c r="K21" s="150"/>
+      <c r="L21" s="161"/>
+      <c r="M21" s="161"/>
+      <c r="N21" s="35"/>
+      <c r="O21" s="72"/>
+      <c r="P21" s="153"/>
+      <c r="Q21" s="161"/>
+      <c r="R21" s="161"/>
+      <c r="S21" s="50"/>
+      <c r="T21" s="172"/>
+      <c r="U21" s="153"/>
+      <c r="V21" s="161"/>
+      <c r="W21" s="161"/>
+      <c r="X21" s="42"/>
+      <c r="Y21" s="42"/>
+      <c r="Z21" s="41"/>
+      <c r="AA21" s="161"/>
+      <c r="AB21" s="161"/>
+      <c r="AC21" s="71"/>
+      <c r="AD21" s="213"/>
+      <c r="AE21" s="216"/>
+      <c r="AF21" s="216"/>
+      <c r="AG21" s="216"/>
+      <c r="AH21" s="35"/>
+      <c r="AI21" s="202"/>
+      <c r="AJ21" s="176"/>
+      <c r="AK21" s="176"/>
+      <c r="AL21" s="176"/>
+      <c r="AM21" s="176"/>
+      <c r="AN21" s="176"/>
+    </row>
+    <row r="22" spans="1:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="85">
+        <v>37</v>
+      </c>
+      <c r="B22" s="96" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="35">
         <v>15</v>
       </c>
-      <c r="D19" s="72"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="73"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="156"/>
-      <c r="J19" s="154"/>
-      <c r="K19" s="151"/>
-      <c r="L19" s="162"/>
-      <c r="M19" s="162"/>
-      <c r="N19" s="36"/>
-      <c r="O19" s="73"/>
-      <c r="P19" s="154"/>
-      <c r="Q19" s="162"/>
-      <c r="R19" s="162"/>
-      <c r="T19" s="173"/>
-      <c r="U19" s="154"/>
-      <c r="V19" s="162"/>
-      <c r="W19" s="162"/>
-      <c r="X19" s="152"/>
-      <c r="Y19" s="156"/>
-      <c r="Z19" s="168"/>
-      <c r="AA19" s="162"/>
-      <c r="AB19" s="162"/>
-      <c r="AC19" s="168"/>
-      <c r="AD19" s="168"/>
-    </row>
-    <row r="20" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="86">
-        <v>35</v>
-      </c>
-      <c r="B20" s="97" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="36">
-        <v>8</v>
-      </c>
-      <c r="D20" s="72"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="73"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="156"/>
-      <c r="J20" s="154"/>
-      <c r="K20" s="155"/>
-      <c r="L20" s="162"/>
-      <c r="M20" s="162"/>
-      <c r="N20" s="36"/>
-      <c r="O20" s="73"/>
-      <c r="P20" s="154"/>
-      <c r="Q20" s="162"/>
-      <c r="R20" s="162"/>
-      <c r="S20" s="51"/>
-      <c r="T20" s="173"/>
-      <c r="U20" s="154"/>
-      <c r="V20" s="162"/>
-      <c r="W20" s="162"/>
-      <c r="X20" s="152"/>
-      <c r="Y20" s="152"/>
-      <c r="AA20" s="162"/>
-      <c r="AB20" s="162"/>
-      <c r="AC20" s="72"/>
-      <c r="AD20" s="96"/>
-    </row>
-    <row r="21" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="86">
-        <v>36</v>
-      </c>
-      <c r="B21" s="97" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" s="36">
-        <v>10</v>
-      </c>
-      <c r="D21" s="72"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="73"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="156"/>
-      <c r="J21" s="154"/>
-      <c r="K21" s="151"/>
-      <c r="L21" s="162"/>
-      <c r="M21" s="162"/>
-      <c r="N21" s="36"/>
-      <c r="O21" s="73"/>
-      <c r="P21" s="154"/>
-      <c r="Q21" s="162"/>
-      <c r="R21" s="162"/>
-      <c r="S21" s="51"/>
-      <c r="T21" s="173"/>
-      <c r="U21" s="154"/>
-      <c r="V21" s="162"/>
-      <c r="W21" s="162"/>
-      <c r="X21" s="43"/>
-      <c r="Y21" s="43"/>
-      <c r="Z21" s="42"/>
-      <c r="AA21" s="162"/>
-      <c r="AB21" s="162"/>
-      <c r="AC21" s="72"/>
-      <c r="AD21" s="96"/>
-    </row>
-    <row r="22" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="86">
-        <v>37</v>
-      </c>
-      <c r="B22" s="97" t="s">
+      <c r="D22" s="71"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="72"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="155"/>
+      <c r="J22" s="153"/>
+      <c r="K22" s="150"/>
+      <c r="L22" s="161"/>
+      <c r="M22" s="161"/>
+      <c r="N22" s="35"/>
+      <c r="O22" s="72"/>
+      <c r="P22" s="153"/>
+      <c r="Q22" s="161"/>
+      <c r="R22" s="161"/>
+      <c r="S22" s="160"/>
+      <c r="T22" s="172"/>
+      <c r="U22" s="153"/>
+      <c r="V22" s="161"/>
+      <c r="W22" s="161"/>
+      <c r="X22" s="42"/>
+      <c r="Y22" s="42"/>
+      <c r="Z22" s="41"/>
+      <c r="AA22" s="161"/>
+      <c r="AB22" s="161"/>
+      <c r="AC22" s="42"/>
+      <c r="AD22" s="213"/>
+      <c r="AE22" s="216"/>
+      <c r="AF22" s="216"/>
+      <c r="AG22" s="216"/>
+      <c r="AH22" s="35"/>
+      <c r="AI22" s="202"/>
+      <c r="AJ22" s="176"/>
+      <c r="AK22" s="176"/>
+      <c r="AL22" s="176"/>
+      <c r="AM22" s="176"/>
+      <c r="AN22" s="176"/>
+    </row>
+    <row r="23" spans="1:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="85">
+        <v>38</v>
+      </c>
+      <c r="B23" s="96" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="36">
-        <v>15</v>
-      </c>
-      <c r="D22" s="72"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="73"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="156"/>
-      <c r="J22" s="154"/>
-      <c r="K22" s="151"/>
-      <c r="L22" s="162"/>
-      <c r="M22" s="162"/>
-      <c r="N22" s="36"/>
-      <c r="O22" s="73"/>
-      <c r="P22" s="154"/>
-      <c r="Q22" s="162"/>
-      <c r="R22" s="162"/>
-      <c r="S22" s="161"/>
-      <c r="T22" s="173"/>
-      <c r="U22" s="154"/>
-      <c r="V22" s="162"/>
-      <c r="W22" s="162"/>
-      <c r="X22" s="43"/>
-      <c r="Y22" s="43"/>
-      <c r="Z22" s="42"/>
-      <c r="AA22" s="162"/>
-      <c r="AB22" s="162"/>
-      <c r="AC22" s="43"/>
-      <c r="AD22" s="96"/>
-    </row>
-    <row r="23" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="86">
-        <v>38</v>
-      </c>
-      <c r="B23" s="97" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" s="47">
+      <c r="C23" s="46">
         <v>3</v>
       </c>
-      <c r="D23" s="37" t="str">
+      <c r="D23" s="36" t="str">
         <f>IF(SUM(K23:AD23)=0," ",SUM(K23:AD23))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E23" s="46"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="150"/>
-      <c r="K23" s="157"/>
-      <c r="L23" s="163"/>
-      <c r="M23" s="163"/>
-      <c r="N23" s="36"/>
-      <c r="O23" s="73"/>
-      <c r="P23" s="154"/>
-      <c r="Q23" s="163"/>
-      <c r="R23" s="162"/>
-      <c r="S23" s="159"/>
-      <c r="T23" s="173"/>
-      <c r="U23" s="154"/>
-      <c r="V23" s="163"/>
-      <c r="W23" s="162"/>
-      <c r="X23" s="156"/>
-      <c r="Y23" s="43"/>
-      <c r="Z23" s="42"/>
-      <c r="AA23" s="163"/>
-      <c r="AB23" s="163"/>
-      <c r="AC23" s="43"/>
-      <c r="AD23" s="96"/>
-    </row>
-    <row r="24" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="86"/>
-      <c r="B24" s="97" t="s">
+      <c r="E23" s="45"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="149"/>
+      <c r="K23" s="156"/>
+      <c r="L23" s="162"/>
+      <c r="M23" s="162"/>
+      <c r="N23" s="35"/>
+      <c r="O23" s="72"/>
+      <c r="P23" s="153"/>
+      <c r="Q23" s="162"/>
+      <c r="R23" s="161"/>
+      <c r="S23" s="158"/>
+      <c r="T23" s="172"/>
+      <c r="U23" s="153"/>
+      <c r="V23" s="162"/>
+      <c r="W23" s="161"/>
+      <c r="X23" s="155"/>
+      <c r="Y23" s="42"/>
+      <c r="Z23" s="41"/>
+      <c r="AA23" s="162"/>
+      <c r="AB23" s="162"/>
+      <c r="AC23" s="42"/>
+      <c r="AD23" s="213"/>
+      <c r="AE23" s="216"/>
+      <c r="AF23" s="216"/>
+      <c r="AG23" s="216"/>
+      <c r="AH23" s="35"/>
+      <c r="AI23" s="202"/>
+      <c r="AJ23" s="176"/>
+      <c r="AK23" s="176"/>
+      <c r="AL23" s="176"/>
+      <c r="AM23" s="176"/>
+      <c r="AN23" s="176"/>
+    </row>
+    <row r="24" spans="1:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="85"/>
+      <c r="B24" s="96" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="46">
+        <v>4</v>
+      </c>
+      <c r="D24" s="36">
+        <v>2</v>
+      </c>
+      <c r="E24" s="45">
+        <v>1</v>
+      </c>
+      <c r="F24" s="35"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="155"/>
+      <c r="J24" s="149"/>
+      <c r="K24" s="156"/>
+      <c r="L24" s="162"/>
+      <c r="M24" s="162"/>
+      <c r="N24" s="35"/>
+      <c r="O24" s="35"/>
+      <c r="P24" s="153"/>
+      <c r="Q24" s="162"/>
+      <c r="R24" s="162"/>
+      <c r="S24" s="35"/>
+      <c r="T24" s="172"/>
+      <c r="U24" s="153"/>
+      <c r="V24" s="162"/>
+      <c r="W24" s="162"/>
+      <c r="X24" s="168"/>
+      <c r="Y24" s="42"/>
+      <c r="Z24" s="41"/>
+      <c r="AA24" s="162"/>
+      <c r="AB24" s="162"/>
+      <c r="AC24" s="42"/>
+      <c r="AD24" s="213"/>
+      <c r="AE24" s="216"/>
+      <c r="AF24" s="216"/>
+      <c r="AG24" s="216"/>
+      <c r="AH24" s="35"/>
+      <c r="AI24" s="202"/>
+      <c r="AJ24" s="176"/>
+      <c r="AK24" s="176"/>
+      <c r="AL24" s="176"/>
+      <c r="AM24" s="176"/>
+      <c r="AN24" s="176"/>
+    </row>
+    <row r="25" spans="1:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="85"/>
+      <c r="B25" s="96" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="47">
+      <c r="C25" s="46">
         <v>4</v>
       </c>
-      <c r="D24" s="37">
+      <c r="D25" s="36">
         <v>2</v>
       </c>
-      <c r="E24" s="46">
+      <c r="E25" s="45">
         <v>1</v>
       </c>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="156"/>
-      <c r="J24" s="150"/>
-      <c r="K24" s="157"/>
-      <c r="L24" s="163"/>
-      <c r="M24" s="163"/>
-      <c r="N24" s="36"/>
-      <c r="O24" s="36"/>
-      <c r="P24" s="154"/>
-      <c r="Q24" s="163"/>
-      <c r="R24" s="163"/>
-      <c r="S24" s="36"/>
-      <c r="T24" s="173"/>
-      <c r="U24" s="154"/>
-      <c r="V24" s="163"/>
-      <c r="W24" s="163"/>
-      <c r="X24" s="169"/>
-      <c r="Y24" s="43"/>
-      <c r="Z24" s="42"/>
-      <c r="AA24" s="163"/>
-      <c r="AB24" s="163"/>
-      <c r="AC24" s="43"/>
-      <c r="AD24" s="96"/>
-    </row>
-    <row r="25" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="86"/>
-      <c r="B25" s="97" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25" s="47">
-        <v>4</v>
-      </c>
-      <c r="D25" s="37">
+      <c r="F25" s="35"/>
+      <c r="G25" s="79"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="155"/>
+      <c r="J25" s="149"/>
+      <c r="K25" s="156"/>
+      <c r="L25" s="162"/>
+      <c r="M25" s="162"/>
+      <c r="N25" s="35"/>
+      <c r="O25" s="35"/>
+      <c r="P25" s="153"/>
+      <c r="Q25" s="162"/>
+      <c r="R25" s="162"/>
+      <c r="S25" s="35"/>
+      <c r="T25" s="172"/>
+      <c r="U25" s="153"/>
+      <c r="V25" s="162"/>
+      <c r="W25" s="162"/>
+      <c r="X25" s="42"/>
+      <c r="Y25" s="168"/>
+      <c r="Z25" s="41"/>
+      <c r="AA25" s="162"/>
+      <c r="AB25" s="162"/>
+      <c r="AC25" s="42"/>
+      <c r="AD25" s="213"/>
+      <c r="AE25" s="212"/>
+      <c r="AF25" s="212"/>
+      <c r="AG25" s="212"/>
+      <c r="AH25" s="35"/>
+      <c r="AI25" s="202"/>
+      <c r="AJ25" s="176"/>
+      <c r="AK25" s="176"/>
+      <c r="AL25" s="176"/>
+      <c r="AM25" s="176"/>
+      <c r="AN25" s="176"/>
+    </row>
+    <row r="26" spans="1:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="85"/>
+      <c r="B26" s="179" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="79">
+        <v>16</v>
+      </c>
+      <c r="D26" s="78">
+        <v>19.5</v>
+      </c>
+      <c r="E26" s="45">
         <v>2</v>
       </c>
-      <c r="E25" s="46">
+      <c r="F26" s="67"/>
+      <c r="G26" s="79"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="180"/>
+      <c r="J26" s="181"/>
+      <c r="K26" s="180"/>
+      <c r="L26" s="182"/>
+      <c r="M26" s="183"/>
+      <c r="N26" s="67"/>
+      <c r="O26" s="79"/>
+      <c r="P26" s="184"/>
+      <c r="Q26" s="183"/>
+      <c r="R26" s="185"/>
+      <c r="S26" s="79"/>
+      <c r="T26" s="172"/>
+      <c r="U26" s="184"/>
+      <c r="V26" s="183"/>
+      <c r="W26" s="183"/>
+      <c r="X26" s="78"/>
+      <c r="Y26" s="178"/>
+      <c r="Z26" s="178"/>
+      <c r="AA26" s="183"/>
+      <c r="AB26" s="183"/>
+      <c r="AC26" s="178"/>
+      <c r="AD26" s="178"/>
+      <c r="AE26" s="212"/>
+      <c r="AF26" s="212"/>
+      <c r="AG26" s="212"/>
+      <c r="AH26" s="35"/>
+      <c r="AI26" s="202"/>
+      <c r="AJ26" s="176"/>
+      <c r="AK26" s="176"/>
+      <c r="AL26" s="176"/>
+      <c r="AM26" s="176"/>
+      <c r="AN26" s="176"/>
+    </row>
+    <row r="27" spans="1:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="85"/>
+      <c r="B27" s="179" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="79">
+        <v>10</v>
+      </c>
+      <c r="D27" s="71"/>
+      <c r="E27" s="34">
         <v>1</v>
       </c>
-      <c r="F25" s="36"/>
-      <c r="G25" s="80"/>
-      <c r="H25" s="38"/>
-      <c r="I25" s="156"/>
-      <c r="J25" s="150"/>
-      <c r="K25" s="157"/>
-      <c r="L25" s="163"/>
-      <c r="M25" s="163"/>
-      <c r="N25" s="36"/>
-      <c r="O25" s="36"/>
-      <c r="P25" s="154"/>
-      <c r="Q25" s="163"/>
-      <c r="R25" s="163"/>
-      <c r="S25" s="36"/>
-      <c r="T25" s="173"/>
-      <c r="U25" s="154"/>
-      <c r="V25" s="163"/>
-      <c r="W25" s="163"/>
-      <c r="X25" s="43"/>
-      <c r="Y25" s="169"/>
-      <c r="Z25" s="42"/>
-      <c r="AA25" s="163"/>
-      <c r="AB25" s="163"/>
-      <c r="AC25" s="43"/>
-      <c r="AD25" s="96"/>
-    </row>
-    <row r="26" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="86"/>
-      <c r="B26" s="180" t="s">
-        <v>57</v>
-      </c>
-      <c r="C26" s="80">
-        <v>16</v>
-      </c>
-      <c r="D26" s="79">
-        <v>19.5</v>
-      </c>
-      <c r="E26" s="46">
-        <v>2</v>
-      </c>
-      <c r="F26" s="68"/>
-      <c r="G26" s="80"/>
-      <c r="H26" s="38"/>
-      <c r="I26" s="181"/>
-      <c r="J26" s="182"/>
-      <c r="K26" s="181"/>
-      <c r="L26" s="183"/>
-      <c r="M26" s="184"/>
-      <c r="N26" s="68"/>
-      <c r="O26" s="80"/>
-      <c r="P26" s="185"/>
-      <c r="Q26" s="184"/>
-      <c r="R26" s="186"/>
-      <c r="S26" s="80"/>
-      <c r="T26" s="173"/>
-      <c r="U26" s="185"/>
-      <c r="V26" s="184"/>
-      <c r="W26" s="184"/>
-      <c r="X26" s="79"/>
-      <c r="Y26" s="179"/>
-      <c r="Z26" s="179"/>
-      <c r="AA26" s="184"/>
-      <c r="AB26" s="184"/>
-      <c r="AC26" s="179"/>
-      <c r="AD26" s="179"/>
-    </row>
-    <row r="27" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="112">
+      <c r="F27" s="67"/>
+      <c r="G27" s="79"/>
+      <c r="H27" s="68"/>
+      <c r="I27" s="180"/>
+      <c r="J27" s="181"/>
+      <c r="K27" s="180"/>
+      <c r="L27" s="182"/>
+      <c r="M27" s="183"/>
+      <c r="N27" s="67"/>
+      <c r="O27" s="79"/>
+      <c r="P27" s="184"/>
+      <c r="Q27" s="183"/>
+      <c r="R27" s="185"/>
+      <c r="S27" s="79"/>
+      <c r="T27" s="172"/>
+      <c r="U27" s="184"/>
+      <c r="V27" s="183"/>
+      <c r="W27" s="183"/>
+      <c r="X27" s="78"/>
+      <c r="Y27" s="217"/>
+      <c r="Z27" s="41"/>
+      <c r="AA27" s="183"/>
+      <c r="AB27" s="183"/>
+      <c r="AC27" s="42"/>
+      <c r="AD27" s="213"/>
+      <c r="AE27" s="212"/>
+      <c r="AF27" s="212"/>
+      <c r="AG27" s="212"/>
+      <c r="AH27" s="178"/>
+      <c r="AI27" s="178"/>
+      <c r="AJ27" s="176"/>
+      <c r="AK27" s="176"/>
+      <c r="AL27" s="176"/>
+      <c r="AM27" s="176"/>
+      <c r="AN27" s="176"/>
+    </row>
+    <row r="28" spans="1:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="111">
         <v>40</v>
       </c>
-      <c r="B27" s="113" t="s">
-        <v>9</v>
-      </c>
-      <c r="C27" s="115">
-        <f>SUM(C28:C31)</f>
-        <v>0</v>
-      </c>
-      <c r="D27" s="116">
-        <f>SUM(D28:D31)</f>
-        <v>0</v>
-      </c>
-      <c r="E27" s="122"/>
-      <c r="F27" s="118"/>
-      <c r="G27" s="122"/>
-      <c r="H27" s="119"/>
-      <c r="I27" s="120"/>
-      <c r="J27" s="121"/>
-      <c r="K27" s="118"/>
-      <c r="L27" s="122"/>
-      <c r="M27" s="123"/>
-      <c r="N27" s="124"/>
-      <c r="O27" s="117"/>
-      <c r="P27" s="114"/>
-      <c r="Q27" s="123"/>
-      <c r="R27" s="124"/>
-      <c r="S27" s="122"/>
-      <c r="T27" s="119"/>
-      <c r="U27" s="114"/>
-      <c r="V27" s="123"/>
-      <c r="W27" s="123"/>
-      <c r="X27" s="123"/>
-      <c r="Y27" s="119"/>
-      <c r="Z27" s="114"/>
-      <c r="AA27" s="123"/>
-      <c r="AB27" s="123"/>
-      <c r="AC27" s="124"/>
-      <c r="AD27" s="125"/>
-      <c r="AH27" s="73"/>
-    </row>
-    <row r="28" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="86">
+      <c r="B28" s="112" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="114">
+        <f>SUM(C29:C32)</f>
+        <v>0</v>
+      </c>
+      <c r="D28" s="115">
+        <f>SUM(D29:D32)</f>
+        <v>0</v>
+      </c>
+      <c r="E28" s="121"/>
+      <c r="F28" s="117"/>
+      <c r="G28" s="121"/>
+      <c r="H28" s="118"/>
+      <c r="I28" s="119"/>
+      <c r="J28" s="120"/>
+      <c r="K28" s="117"/>
+      <c r="L28" s="121"/>
+      <c r="M28" s="122"/>
+      <c r="N28" s="123"/>
+      <c r="O28" s="116"/>
+      <c r="P28" s="113"/>
+      <c r="Q28" s="122"/>
+      <c r="R28" s="123"/>
+      <c r="S28" s="121"/>
+      <c r="T28" s="118"/>
+      <c r="U28" s="113"/>
+      <c r="V28" s="122"/>
+      <c r="W28" s="122"/>
+      <c r="X28" s="122"/>
+      <c r="Y28" s="118"/>
+      <c r="Z28" s="113"/>
+      <c r="AA28" s="122"/>
+      <c r="AB28" s="122"/>
+      <c r="AC28" s="123"/>
+      <c r="AD28" s="124"/>
+      <c r="AE28" s="215"/>
+      <c r="AF28" s="215"/>
+      <c r="AG28" s="215"/>
+      <c r="AH28" s="121"/>
+      <c r="AI28" s="116"/>
+      <c r="AJ28" s="215"/>
+      <c r="AK28" s="215"/>
+      <c r="AL28" s="215"/>
+      <c r="AM28" s="215"/>
+      <c r="AN28" s="215"/>
+    </row>
+    <row r="29" spans="1:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="85">
         <v>30</v>
       </c>
-      <c r="B28" s="98" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" s="36"/>
-      <c r="D28" s="72" t="str">
-        <f>IF(SUM(K28:AD28)=0," ",SUM(K28:AD28))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E28" s="35">
-        <v>1</v>
-      </c>
-      <c r="F28" s="36"/>
-      <c r="G28" s="73"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="39"/>
-      <c r="J28" s="106"/>
-      <c r="K28" s="73"/>
-      <c r="L28" s="41"/>
-      <c r="M28" s="41"/>
-      <c r="N28" s="41"/>
-      <c r="O28" s="74"/>
-      <c r="P28" s="45"/>
-      <c r="Q28" s="43"/>
-      <c r="R28" s="41"/>
-      <c r="S28" s="43"/>
-      <c r="T28" s="44"/>
-      <c r="U28" s="72"/>
-      <c r="V28" s="41"/>
-      <c r="W28" s="41"/>
-      <c r="X28" s="41"/>
-      <c r="Y28" s="36"/>
-      <c r="Z28" s="45"/>
-      <c r="AA28" s="43"/>
-      <c r="AB28" s="43"/>
-      <c r="AC28" s="43"/>
-      <c r="AD28" s="99"/>
-    </row>
-    <row r="29" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="86">
-        <v>31</v>
-      </c>
-      <c r="B29" s="98" t="s">
-        <v>16</v>
-      </c>
-      <c r="C29" s="36"/>
-      <c r="D29" s="72" t="str">
+      <c r="B29" s="97" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="35"/>
+      <c r="D29" s="71" t="str">
         <f>IF(SUM(K29:AD29)=0," ",SUM(K29:AD29))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E29" s="35">
+      <c r="E29" s="34">
         <v>1</v>
       </c>
-      <c r="F29" s="36"/>
-      <c r="G29" s="73"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="106"/>
-      <c r="K29" s="73"/>
-      <c r="L29" s="41"/>
-      <c r="M29" s="41"/>
-      <c r="N29" s="41"/>
-      <c r="O29" s="74"/>
-      <c r="P29" s="45"/>
-      <c r="Q29" s="43"/>
-      <c r="R29" s="41"/>
-      <c r="S29" s="43"/>
-      <c r="T29" s="44"/>
-      <c r="U29" s="72"/>
-      <c r="V29" s="41"/>
-      <c r="W29" s="41"/>
-      <c r="X29" s="41"/>
-      <c r="Y29" s="36"/>
-      <c r="Z29" s="45"/>
-      <c r="AA29" s="51"/>
-      <c r="AB29" s="51"/>
-      <c r="AC29" s="51"/>
-      <c r="AD29" s="100"/>
-    </row>
-    <row r="30" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="86">
-        <v>32</v>
-      </c>
-      <c r="B30" s="101" t="s">
-        <v>14</v>
-      </c>
-      <c r="C30" s="68"/>
-      <c r="D30" s="72" t="str">
+      <c r="F29" s="35"/>
+      <c r="G29" s="72"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="105"/>
+      <c r="K29" s="72"/>
+      <c r="L29" s="40"/>
+      <c r="M29" s="40"/>
+      <c r="N29" s="40"/>
+      <c r="O29" s="73"/>
+      <c r="P29" s="44"/>
+      <c r="Q29" s="42"/>
+      <c r="R29" s="40"/>
+      <c r="S29" s="42"/>
+      <c r="T29" s="43"/>
+      <c r="U29" s="71"/>
+      <c r="V29" s="40"/>
+      <c r="W29" s="40"/>
+      <c r="X29" s="40"/>
+      <c r="Y29" s="35"/>
+      <c r="Z29" s="44"/>
+      <c r="AA29" s="42"/>
+      <c r="AB29" s="42"/>
+      <c r="AC29" s="42"/>
+      <c r="AD29" s="98"/>
+      <c r="AE29" s="72"/>
+      <c r="AF29" s="72"/>
+      <c r="AG29" s="72"/>
+      <c r="AH29" s="72"/>
+      <c r="AI29" s="202"/>
+      <c r="AJ29" s="218"/>
+      <c r="AK29" s="218"/>
+      <c r="AL29" s="218"/>
+      <c r="AM29" s="218"/>
+      <c r="AN29" s="218"/>
+    </row>
+    <row r="30" spans="1:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="85">
+        <v>31</v>
+      </c>
+      <c r="B30" s="97" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="35"/>
+      <c r="D30" s="71" t="str">
         <f>IF(SUM(K30:AD30)=0," ",SUM(K30:AD30))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E30" s="76">
+      <c r="E30" s="34">
         <v>1</v>
       </c>
-      <c r="F30" s="48"/>
-      <c r="G30" s="56"/>
-      <c r="H30" s="53"/>
-      <c r="I30" s="39"/>
-      <c r="J30" s="106"/>
-      <c r="K30" s="56"/>
-      <c r="L30" s="49"/>
-      <c r="M30" s="49"/>
-      <c r="N30" s="49"/>
-      <c r="O30" s="109"/>
-      <c r="P30" s="77"/>
-      <c r="Q30" s="78"/>
-      <c r="R30" s="49"/>
-      <c r="S30" s="78"/>
-      <c r="T30" s="55"/>
-      <c r="U30" s="79"/>
-      <c r="V30" s="61"/>
-      <c r="W30" s="61"/>
-      <c r="X30" s="61"/>
-      <c r="Y30" s="80"/>
-      <c r="Z30" s="77"/>
-      <c r="AA30" s="43"/>
-      <c r="AB30" s="43"/>
-      <c r="AC30" s="43"/>
-      <c r="AD30" s="93"/>
-    </row>
-    <row r="31" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F30" s="35"/>
+      <c r="G30" s="72"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="105"/>
+      <c r="K30" s="72"/>
+      <c r="L30" s="40"/>
+      <c r="M30" s="40"/>
+      <c r="N30" s="40"/>
+      <c r="O30" s="73"/>
+      <c r="P30" s="44"/>
+      <c r="Q30" s="42"/>
+      <c r="R30" s="40"/>
+      <c r="S30" s="42"/>
+      <c r="T30" s="43"/>
+      <c r="U30" s="71"/>
+      <c r="V30" s="40"/>
+      <c r="W30" s="40"/>
+      <c r="X30" s="40"/>
+      <c r="Y30" s="35"/>
+      <c r="Z30" s="44"/>
+      <c r="AA30" s="50"/>
+      <c r="AB30" s="50"/>
+      <c r="AC30" s="50"/>
+      <c r="AD30" s="99"/>
+      <c r="AE30" s="72"/>
+      <c r="AF30" s="72"/>
+      <c r="AG30" s="72"/>
+      <c r="AH30" s="72"/>
+      <c r="AI30" s="202"/>
+      <c r="AJ30" s="218"/>
+      <c r="AK30" s="218"/>
+      <c r="AL30" s="218"/>
+      <c r="AM30" s="218"/>
+      <c r="AN30" s="218"/>
+    </row>
+    <row r="31" spans="1:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="85">
-        <v>33</v>
-      </c>
-      <c r="B31" s="101" t="s">
-        <v>27</v>
-      </c>
-      <c r="C31" s="58"/>
-      <c r="D31" s="67" t="str">
+        <v>32</v>
+      </c>
+      <c r="B31" s="100" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="67"/>
+      <c r="D31" s="71" t="str">
         <f>IF(SUM(K31:AD31)=0," ",SUM(K31:AD31))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E31" s="57">
+      <c r="E31" s="75">
+        <v>1</v>
+      </c>
+      <c r="F31" s="47"/>
+      <c r="G31" s="55"/>
+      <c r="H31" s="52"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="105"/>
+      <c r="K31" s="55"/>
+      <c r="L31" s="48"/>
+      <c r="M31" s="48"/>
+      <c r="N31" s="48"/>
+      <c r="O31" s="108"/>
+      <c r="P31" s="76"/>
+      <c r="Q31" s="77"/>
+      <c r="R31" s="48"/>
+      <c r="S31" s="77"/>
+      <c r="T31" s="54"/>
+      <c r="U31" s="78"/>
+      <c r="V31" s="60"/>
+      <c r="W31" s="60"/>
+      <c r="X31" s="60"/>
+      <c r="Y31" s="79"/>
+      <c r="Z31" s="76"/>
+      <c r="AA31" s="42"/>
+      <c r="AB31" s="42"/>
+      <c r="AC31" s="42"/>
+      <c r="AD31" s="92"/>
+      <c r="AE31" s="79"/>
+      <c r="AF31" s="79"/>
+      <c r="AG31" s="79"/>
+      <c r="AH31" s="79"/>
+      <c r="AI31" s="209"/>
+      <c r="AJ31" s="176"/>
+      <c r="AK31" s="176"/>
+      <c r="AL31" s="176"/>
+      <c r="AM31" s="176"/>
+      <c r="AN31" s="176"/>
+    </row>
+    <row r="32" spans="1:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="84">
+        <v>33</v>
+      </c>
+      <c r="B32" s="100" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" s="57"/>
+      <c r="D32" s="66" t="str">
+        <f>IF(SUM(K32:AD32)=0," ",SUM(K32:AD32))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E32" s="56">
         <v>2</v>
       </c>
-      <c r="F31" s="68"/>
-      <c r="G31" s="80"/>
-      <c r="H31" s="69"/>
-      <c r="I31" s="39"/>
-      <c r="J31" s="107"/>
-      <c r="K31" s="65"/>
-      <c r="L31" s="60"/>
-      <c r="M31" s="60"/>
-      <c r="N31" s="60"/>
-      <c r="O31" s="70"/>
-      <c r="P31" s="66"/>
-      <c r="Q31" s="63"/>
-      <c r="R31" s="61"/>
-      <c r="S31" s="63"/>
-      <c r="T31" s="64"/>
-      <c r="U31" s="67"/>
-      <c r="V31" s="60"/>
-      <c r="W31" s="71"/>
-      <c r="X31" s="60"/>
-      <c r="Y31" s="65"/>
-      <c r="Z31" s="66"/>
-      <c r="AA31" s="63"/>
-      <c r="AB31" s="63"/>
-      <c r="AC31" s="63"/>
-      <c r="AD31" s="102"/>
-    </row>
-    <row r="32" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="112">
+      <c r="F32" s="67"/>
+      <c r="G32" s="79"/>
+      <c r="H32" s="68"/>
+      <c r="I32" s="38"/>
+      <c r="J32" s="106"/>
+      <c r="K32" s="64"/>
+      <c r="L32" s="59"/>
+      <c r="M32" s="59"/>
+      <c r="N32" s="59"/>
+      <c r="O32" s="69"/>
+      <c r="P32" s="65"/>
+      <c r="Q32" s="62"/>
+      <c r="R32" s="60"/>
+      <c r="S32" s="62"/>
+      <c r="T32" s="63"/>
+      <c r="U32" s="66"/>
+      <c r="V32" s="59"/>
+      <c r="W32" s="70"/>
+      <c r="X32" s="59"/>
+      <c r="Y32" s="64"/>
+      <c r="Z32" s="65"/>
+      <c r="AA32" s="62"/>
+      <c r="AB32" s="62"/>
+      <c r="AC32" s="62"/>
+      <c r="AD32" s="101"/>
+      <c r="AE32" s="64"/>
+      <c r="AF32" s="64"/>
+      <c r="AG32" s="64"/>
+      <c r="AH32" s="64"/>
+      <c r="AI32" s="205"/>
+      <c r="AJ32" s="220"/>
+      <c r="AK32" s="220"/>
+      <c r="AL32" s="220"/>
+      <c r="AM32" s="220"/>
+      <c r="AN32" s="220"/>
+    </row>
+    <row r="33" spans="1:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="111">
         <v>50</v>
       </c>
-      <c r="B32" s="113" t="s">
-        <v>13</v>
-      </c>
-      <c r="C32" s="115">
-        <f>SUM(C33)</f>
+      <c r="B33" s="112" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="114">
+        <f>SUM(C34)</f>
         <v>16.2</v>
       </c>
-      <c r="D32" s="116">
-        <f>SUM(D33)</f>
-        <v>0</v>
-      </c>
-      <c r="E32" s="117"/>
-      <c r="F32" s="118"/>
-      <c r="G32" s="122"/>
-      <c r="H32" s="119"/>
-      <c r="I32" s="120"/>
-      <c r="J32" s="121"/>
-      <c r="K32" s="118"/>
-      <c r="L32" s="122"/>
-      <c r="M32" s="123"/>
-      <c r="N32" s="124"/>
-      <c r="O32" s="117"/>
-      <c r="P32" s="114"/>
-      <c r="Q32" s="123"/>
-      <c r="R32" s="124"/>
-      <c r="S32" s="122"/>
-      <c r="T32" s="119"/>
-      <c r="U32" s="114"/>
-      <c r="V32" s="123"/>
-      <c r="W32" s="123"/>
-      <c r="X32" s="123"/>
-      <c r="Y32" s="119"/>
-      <c r="Z32" s="114"/>
-      <c r="AA32" s="123"/>
-      <c r="AB32" s="123"/>
-      <c r="AC32" s="124"/>
-      <c r="AD32" s="125"/>
-    </row>
-    <row r="33" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="87">
+      <c r="D33" s="115">
+        <f>SUM(D34)</f>
+        <v>0</v>
+      </c>
+      <c r="E33" s="116"/>
+      <c r="F33" s="117"/>
+      <c r="G33" s="121"/>
+      <c r="H33" s="118"/>
+      <c r="I33" s="119"/>
+      <c r="J33" s="120"/>
+      <c r="K33" s="117"/>
+      <c r="L33" s="121"/>
+      <c r="M33" s="122"/>
+      <c r="N33" s="123"/>
+      <c r="O33" s="116"/>
+      <c r="P33" s="113"/>
+      <c r="Q33" s="122"/>
+      <c r="R33" s="123"/>
+      <c r="S33" s="121"/>
+      <c r="T33" s="118"/>
+      <c r="U33" s="113"/>
+      <c r="V33" s="122"/>
+      <c r="W33" s="122"/>
+      <c r="X33" s="122"/>
+      <c r="Y33" s="118"/>
+      <c r="Z33" s="113"/>
+      <c r="AA33" s="122"/>
+      <c r="AB33" s="122"/>
+      <c r="AC33" s="123"/>
+      <c r="AD33" s="124"/>
+      <c r="AE33" s="121"/>
+      <c r="AF33" s="121"/>
+      <c r="AG33" s="121"/>
+      <c r="AH33" s="121"/>
+      <c r="AI33" s="116"/>
+      <c r="AJ33" s="121"/>
+      <c r="AK33" s="121"/>
+      <c r="AL33" s="121"/>
+      <c r="AM33" s="121"/>
+      <c r="AN33" s="121"/>
+    </row>
+    <row r="34" spans="1:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="86">
         <v>51</v>
       </c>
-      <c r="B33" s="101" t="s">
-        <v>6</v>
-      </c>
-      <c r="C33" s="68">
-        <f>(C5+C11+C15+C27)*0.2</f>
+      <c r="B34" s="100" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="67">
+        <f>(C5+C11+C15+C28)*0.2</f>
         <v>16.2</v>
       </c>
-      <c r="D33" s="79" t="str">
-        <f>IF(SUM(K33:AD33)=0," ",SUM(K33:AD33))</f>
+      <c r="D34" s="78" t="str">
+        <f>IF(SUM(K34:AD34)=0," ",SUM(K34:AD34))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E33" s="76">
+      <c r="E34" s="75">
         <v>3</v>
       </c>
-      <c r="F33" s="68"/>
-      <c r="G33" s="80"/>
-      <c r="H33" s="69"/>
-      <c r="I33" s="39"/>
-      <c r="J33" s="105"/>
-      <c r="K33" s="80"/>
-      <c r="L33" s="61"/>
-      <c r="M33" s="61"/>
-      <c r="N33" s="61"/>
-      <c r="O33" s="109"/>
-      <c r="P33" s="77"/>
-      <c r="Q33" s="78"/>
-      <c r="R33" s="61"/>
-      <c r="S33" s="78"/>
-      <c r="T33" s="55"/>
-      <c r="U33" s="79"/>
-      <c r="V33" s="61"/>
-      <c r="W33" s="61"/>
-      <c r="X33" s="61"/>
-      <c r="Y33" s="69"/>
-      <c r="Z33" s="81"/>
-      <c r="AA33" s="78"/>
-      <c r="AB33" s="78"/>
-      <c r="AC33" s="78"/>
-      <c r="AD33" s="93"/>
-    </row>
-    <row r="34" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="87">
+      <c r="F34" s="67"/>
+      <c r="G34" s="79"/>
+      <c r="H34" s="68"/>
+      <c r="I34" s="38"/>
+      <c r="J34" s="104"/>
+      <c r="K34" s="79"/>
+      <c r="L34" s="60"/>
+      <c r="M34" s="60"/>
+      <c r="N34" s="60"/>
+      <c r="O34" s="108"/>
+      <c r="P34" s="76"/>
+      <c r="Q34" s="77"/>
+      <c r="R34" s="60"/>
+      <c r="S34" s="77"/>
+      <c r="T34" s="54"/>
+      <c r="U34" s="78"/>
+      <c r="V34" s="60"/>
+      <c r="W34" s="60"/>
+      <c r="X34" s="60"/>
+      <c r="Y34" s="68"/>
+      <c r="Z34" s="80"/>
+      <c r="AA34" s="77"/>
+      <c r="AB34" s="77"/>
+      <c r="AC34" s="77"/>
+      <c r="AD34" s="92"/>
+      <c r="AE34" s="79"/>
+      <c r="AF34" s="79"/>
+      <c r="AG34" s="79"/>
+      <c r="AH34" s="79"/>
+      <c r="AI34" s="209"/>
+      <c r="AJ34" s="176"/>
+      <c r="AK34" s="176"/>
+      <c r="AL34" s="176"/>
+      <c r="AM34" s="176"/>
+      <c r="AN34" s="176"/>
+    </row>
+    <row r="35" spans="1:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="86">
         <v>52</v>
       </c>
-      <c r="B34" s="174" t="s">
+      <c r="B35" s="173" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35" s="79">
+        <v>1.5</v>
+      </c>
+      <c r="D35" s="78">
+        <v>0.75</v>
+      </c>
+      <c r="E35" s="75"/>
+      <c r="F35" s="67"/>
+      <c r="G35" s="79"/>
+      <c r="H35" s="68"/>
+      <c r="I35" s="174"/>
+      <c r="J35" s="175"/>
+      <c r="K35" s="79"/>
+      <c r="L35" s="176"/>
+      <c r="M35" s="177"/>
+      <c r="N35" s="60"/>
+      <c r="O35" s="54"/>
+      <c r="P35" s="76"/>
+      <c r="Q35" s="78"/>
+      <c r="R35" s="60"/>
+      <c r="S35" s="79"/>
+      <c r="T35" s="54"/>
+      <c r="U35" s="79"/>
+      <c r="V35" s="177"/>
+      <c r="W35" s="177"/>
+      <c r="X35" s="40"/>
+      <c r="Y35" s="168"/>
+      <c r="Z35" s="76"/>
+      <c r="AA35" s="78"/>
+      <c r="AB35" s="78"/>
+      <c r="AC35" s="42"/>
+      <c r="AD35" s="168"/>
+      <c r="AE35" s="79"/>
+      <c r="AF35" s="79"/>
+      <c r="AG35" s="79"/>
+      <c r="AH35" s="79"/>
+      <c r="AI35" s="208"/>
+      <c r="AJ35" s="176"/>
+      <c r="AK35" s="176"/>
+      <c r="AL35" s="176"/>
+      <c r="AM35" s="176"/>
+      <c r="AN35" s="178"/>
+    </row>
+    <row r="36" spans="1:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="86"/>
+      <c r="B36" s="173" t="s">
         <v>49</v>
       </c>
-      <c r="C34" s="80">
+      <c r="C36" s="79">
         <v>0.5</v>
       </c>
-      <c r="D34" s="79">
+      <c r="D36" s="78">
         <v>0.25</v>
       </c>
-      <c r="E34" s="76"/>
-      <c r="F34" s="68"/>
-      <c r="G34" s="80"/>
-      <c r="H34" s="69"/>
-      <c r="I34" s="175"/>
-      <c r="J34" s="176"/>
-      <c r="K34" s="80"/>
-      <c r="L34" s="177"/>
-      <c r="M34" s="178"/>
-      <c r="N34" s="61"/>
-      <c r="O34" s="55"/>
-      <c r="P34" s="77"/>
-      <c r="Q34" s="79"/>
-      <c r="R34" s="61"/>
-      <c r="S34" s="80"/>
-      <c r="T34" s="55"/>
-      <c r="U34" s="80"/>
-      <c r="V34" s="178"/>
-      <c r="W34" s="178"/>
-      <c r="X34" s="41"/>
-      <c r="Y34" s="169"/>
-      <c r="Z34" s="77"/>
-      <c r="AA34" s="79"/>
-      <c r="AB34" s="79"/>
-      <c r="AC34" s="43"/>
-      <c r="AD34" s="169"/>
-    </row>
-    <row r="35" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="87"/>
-      <c r="B35" s="174" t="s">
-        <v>50</v>
-      </c>
-      <c r="C35" s="80">
-        <v>0.5</v>
-      </c>
-      <c r="D35" s="79">
-        <v>0.25</v>
-      </c>
-      <c r="E35" s="76"/>
-      <c r="F35" s="68"/>
-      <c r="G35" s="80"/>
-      <c r="H35" s="69"/>
-      <c r="I35" s="175"/>
-      <c r="J35" s="176"/>
-      <c r="K35" s="80"/>
-      <c r="L35" s="177"/>
-      <c r="M35" s="178"/>
-      <c r="N35" s="61"/>
-      <c r="O35" s="55"/>
-      <c r="P35" s="77"/>
-      <c r="Q35" s="79"/>
-      <c r="R35" s="61"/>
-      <c r="S35" s="80"/>
-      <c r="T35" s="55"/>
-      <c r="U35" s="80"/>
-      <c r="V35" s="178"/>
-      <c r="W35" s="178"/>
-      <c r="X35" s="41"/>
-      <c r="Y35" s="179"/>
-      <c r="Z35" s="77"/>
-      <c r="AA35" s="79"/>
-      <c r="AB35" s="79"/>
-      <c r="AC35" s="78"/>
-      <c r="AD35" s="169"/>
-    </row>
-    <row r="36" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="112">
+      <c r="E36" s="75"/>
+      <c r="F36" s="67"/>
+      <c r="G36" s="79"/>
+      <c r="H36" s="68"/>
+      <c r="I36" s="174"/>
+      <c r="J36" s="175"/>
+      <c r="K36" s="79"/>
+      <c r="L36" s="176"/>
+      <c r="M36" s="177"/>
+      <c r="N36" s="60"/>
+      <c r="O36" s="54"/>
+      <c r="P36" s="76"/>
+      <c r="Q36" s="78"/>
+      <c r="R36" s="60"/>
+      <c r="S36" s="79"/>
+      <c r="T36" s="54"/>
+      <c r="U36" s="79"/>
+      <c r="V36" s="177"/>
+      <c r="W36" s="177"/>
+      <c r="X36" s="40"/>
+      <c r="Y36" s="178"/>
+      <c r="Z36" s="76"/>
+      <c r="AA36" s="78"/>
+      <c r="AB36" s="78"/>
+      <c r="AC36" s="77"/>
+      <c r="AD36" s="168"/>
+      <c r="AE36" s="64"/>
+      <c r="AF36" s="64"/>
+      <c r="AG36" s="64"/>
+      <c r="AH36" s="64"/>
+      <c r="AI36" s="208"/>
+      <c r="AJ36" s="176"/>
+      <c r="AK36" s="176"/>
+      <c r="AL36" s="176"/>
+      <c r="AM36" s="176"/>
+      <c r="AN36" s="178"/>
+    </row>
+    <row r="37" spans="1:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="111">
         <v>60</v>
       </c>
-      <c r="B36" s="113" t="s">
-        <v>10</v>
-      </c>
-      <c r="C36" s="115">
-        <f>SUM(C37:C38)</f>
-        <v>0</v>
-      </c>
-      <c r="D36" s="116">
-        <f>SUM(D37:D38)</f>
-        <v>0</v>
-      </c>
-      <c r="E36" s="117"/>
-      <c r="F36" s="118"/>
-      <c r="G36" s="122"/>
-      <c r="H36" s="119"/>
-      <c r="I36" s="120"/>
-      <c r="J36" s="121"/>
-      <c r="K36" s="118"/>
-      <c r="L36" s="122"/>
-      <c r="M36" s="123"/>
-      <c r="N36" s="124"/>
-      <c r="O36" s="117"/>
-      <c r="P36" s="114"/>
-      <c r="Q36" s="123"/>
-      <c r="R36" s="124"/>
-      <c r="S36" s="122"/>
-      <c r="T36" s="119"/>
-      <c r="U36" s="114"/>
-      <c r="V36" s="123"/>
-      <c r="W36" s="123"/>
-      <c r="X36" s="123"/>
-      <c r="Y36" s="119"/>
-      <c r="Z36" s="114"/>
-      <c r="AA36" s="123"/>
-      <c r="AB36" s="123"/>
-      <c r="AC36" s="124"/>
-      <c r="AD36" s="125"/>
-    </row>
-    <row r="37" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="86">
+      <c r="B37" s="112" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" s="114">
+        <f>SUM(C38:C39)</f>
+        <v>0</v>
+      </c>
+      <c r="D37" s="115">
+        <f>SUM(D38:D39)</f>
+        <v>0</v>
+      </c>
+      <c r="E37" s="116"/>
+      <c r="F37" s="117"/>
+      <c r="G37" s="121"/>
+      <c r="H37" s="118"/>
+      <c r="I37" s="119"/>
+      <c r="J37" s="120"/>
+      <c r="K37" s="117"/>
+      <c r="L37" s="121"/>
+      <c r="M37" s="122"/>
+      <c r="N37" s="123"/>
+      <c r="O37" s="116"/>
+      <c r="P37" s="113"/>
+      <c r="Q37" s="122"/>
+      <c r="R37" s="123"/>
+      <c r="S37" s="121"/>
+      <c r="T37" s="118"/>
+      <c r="U37" s="113"/>
+      <c r="V37" s="122"/>
+      <c r="W37" s="122"/>
+      <c r="X37" s="122"/>
+      <c r="Y37" s="118"/>
+      <c r="Z37" s="113"/>
+      <c r="AA37" s="122"/>
+      <c r="AB37" s="122"/>
+      <c r="AC37" s="123"/>
+      <c r="AD37" s="124"/>
+      <c r="AE37" s="121"/>
+      <c r="AF37" s="121"/>
+      <c r="AG37" s="121"/>
+      <c r="AH37" s="121"/>
+      <c r="AI37" s="116"/>
+      <c r="AJ37" s="121"/>
+      <c r="AK37" s="121"/>
+      <c r="AL37" s="121"/>
+      <c r="AM37" s="121"/>
+      <c r="AN37" s="121"/>
+    </row>
+    <row r="38" spans="1:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="85">
         <v>61</v>
       </c>
-      <c r="B37" s="97" t="s">
-        <v>35</v>
-      </c>
-      <c r="C37" s="36"/>
-      <c r="D37" s="72" t="str">
-        <f>IF(SUM(K37:AD37)=0," ",SUM(K37:AD37))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E37" s="35">
-        <v>2</v>
-      </c>
-      <c r="F37" s="36"/>
-      <c r="G37" s="73"/>
-      <c r="H37" s="38"/>
-      <c r="I37" s="39"/>
-      <c r="J37" s="110"/>
-      <c r="K37" s="73"/>
-      <c r="L37" s="41"/>
-      <c r="M37" s="41"/>
-      <c r="N37" s="41"/>
-      <c r="O37" s="74"/>
-      <c r="P37" s="45"/>
-      <c r="Q37" s="43"/>
-      <c r="R37" s="41"/>
-      <c r="S37" s="43"/>
-      <c r="T37" s="44"/>
-      <c r="U37" s="72"/>
-      <c r="V37" s="41"/>
-      <c r="W37" s="41"/>
-      <c r="X37" s="41"/>
-      <c r="Y37" s="73"/>
-      <c r="Z37" s="42"/>
-      <c r="AA37" s="43"/>
-      <c r="AB37" s="43"/>
-      <c r="AC37" s="43"/>
-      <c r="AD37" s="100"/>
-    </row>
-    <row r="38" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="85">
-        <v>62</v>
-      </c>
-      <c r="B38" s="98" t="s">
-        <v>36</v>
-      </c>
-      <c r="C38" s="47"/>
-      <c r="D38" s="37" t="str">
+      <c r="B38" s="96" t="s">
+        <v>34</v>
+      </c>
+      <c r="C38" s="35"/>
+      <c r="D38" s="71" t="str">
         <f>IF(SUM(K38:AD38)=0," ",SUM(K38:AD38))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E38" s="46">
-        <v>1</v>
-      </c>
-      <c r="F38" s="82"/>
-      <c r="G38" s="139"/>
-      <c r="H38" s="83"/>
-      <c r="I38" s="39"/>
-      <c r="J38" s="108"/>
-      <c r="K38" s="56"/>
-      <c r="L38" s="49"/>
-      <c r="M38" s="49"/>
-      <c r="N38" s="49"/>
-      <c r="O38" s="74"/>
-      <c r="P38" s="75"/>
-      <c r="Q38" s="51"/>
-      <c r="R38" s="41"/>
-      <c r="S38" s="51"/>
-      <c r="T38" s="52"/>
-      <c r="U38" s="37"/>
-      <c r="V38" s="49"/>
-      <c r="W38" s="41"/>
-      <c r="X38" s="49"/>
-      <c r="Y38" s="56"/>
-      <c r="Z38" s="50"/>
-      <c r="AA38" s="51"/>
-      <c r="AB38" s="51"/>
-      <c r="AC38" s="51"/>
-      <c r="AD38" s="100"/>
-    </row>
-    <row r="39" spans="1:30" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="111"/>
-      <c r="B39" s="130" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" s="131">
-        <f>SUM(C5+C11+C15+C27+C36)</f>
-        <v>81</v>
-      </c>
-      <c r="D39" s="131" t="str">
+      <c r="E38" s="34">
+        <v>2</v>
+      </c>
+      <c r="F38" s="35"/>
+      <c r="G38" s="72"/>
+      <c r="H38" s="37"/>
+      <c r="I38" s="38"/>
+      <c r="J38" s="109"/>
+      <c r="K38" s="72"/>
+      <c r="L38" s="40"/>
+      <c r="M38" s="40"/>
+      <c r="N38" s="40"/>
+      <c r="O38" s="73"/>
+      <c r="P38" s="44"/>
+      <c r="Q38" s="42"/>
+      <c r="R38" s="40"/>
+      <c r="S38" s="42"/>
+      <c r="T38" s="43"/>
+      <c r="U38" s="71"/>
+      <c r="V38" s="40"/>
+      <c r="W38" s="40"/>
+      <c r="X38" s="40"/>
+      <c r="Y38" s="72"/>
+      <c r="Z38" s="41"/>
+      <c r="AA38" s="42"/>
+      <c r="AB38" s="42"/>
+      <c r="AC38" s="42"/>
+      <c r="AD38" s="99"/>
+      <c r="AE38" s="72"/>
+      <c r="AF38" s="72"/>
+      <c r="AG38" s="72"/>
+      <c r="AH38" s="72"/>
+      <c r="AI38" s="202"/>
+      <c r="AJ38" s="218"/>
+      <c r="AK38" s="218"/>
+      <c r="AL38" s="218"/>
+      <c r="AM38" s="218"/>
+      <c r="AN38" s="218"/>
+    </row>
+    <row r="39" spans="1:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="84">
+        <v>62</v>
+      </c>
+      <c r="B39" s="97" t="s">
+        <v>35</v>
+      </c>
+      <c r="C39" s="46"/>
+      <c r="D39" s="36" t="str">
         <f>IF(SUM(K39:AD39)=0," ",SUM(K39:AD39))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E39" s="131"/>
-      <c r="F39" s="131"/>
-      <c r="G39" s="131"/>
-      <c r="H39" s="131"/>
-      <c r="I39" s="132"/>
-      <c r="J39" s="133"/>
-      <c r="K39" s="134">
-        <f t="shared" ref="K39:AD39" si="3">SUM(K5:K38)</f>
-        <v>0</v>
-      </c>
-      <c r="L39" s="131">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M39" s="135">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="N39" s="135">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O39" s="135">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P39" s="135">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Q39" s="131">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="R39" s="135">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="S39" s="131">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="T39" s="135">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U39" s="135">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="V39" s="131">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="W39" s="135">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="X39" s="131">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Y39" s="135">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Z39" s="135">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AA39" s="131">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AB39" s="135">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AC39" s="131">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AD39" s="136">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="137"/>
-      <c r="B40" s="190"/>
-      <c r="C40" s="190"/>
-      <c r="D40" s="190"/>
-      <c r="E40" s="190"/>
-      <c r="F40" s="190"/>
-      <c r="G40" s="190"/>
-      <c r="H40" s="190"/>
-      <c r="I40" s="190"/>
-      <c r="J40" s="190"/>
-    </row>
-    <row r="41" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="138"/>
-      <c r="B41" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C41" s="15"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15"/>
-      <c r="G41" s="15"/>
-      <c r="H41" s="15"/>
-      <c r="I41" s="15"/>
-      <c r="J41" s="15"/>
-      <c r="K41" s="188"/>
-      <c r="L41" s="189"/>
-      <c r="M41" s="189"/>
-      <c r="N41" s="189"/>
-      <c r="O41" s="189"/>
-      <c r="P41" s="189"/>
-      <c r="Q41" s="189"/>
-      <c r="R41" s="189"/>
-      <c r="S41" s="189"/>
-      <c r="T41" s="189"/>
-      <c r="U41" s="189"/>
-      <c r="V41" s="189"/>
-      <c r="W41" s="189"/>
-      <c r="X41" s="189"/>
-      <c r="Y41" s="189"/>
-      <c r="Z41" s="189"/>
-      <c r="AA41" s="189"/>
-      <c r="AB41" s="189"/>
-      <c r="AC41" s="189"/>
-      <c r="AD41" s="189"/>
-    </row>
-    <row r="42" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="173"/>
-      <c r="B42" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="C42" s="18"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
-      <c r="H42" s="18"/>
-      <c r="I42" s="18"/>
-      <c r="J42" s="18"/>
+      <c r="E39" s="45">
+        <v>1</v>
+      </c>
+      <c r="F39" s="81"/>
+      <c r="G39" s="138"/>
+      <c r="H39" s="82"/>
+      <c r="I39" s="38"/>
+      <c r="J39" s="107"/>
+      <c r="K39" s="55"/>
+      <c r="L39" s="48"/>
+      <c r="M39" s="48"/>
+      <c r="N39" s="48"/>
+      <c r="O39" s="73"/>
+      <c r="P39" s="74"/>
+      <c r="Q39" s="50"/>
+      <c r="R39" s="40"/>
+      <c r="S39" s="50"/>
+      <c r="T39" s="51"/>
+      <c r="U39" s="36"/>
+      <c r="V39" s="48"/>
+      <c r="W39" s="40"/>
+      <c r="X39" s="48"/>
+      <c r="Y39" s="55"/>
+      <c r="Z39" s="49"/>
+      <c r="AA39" s="50"/>
+      <c r="AB39" s="50"/>
+      <c r="AC39" s="50"/>
+      <c r="AD39" s="99"/>
+      <c r="AE39" s="55"/>
+      <c r="AF39" s="55"/>
+      <c r="AG39" s="55"/>
+      <c r="AH39" s="55"/>
+      <c r="AI39" s="203"/>
+      <c r="AJ39" s="218"/>
+      <c r="AK39" s="218"/>
+      <c r="AL39" s="218"/>
+      <c r="AM39" s="218"/>
+      <c r="AN39" s="218"/>
+    </row>
+    <row r="40" spans="1:40" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="110"/>
+      <c r="B40" s="129" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" s="130">
+        <f>SUM(C5+C11+C15+C28+C37)</f>
+        <v>81</v>
+      </c>
+      <c r="D40" s="130" t="str">
+        <f>IF(SUM(K40:AD40)=0," ",SUM(K40:AD40))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E40" s="130"/>
+      <c r="F40" s="130"/>
+      <c r="G40" s="130"/>
+      <c r="H40" s="130"/>
+      <c r="I40" s="131"/>
+      <c r="J40" s="132"/>
+      <c r="K40" s="133">
+        <f t="shared" ref="K40:Y40" si="1">SUM(K5:K39)</f>
+        <v>0</v>
+      </c>
+      <c r="L40" s="130">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M40" s="134">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N40" s="134">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O40" s="134">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P40" s="134">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q40" s="130">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R40" s="134">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S40" s="130">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T40" s="134">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U40" s="134">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V40" s="130">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W40" s="134">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X40" s="130">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Y40" s="134">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Z40" s="134">
+        <f>SUM(Z5:Z39)</f>
+        <v>0</v>
+      </c>
+      <c r="AA40" s="130">
+        <f>SUM(AA5:AA39)</f>
+        <v>0</v>
+      </c>
+      <c r="AB40" s="134">
+        <f>SUM(AB5:AB39)</f>
+        <v>0</v>
+      </c>
+      <c r="AC40" s="130">
+        <f>SUM(AC5:AC39)</f>
+        <v>0</v>
+      </c>
+      <c r="AD40" s="135">
+        <f>SUM(AD5:AD39)</f>
+        <v>0</v>
+      </c>
+      <c r="AE40" s="134"/>
+      <c r="AF40" s="134"/>
+      <c r="AG40" s="134"/>
+      <c r="AH40" s="134"/>
+      <c r="AI40" s="134"/>
+      <c r="AJ40" s="221"/>
+      <c r="AK40" s="221"/>
+      <c r="AL40" s="221"/>
+      <c r="AM40" s="221"/>
+      <c r="AN40" s="221"/>
+    </row>
+    <row r="41" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="136"/>
+      <c r="B41" s="189"/>
+      <c r="C41" s="189"/>
+      <c r="D41" s="189"/>
+      <c r="E41" s="189"/>
+      <c r="F41" s="189"/>
+      <c r="G41" s="189"/>
+      <c r="H41" s="189"/>
+      <c r="I41" s="189"/>
+      <c r="J41" s="189"/>
+    </row>
+    <row r="42" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="137"/>
+      <c r="B42" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42" s="15"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15"/>
+      <c r="I42" s="15"/>
+      <c r="J42" s="15"/>
       <c r="K42" s="187"/>
-      <c r="L42" s="187"/>
-      <c r="M42" s="187"/>
-      <c r="N42" s="187"/>
-      <c r="O42" s="187"/>
-      <c r="P42" s="187"/>
-      <c r="Q42" s="187"/>
-      <c r="R42" s="187"/>
-      <c r="S42" s="187"/>
-      <c r="T42" s="187"/>
-      <c r="U42" s="187"/>
-      <c r="V42" s="187"/>
-      <c r="W42" s="187"/>
-      <c r="X42" s="187"/>
-      <c r="Y42" s="187"/>
-      <c r="Z42" s="187"/>
-      <c r="AA42" s="187"/>
-      <c r="AB42" s="187"/>
-      <c r="AC42" s="187"/>
-      <c r="AD42" s="187"/>
-    </row>
-    <row r="43" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="17"/>
-      <c r="B43" s="14"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="18"/>
-      <c r="I43" s="18"/>
-      <c r="J43" s="18"/>
-      <c r="K43" s="187"/>
-      <c r="L43" s="187"/>
-      <c r="M43" s="187"/>
-      <c r="N43" s="187"/>
-      <c r="O43" s="187"/>
-      <c r="P43" s="187"/>
-      <c r="Q43" s="187"/>
-      <c r="R43" s="187"/>
-      <c r="S43" s="187"/>
-      <c r="T43" s="187"/>
-      <c r="U43" s="187"/>
-      <c r="V43" s="187"/>
-      <c r="W43" s="187"/>
-      <c r="X43" s="187"/>
-      <c r="Y43" s="187"/>
-      <c r="Z43" s="187"/>
-      <c r="AA43" s="187"/>
-      <c r="AB43" s="187"/>
-      <c r="AC43" s="187"/>
-      <c r="AD43" s="187"/>
-    </row>
-    <row r="44" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="20"/>
-      <c r="B44" s="18"/>
-      <c r="J44" s="9"/>
-    </row>
-    <row r="45" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="20"/>
-      <c r="B45" s="18"/>
+      <c r="L42" s="188"/>
+      <c r="M42" s="188"/>
+      <c r="N42" s="188"/>
+      <c r="O42" s="188"/>
+      <c r="P42" s="188"/>
+      <c r="Q42" s="188"/>
+      <c r="R42" s="188"/>
+      <c r="S42" s="188"/>
+      <c r="T42" s="188"/>
+      <c r="U42" s="188"/>
+      <c r="V42" s="188"/>
+      <c r="W42" s="188"/>
+      <c r="X42" s="188"/>
+      <c r="Y42" s="188"/>
+      <c r="Z42" s="188"/>
+      <c r="AA42" s="188"/>
+      <c r="AB42" s="188"/>
+      <c r="AC42" s="188"/>
+      <c r="AD42" s="188"/>
+      <c r="AE42" s="188"/>
+      <c r="AF42" s="188"/>
+      <c r="AG42" s="188"/>
+      <c r="AH42" s="188"/>
+      <c r="AI42" s="188"/>
+      <c r="AJ42" s="188"/>
+      <c r="AK42" s="188"/>
+      <c r="AL42" s="188"/>
+      <c r="AM42" s="188"/>
+      <c r="AN42" s="188"/>
+    </row>
+    <row r="43" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="172"/>
+      <c r="B43" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C43" s="17"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="17"/>
+      <c r="H43" s="17"/>
+      <c r="I43" s="17"/>
+      <c r="J43" s="17"/>
+      <c r="K43" s="186"/>
+      <c r="L43" s="186"/>
+      <c r="M43" s="186"/>
+      <c r="N43" s="186"/>
+      <c r="O43" s="186"/>
+      <c r="P43" s="186"/>
+      <c r="Q43" s="186"/>
+      <c r="R43" s="186"/>
+      <c r="S43" s="186"/>
+      <c r="T43" s="186"/>
+      <c r="U43" s="186"/>
+      <c r="V43" s="186"/>
+      <c r="W43" s="186"/>
+      <c r="X43" s="186"/>
+      <c r="Y43" s="186"/>
+      <c r="Z43" s="186"/>
+      <c r="AA43" s="186"/>
+      <c r="AB43" s="186"/>
+      <c r="AC43" s="186"/>
+      <c r="AD43" s="186"/>
+      <c r="AE43" s="186"/>
+      <c r="AF43" s="186"/>
+      <c r="AG43" s="186"/>
+      <c r="AH43" s="186"/>
+      <c r="AI43" s="186"/>
+      <c r="AJ43" s="186"/>
+      <c r="AK43" s="186"/>
+      <c r="AL43" s="186"/>
+      <c r="AM43" s="186"/>
+      <c r="AN43" s="186"/>
+    </row>
+    <row r="44" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="210"/>
+      <c r="B44" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C44" s="17"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="17"/>
+      <c r="H44" s="17"/>
+      <c r="I44" s="17"/>
+      <c r="J44" s="17"/>
+      <c r="K44" s="186"/>
+      <c r="L44" s="186"/>
+      <c r="M44" s="186"/>
+      <c r="N44" s="186"/>
+      <c r="O44" s="186"/>
+      <c r="P44" s="186"/>
+      <c r="Q44" s="186"/>
+      <c r="R44" s="186"/>
+      <c r="S44" s="186"/>
+      <c r="T44" s="186"/>
+      <c r="U44" s="186"/>
+      <c r="V44" s="186"/>
+      <c r="W44" s="186"/>
+      <c r="X44" s="186"/>
+      <c r="Y44" s="186"/>
+      <c r="Z44" s="186"/>
+      <c r="AA44" s="186"/>
+      <c r="AB44" s="186"/>
+      <c r="AC44" s="186"/>
+      <c r="AD44" s="186"/>
+      <c r="AE44" s="186"/>
+      <c r="AF44" s="186"/>
+      <c r="AG44" s="186"/>
+      <c r="AH44" s="186"/>
+      <c r="AI44" s="186"/>
+      <c r="AJ44" s="186"/>
+      <c r="AK44" s="186"/>
+      <c r="AL44" s="186"/>
+      <c r="AM44" s="186"/>
+      <c r="AN44" s="186"/>
+    </row>
+    <row r="45" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="19"/>
+      <c r="B45" s="17"/>
       <c r="J45" s="9"/>
     </row>
-    <row r="46" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="19"/>
+      <c r="B46" s="17"/>
       <c r="J46" s="9"/>
     </row>
-    <row r="47" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="20"/>
+    <row r="47" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J47" s="9"/>
     </row>
-    <row r="48" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="19"/>
       <c r="J48" s="9"/>
     </row>
-    <row r="49" spans="10:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="10:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J49" s="9"/>
     </row>
-    <row r="60" spans="10:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AH60" s="9"/>
-      <c r="AI60" s="9"/>
-      <c r="AJ60" s="9"/>
-      <c r="AK60" s="9"/>
-      <c r="AL60" s="9"/>
-      <c r="AM60" s="9"/>
-      <c r="AN60" s="9"/>
-    </row>
-    <row r="61" spans="10:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AH61" s="9"/>
-      <c r="AI61" s="9"/>
-      <c r="AJ61" s="9"/>
-      <c r="AK61" s="9"/>
-      <c r="AL61" s="9"/>
-      <c r="AM61" s="9"/>
-      <c r="AN61" s="9"/>
-    </row>
-    <row r="62" spans="10:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AH62" s="9"/>
-      <c r="AI62" s="9"/>
-      <c r="AJ62" s="9"/>
-      <c r="AK62" s="9"/>
-      <c r="AL62" s="9"/>
-      <c r="AM62" s="9"/>
-      <c r="AN62" s="9"/>
-    </row>
-    <row r="63" spans="10:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AH63" s="9"/>
-      <c r="AI63" s="9"/>
-      <c r="AJ63" s="9"/>
-      <c r="AK63" s="9"/>
-      <c r="AL63" s="9"/>
-      <c r="AM63" s="9"/>
-      <c r="AN63" s="9"/>
-    </row>
-    <row r="64" spans="10:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AH64" s="9"/>
-      <c r="AI64" s="9"/>
-      <c r="AJ64" s="9"/>
-      <c r="AK64" s="9"/>
-      <c r="AL64" s="9"/>
-      <c r="AM64" s="9"/>
-      <c r="AN64" s="9"/>
-    </row>
-    <row r="65" spans="34:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AH65" s="9"/>
-      <c r="AI65" s="9"/>
-      <c r="AJ65" s="9"/>
-      <c r="AK65" s="9"/>
-      <c r="AL65" s="9"/>
-      <c r="AM65" s="9"/>
-      <c r="AN65" s="9"/>
-    </row>
-    <row r="66" spans="34:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AH66" s="9"/>
-      <c r="AI66" s="9"/>
-      <c r="AJ66" s="9"/>
-      <c r="AK66" s="9"/>
-      <c r="AL66" s="9"/>
-      <c r="AM66" s="9"/>
-      <c r="AN66" s="9"/>
-    </row>
-    <row r="67" spans="34:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AH67" s="9"/>
-      <c r="AI67" s="9"/>
-      <c r="AJ67" s="9"/>
-      <c r="AK67" s="9"/>
-      <c r="AL67" s="9"/>
-      <c r="AM67" s="9"/>
-      <c r="AN67" s="9"/>
+    <row r="50" spans="10:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J50" s="9"/>
+    </row>
+    <row r="61" spans="10:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AR61" s="9"/>
+      <c r="AS61" s="9"/>
+      <c r="AT61" s="9"/>
+      <c r="AU61" s="9"/>
+      <c r="AV61" s="9"/>
+      <c r="AW61" s="9"/>
+      <c r="AX61" s="9"/>
+    </row>
+    <row r="62" spans="10:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AR62" s="9"/>
+      <c r="AS62" s="9"/>
+      <c r="AT62" s="9"/>
+      <c r="AU62" s="9"/>
+      <c r="AV62" s="9"/>
+      <c r="AW62" s="9"/>
+      <c r="AX62" s="9"/>
+    </row>
+    <row r="63" spans="10:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AR63" s="9"/>
+      <c r="AS63" s="9"/>
+      <c r="AT63" s="9"/>
+      <c r="AU63" s="9"/>
+      <c r="AV63" s="9"/>
+      <c r="AW63" s="9"/>
+      <c r="AX63" s="9"/>
+    </row>
+    <row r="64" spans="10:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AR64" s="9"/>
+      <c r="AS64" s="9"/>
+      <c r="AT64" s="9"/>
+      <c r="AU64" s="9"/>
+      <c r="AV64" s="9"/>
+      <c r="AW64" s="9"/>
+      <c r="AX64" s="9"/>
+    </row>
+    <row r="65" spans="44:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AR65" s="9"/>
+      <c r="AS65" s="9"/>
+      <c r="AT65" s="9"/>
+      <c r="AU65" s="9"/>
+      <c r="AV65" s="9"/>
+      <c r="AW65" s="9"/>
+      <c r="AX65" s="9"/>
+    </row>
+    <row r="66" spans="44:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AR66" s="9"/>
+      <c r="AS66" s="9"/>
+      <c r="AT66" s="9"/>
+      <c r="AU66" s="9"/>
+      <c r="AV66" s="9"/>
+      <c r="AW66" s="9"/>
+      <c r="AX66" s="9"/>
+    </row>
+    <row r="67" spans="44:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AR67" s="9"/>
+      <c r="AS67" s="9"/>
+      <c r="AT67" s="9"/>
+      <c r="AU67" s="9"/>
+      <c r="AV67" s="9"/>
+      <c r="AW67" s="9"/>
+      <c r="AX67" s="9"/>
+    </row>
+    <row r="68" spans="44:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AR68" s="9"/>
+      <c r="AS68" s="9"/>
+      <c r="AT68" s="9"/>
+      <c r="AU68" s="9"/>
+      <c r="AV68" s="9"/>
+      <c r="AW68" s="9"/>
+      <c r="AX68" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="K42:AD43"/>
-    <mergeCell ref="K41:AD41"/>
-    <mergeCell ref="B40:J40"/>
-    <mergeCell ref="A1:AD1"/>
+  <mergeCells count="11">
+    <mergeCell ref="K43:AN44"/>
+    <mergeCell ref="K42:AN42"/>
+    <mergeCell ref="B41:J41"/>
+    <mergeCell ref="A1:AN1"/>
     <mergeCell ref="U3:Y3"/>
     <mergeCell ref="Z3:AD3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="K3:O3"/>
     <mergeCell ref="P3:T3"/>
+    <mergeCell ref="AE3:AI3"/>
+    <mergeCell ref="AJ3:AN3"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -5040,21 +5612,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="197"/>
-      <c r="B1" s="197"/>
-      <c r="C1" s="197"/>
-      <c r="D1" s="197"/>
-      <c r="E1" s="197"/>
-      <c r="F1" s="197"/>
-      <c r="G1" s="197"/>
-      <c r="H1" s="197"/>
-      <c r="I1" s="197"/>
-      <c r="J1" s="197"/>
-      <c r="K1" s="197"/>
-      <c r="L1" s="197"/>
-      <c r="M1" s="197"/>
-      <c r="N1" s="197"/>
-      <c r="O1" s="197"/>
+      <c r="A1" s="196"/>
+      <c r="B1" s="196"/>
+      <c r="C1" s="196"/>
+      <c r="D1" s="196"/>
+      <c r="E1" s="196"/>
+      <c r="F1" s="196"/>
+      <c r="G1" s="196"/>
+      <c r="H1" s="196"/>
+      <c r="I1" s="196"/>
+      <c r="J1" s="196"/>
+      <c r="K1" s="196"/>
+      <c r="L1" s="196"/>
+      <c r="M1" s="196"/>
+      <c r="N1" s="196"/>
+      <c r="O1" s="196"/>
     </row>
     <row r="2" spans="1:15" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -5075,13 +5647,13 @@
     </row>
     <row r="3" spans="1:15" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -5093,7 +5665,7 @@
         <v>42702</v>
       </c>
       <c r="C4" s="5">
-        <f>'IPA Zeitplanung'!K39</f>
+        <f>'IPA Zeitplanung'!K40</f>
         <v>0</v>
       </c>
     </row>
@@ -5106,7 +5678,7 @@
         <v>42703</v>
       </c>
       <c r="C5" s="5">
-        <f>'IPA Zeitplanung'!L39</f>
+        <f>'IPA Zeitplanung'!L40</f>
         <v>0</v>
       </c>
     </row>
@@ -5119,7 +5691,7 @@
         <v>42704</v>
       </c>
       <c r="C6" s="5">
-        <f>'IPA Zeitplanung'!M39</f>
+        <f>'IPA Zeitplanung'!M40</f>
         <v>0</v>
       </c>
     </row>
@@ -5132,7 +5704,7 @@
         <v>42705</v>
       </c>
       <c r="C7" s="5">
-        <f>'IPA Zeitplanung'!N39</f>
+        <f>'IPA Zeitplanung'!N40</f>
         <v>0</v>
       </c>
     </row>
@@ -5145,7 +5717,7 @@
         <v>42706</v>
       </c>
       <c r="C8" s="5">
-        <f>'IPA Zeitplanung'!O39</f>
+        <f>'IPA Zeitplanung'!O40</f>
         <v>0</v>
       </c>
     </row>
@@ -5158,7 +5730,7 @@
         <v>42709</v>
       </c>
       <c r="C9" s="5">
-        <f>'IPA Zeitplanung'!P39</f>
+        <f>'IPA Zeitplanung'!P40</f>
         <v>0</v>
       </c>
     </row>
@@ -5171,7 +5743,7 @@
         <v>42710</v>
       </c>
       <c r="C10" s="5">
-        <f>'IPA Zeitplanung'!Q39</f>
+        <f>'IPA Zeitplanung'!Q40</f>
         <v>0</v>
       </c>
     </row>
@@ -5184,7 +5756,7 @@
         <v>42711</v>
       </c>
       <c r="C11" s="5">
-        <f>'IPA Zeitplanung'!R39</f>
+        <f>'IPA Zeitplanung'!R40</f>
         <v>0</v>
       </c>
     </row>
@@ -5197,7 +5769,7 @@
         <v>42712</v>
       </c>
       <c r="C12" s="5">
-        <f>'IPA Zeitplanung'!S39</f>
+        <f>'IPA Zeitplanung'!S40</f>
         <v>0</v>
       </c>
     </row>
@@ -5210,7 +5782,7 @@
         <v>42713</v>
       </c>
       <c r="C13" s="5">
-        <f>'IPA Zeitplanung'!T39</f>
+        <f>'IPA Zeitplanung'!T40</f>
         <v>0</v>
       </c>
     </row>
@@ -5223,7 +5795,7 @@
         <v>42716</v>
       </c>
       <c r="C14" s="5">
-        <f>'IPA Zeitplanung'!U39</f>
+        <f>'IPA Zeitplanung'!U40</f>
         <v>0</v>
       </c>
     </row>
@@ -5236,7 +5808,7 @@
         <v>42717</v>
       </c>
       <c r="C15" s="5">
-        <f>'IPA Zeitplanung'!V39</f>
+        <f>'IPA Zeitplanung'!V40</f>
         <v>0</v>
       </c>
     </row>
@@ -5249,7 +5821,7 @@
         <v>42718</v>
       </c>
       <c r="C16" s="5">
-        <f>'IPA Zeitplanung'!W39</f>
+        <f>'IPA Zeitplanung'!W40</f>
         <v>0</v>
       </c>
     </row>
@@ -5262,7 +5834,7 @@
         <v>42719</v>
       </c>
       <c r="C17" s="5">
-        <f>'IPA Zeitplanung'!X39</f>
+        <f>'IPA Zeitplanung'!X40</f>
         <v>0</v>
       </c>
     </row>
@@ -5275,7 +5847,7 @@
         <v>42720</v>
       </c>
       <c r="C18" s="5">
-        <f>'IPA Zeitplanung'!Y39</f>
+        <f>'IPA Zeitplanung'!Y40</f>
         <v>0</v>
       </c>
     </row>
@@ -5288,7 +5860,7 @@
         <v>42723</v>
       </c>
       <c r="C19" s="5">
-        <f>'IPA Zeitplanung'!Z39</f>
+        <f>'IPA Zeitplanung'!Z40</f>
         <v>0</v>
       </c>
     </row>
@@ -5301,7 +5873,7 @@
         <v>42724</v>
       </c>
       <c r="C20" s="5">
-        <f>'IPA Zeitplanung'!AA39</f>
+        <f>'IPA Zeitplanung'!AA40</f>
         <v>0</v>
       </c>
     </row>
@@ -5314,7 +5886,7 @@
         <v>42725</v>
       </c>
       <c r="C21" s="5">
-        <f>'IPA Zeitplanung'!AB39</f>
+        <f>'IPA Zeitplanung'!AB40</f>
         <v>0</v>
       </c>
     </row>
@@ -5327,7 +5899,7 @@
         <v>42726</v>
       </c>
       <c r="C22" s="5">
-        <f>'IPA Zeitplanung'!AC39</f>
+        <f>'IPA Zeitplanung'!AC40</f>
         <v>0</v>
       </c>
     </row>
@@ -5340,7 +5912,7 @@
         <v>42727</v>
       </c>
       <c r="C23" s="5">
-        <f>'IPA Zeitplanung'!AD39</f>
+        <f>'IPA Zeitplanung'!AD40</f>
         <v>0</v>
       </c>
     </row>
@@ -5360,22 +5932,22 @@
     <row r="25" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="198" t="s">
+      <c r="A27" s="197" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="198"/>
+      <c r="C27" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="199"/>
-      <c r="C27" s="4" t="s">
+      <c r="D27" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="28" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="195" t="s">
-        <v>12</v>
-      </c>
-      <c r="B28" s="196"/>
+      <c r="A28" s="194" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="195"/>
       <c r="C28" s="5">
         <f>'IPA Zeitplanung'!C5</f>
         <v>0</v>
@@ -5386,10 +5958,10 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="200" t="s">
-        <v>17</v>
-      </c>
-      <c r="B29" s="201"/>
+      <c r="A29" s="199" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="200"/>
       <c r="C29" s="5">
         <f>'IPA Zeitplanung'!C11</f>
         <v>0</v>
@@ -5400,10 +5972,10 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="195" t="s">
-        <v>11</v>
-      </c>
-      <c r="B30" s="196"/>
+      <c r="A30" s="194" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="195"/>
       <c r="C30" s="5">
         <f>'IPA Zeitplanung'!C15</f>
         <v>81</v>
@@ -5414,44 +5986,44 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="200" t="s">
+      <c r="A31" s="199" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="200"/>
+      <c r="C31" s="5">
+        <f>'IPA Zeitplanung'!C28</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="5">
+        <f>'IPA Zeitplanung'!D28</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="194" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="195"/>
+      <c r="C32" s="5">
+        <f>'IPA Zeitplanung'!C33</f>
+        <v>16.2</v>
+      </c>
+      <c r="D32" s="5">
+        <f>SUM('IPA Zeitplanung'!D33)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="194" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="201"/>
-      <c r="C31" s="5">
-        <f>'IPA Zeitplanung'!C27</f>
-        <v>0</v>
-      </c>
-      <c r="D31" s="5">
-        <f>'IPA Zeitplanung'!D27</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="195" t="s">
-        <v>13</v>
-      </c>
-      <c r="B32" s="196"/>
-      <c r="C32" s="5">
-        <f>'IPA Zeitplanung'!C32</f>
-        <v>16.2</v>
-      </c>
-      <c r="D32" s="5">
-        <f>SUM('IPA Zeitplanung'!D32)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="195" t="s">
-        <v>10</v>
-      </c>
-      <c r="B33" s="196"/>
+      <c r="B33" s="195"/>
       <c r="C33" s="5">
-        <f>'IPA Zeitplanung'!C36</f>
+        <f>'IPA Zeitplanung'!C37</f>
         <v>0</v>
       </c>
       <c r="D33" s="5">
-        <f>'IPA Zeitplanung'!D36</f>
+        <f>'IPA Zeitplanung'!D37</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
login auf start seite und funktionierend
</commit_message>
<xml_diff>
--- a/documents/Zeitplanung.xlsx
+++ b/documents/Zeitplanung.xlsx
@@ -2169,6 +2169,69 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="25" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="54" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="54" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="48" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="32" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="52" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="84" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2210,69 +2273,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="59" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="60" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="54" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="54" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="48" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="32" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="52" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="84" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20 % - Akzent4" xfId="6" builtinId="42"/>
@@ -3195,10 +3195,10 @@
   <dimension ref="A1:AX68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="10" ySplit="4" topLeftCell="R5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="4" topLeftCell="K14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="N1" sqref="N1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AP13" sqref="AP13"/>
+      <selection pane="bottomRight" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3218,48 +3218,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="190" t="s">
+      <c r="A1" s="211" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="190"/>
-      <c r="C1" s="190"/>
-      <c r="D1" s="190"/>
-      <c r="E1" s="190"/>
-      <c r="F1" s="190"/>
-      <c r="G1" s="190"/>
-      <c r="H1" s="190"/>
-      <c r="I1" s="190"/>
-      <c r="J1" s="190"/>
-      <c r="K1" s="190"/>
-      <c r="L1" s="190"/>
-      <c r="M1" s="190"/>
-      <c r="N1" s="190"/>
-      <c r="O1" s="190"/>
-      <c r="P1" s="190"/>
-      <c r="Q1" s="190"/>
-      <c r="R1" s="190"/>
-      <c r="S1" s="190"/>
-      <c r="T1" s="190"/>
-      <c r="U1" s="190"/>
-      <c r="V1" s="190"/>
-      <c r="W1" s="190"/>
-      <c r="X1" s="190"/>
-      <c r="Y1" s="190"/>
-      <c r="Z1" s="190"/>
-      <c r="AA1" s="190"/>
-      <c r="AB1" s="190"/>
-      <c r="AC1" s="190"/>
-      <c r="AD1" s="190"/>
-      <c r="AE1" s="190"/>
-      <c r="AF1" s="190"/>
-      <c r="AG1" s="190"/>
-      <c r="AH1" s="190"/>
-      <c r="AI1" s="190"/>
-      <c r="AJ1" s="190"/>
-      <c r="AK1" s="190"/>
-      <c r="AL1" s="190"/>
-      <c r="AM1" s="190"/>
-      <c r="AN1" s="190"/>
+      <c r="B1" s="211"/>
+      <c r="C1" s="211"/>
+      <c r="D1" s="211"/>
+      <c r="E1" s="211"/>
+      <c r="F1" s="211"/>
+      <c r="G1" s="211"/>
+      <c r="H1" s="211"/>
+      <c r="I1" s="211"/>
+      <c r="J1" s="211"/>
+      <c r="K1" s="211"/>
+      <c r="L1" s="211"/>
+      <c r="M1" s="211"/>
+      <c r="N1" s="211"/>
+      <c r="O1" s="211"/>
+      <c r="P1" s="211"/>
+      <c r="Q1" s="211"/>
+      <c r="R1" s="211"/>
+      <c r="S1" s="211"/>
+      <c r="T1" s="211"/>
+      <c r="U1" s="211"/>
+      <c r="V1" s="211"/>
+      <c r="W1" s="211"/>
+      <c r="X1" s="211"/>
+      <c r="Y1" s="211"/>
+      <c r="Z1" s="211"/>
+      <c r="AA1" s="211"/>
+      <c r="AB1" s="211"/>
+      <c r="AC1" s="211"/>
+      <c r="AD1" s="211"/>
+      <c r="AE1" s="211"/>
+      <c r="AF1" s="211"/>
+      <c r="AG1" s="211"/>
+      <c r="AH1" s="211"/>
+      <c r="AI1" s="211"/>
+      <c r="AJ1" s="211"/>
+      <c r="AK1" s="211"/>
+      <c r="AL1" s="211"/>
+      <c r="AM1" s="211"/>
+      <c r="AN1" s="211"/>
     </row>
     <row r="2" spans="1:41" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10"/>
@@ -3276,58 +3276,58 @@
     <row r="3" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="83"/>
       <c r="B3" s="87"/>
-      <c r="C3" s="191" t="s">
+      <c r="C3" s="212" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="191"/>
+      <c r="D3" s="212"/>
       <c r="E3" s="22"/>
       <c r="F3" s="23"/>
       <c r="G3" s="25"/>
       <c r="H3" s="24"/>
       <c r="I3" s="25"/>
       <c r="J3" s="22"/>
-      <c r="K3" s="191" t="s">
+      <c r="K3" s="212" t="s">
         <v>52</v>
       </c>
-      <c r="L3" s="191"/>
-      <c r="M3" s="191"/>
-      <c r="N3" s="191"/>
-      <c r="O3" s="192"/>
-      <c r="P3" s="193" t="s">
+      <c r="L3" s="212"/>
+      <c r="M3" s="212"/>
+      <c r="N3" s="212"/>
+      <c r="O3" s="213"/>
+      <c r="P3" s="214" t="s">
         <v>53</v>
       </c>
-      <c r="Q3" s="191"/>
-      <c r="R3" s="191"/>
-      <c r="S3" s="191"/>
-      <c r="T3" s="192"/>
-      <c r="U3" s="191" t="s">
+      <c r="Q3" s="212"/>
+      <c r="R3" s="212"/>
+      <c r="S3" s="212"/>
+      <c r="T3" s="213"/>
+      <c r="U3" s="212" t="s">
         <v>54</v>
       </c>
-      <c r="V3" s="191"/>
-      <c r="W3" s="191"/>
-      <c r="X3" s="191"/>
-      <c r="Y3" s="192"/>
-      <c r="Z3" s="193" t="s">
+      <c r="V3" s="212"/>
+      <c r="W3" s="212"/>
+      <c r="X3" s="212"/>
+      <c r="Y3" s="213"/>
+      <c r="Z3" s="214" t="s">
         <v>55</v>
       </c>
-      <c r="AA3" s="191"/>
-      <c r="AB3" s="191"/>
-      <c r="AC3" s="191"/>
-      <c r="AD3" s="192"/>
-      <c r="AE3" s="193" t="s">
+      <c r="AA3" s="212"/>
+      <c r="AB3" s="212"/>
+      <c r="AC3" s="212"/>
+      <c r="AD3" s="213"/>
+      <c r="AE3" s="214" t="s">
         <v>59</v>
       </c>
-      <c r="AF3" s="191"/>
-      <c r="AG3" s="191"/>
-      <c r="AH3" s="191"/>
-      <c r="AI3" s="192"/>
-      <c r="AJ3" s="193" t="s">
+      <c r="AF3" s="212"/>
+      <c r="AG3" s="212"/>
+      <c r="AH3" s="212"/>
+      <c r="AI3" s="213"/>
+      <c r="AJ3" s="214" t="s">
         <v>60</v>
       </c>
-      <c r="AK3" s="191"/>
-      <c r="AL3" s="191"/>
-      <c r="AM3" s="191"/>
-      <c r="AN3" s="192"/>
+      <c r="AK3" s="212"/>
+      <c r="AL3" s="212"/>
+      <c r="AM3" s="212"/>
+      <c r="AN3" s="213"/>
       <c r="AO3" s="13"/>
     </row>
     <row r="4" spans="1:41" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3559,12 +3559,12 @@
       <c r="AF6" s="72"/>
       <c r="AG6" s="72"/>
       <c r="AH6" s="72"/>
-      <c r="AI6" s="202"/>
-      <c r="AJ6" s="218"/>
-      <c r="AK6" s="218"/>
-      <c r="AL6" s="218"/>
-      <c r="AM6" s="218"/>
-      <c r="AN6" s="218"/>
+      <c r="AI6" s="187"/>
+      <c r="AJ6" s="203"/>
+      <c r="AK6" s="203"/>
+      <c r="AL6" s="203"/>
+      <c r="AM6" s="203"/>
+      <c r="AN6" s="203"/>
     </row>
     <row r="7" spans="1:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="84">
@@ -3610,7 +3610,7 @@
       <c r="AF7" s="55"/>
       <c r="AG7" s="55"/>
       <c r="AH7" s="55"/>
-      <c r="AI7" s="203"/>
+      <c r="AI7" s="188"/>
       <c r="AJ7" s="176"/>
       <c r="AK7" s="176"/>
       <c r="AL7" s="176"/>
@@ -3661,12 +3661,12 @@
       <c r="AF8" s="55"/>
       <c r="AG8" s="55"/>
       <c r="AH8" s="55"/>
-      <c r="AI8" s="203"/>
-      <c r="AJ8" s="219"/>
-      <c r="AK8" s="219"/>
-      <c r="AL8" s="219"/>
-      <c r="AM8" s="219"/>
-      <c r="AN8" s="219"/>
+      <c r="AI8" s="188"/>
+      <c r="AJ8" s="204"/>
+      <c r="AK8" s="204"/>
+      <c r="AL8" s="204"/>
+      <c r="AM8" s="204"/>
+      <c r="AN8" s="204"/>
     </row>
     <row r="9" spans="1:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="84">
@@ -3707,7 +3707,7 @@
       <c r="AB9" s="50"/>
       <c r="AC9" s="36"/>
       <c r="AD9" s="166"/>
-      <c r="AI9" s="204"/>
+      <c r="AI9" s="189"/>
       <c r="AJ9" s="176"/>
       <c r="AK9" s="176"/>
       <c r="AL9" s="176"/>
@@ -3758,12 +3758,12 @@
       <c r="AF10" s="64"/>
       <c r="AG10" s="64"/>
       <c r="AH10" s="64"/>
-      <c r="AI10" s="205"/>
-      <c r="AJ10" s="220"/>
-      <c r="AK10" s="220"/>
-      <c r="AL10" s="220"/>
-      <c r="AM10" s="220"/>
-      <c r="AN10" s="220"/>
+      <c r="AI10" s="190"/>
+      <c r="AJ10" s="205"/>
+      <c r="AK10" s="205"/>
+      <c r="AL10" s="205"/>
+      <c r="AM10" s="205"/>
+      <c r="AN10" s="205"/>
     </row>
     <row r="11" spans="1:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="111">
@@ -3859,12 +3859,12 @@
       <c r="AF12" s="72"/>
       <c r="AG12" s="72"/>
       <c r="AH12" s="72"/>
-      <c r="AI12" s="202"/>
-      <c r="AJ12" s="218"/>
-      <c r="AK12" s="218"/>
-      <c r="AL12" s="218"/>
-      <c r="AM12" s="218"/>
-      <c r="AN12" s="218"/>
+      <c r="AI12" s="187"/>
+      <c r="AJ12" s="203"/>
+      <c r="AK12" s="203"/>
+      <c r="AL12" s="203"/>
+      <c r="AM12" s="203"/>
+      <c r="AN12" s="203"/>
     </row>
     <row r="13" spans="1:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="85">
@@ -3906,12 +3906,12 @@
       <c r="AF13" s="72"/>
       <c r="AG13" s="72"/>
       <c r="AH13" s="72"/>
-      <c r="AI13" s="202"/>
-      <c r="AJ13" s="218"/>
-      <c r="AK13" s="218"/>
-      <c r="AL13" s="218"/>
-      <c r="AM13" s="218"/>
-      <c r="AN13" s="218"/>
+      <c r="AI13" s="187"/>
+      <c r="AJ13" s="203"/>
+      <c r="AK13" s="203"/>
+      <c r="AL13" s="203"/>
+      <c r="AM13" s="203"/>
+      <c r="AN13" s="203"/>
     </row>
     <row r="14" spans="1:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="85">
@@ -3953,12 +3953,12 @@
       <c r="AF14" s="72"/>
       <c r="AG14" s="72"/>
       <c r="AH14" s="72"/>
-      <c r="AI14" s="202"/>
-      <c r="AJ14" s="218"/>
-      <c r="AK14" s="218"/>
-      <c r="AL14" s="218"/>
-      <c r="AM14" s="218"/>
-      <c r="AN14" s="218"/>
+      <c r="AI14" s="187"/>
+      <c r="AJ14" s="203"/>
+      <c r="AK14" s="203"/>
+      <c r="AL14" s="203"/>
+      <c r="AM14" s="203"/>
+      <c r="AN14" s="203"/>
     </row>
     <row r="15" spans="1:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="111">
@@ -4001,16 +4001,16 @@
       <c r="AB15" s="122"/>
       <c r="AC15" s="123"/>
       <c r="AD15" s="124"/>
-      <c r="AE15" s="214"/>
-      <c r="AF15" s="214"/>
-      <c r="AG15" s="214"/>
+      <c r="AE15" s="199"/>
+      <c r="AF15" s="199"/>
+      <c r="AG15" s="199"/>
       <c r="AH15" s="121"/>
       <c r="AI15" s="116"/>
-      <c r="AJ15" s="214"/>
-      <c r="AK15" s="214"/>
-      <c r="AL15" s="214"/>
-      <c r="AM15" s="214"/>
-      <c r="AN15" s="214"/>
+      <c r="AJ15" s="199"/>
+      <c r="AK15" s="199"/>
+      <c r="AL15" s="199"/>
+      <c r="AM15" s="199"/>
+      <c r="AN15" s="199"/>
     </row>
     <row r="16" spans="1:41" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="85">
@@ -4052,12 +4052,12 @@
       <c r="AA16" s="161"/>
       <c r="AB16" s="161"/>
       <c r="AC16" s="71"/>
-      <c r="AD16" s="213"/>
-      <c r="AE16" s="216"/>
-      <c r="AF16" s="216"/>
-      <c r="AG16" s="216"/>
+      <c r="AD16" s="198"/>
+      <c r="AE16" s="201"/>
+      <c r="AF16" s="201"/>
+      <c r="AG16" s="201"/>
       <c r="AH16" s="150"/>
-      <c r="AI16" s="206"/>
+      <c r="AI16" s="191"/>
       <c r="AJ16" s="176"/>
       <c r="AK16" s="176"/>
       <c r="AL16" s="176"/>
@@ -4104,12 +4104,12 @@
       <c r="AA17" s="161"/>
       <c r="AB17" s="161"/>
       <c r="AC17" s="71"/>
-      <c r="AD17" s="213"/>
-      <c r="AE17" s="212"/>
-      <c r="AF17" s="212"/>
-      <c r="AG17" s="212"/>
+      <c r="AD17" s="198"/>
+      <c r="AE17" s="197"/>
+      <c r="AF17" s="197"/>
+      <c r="AG17" s="197"/>
       <c r="AH17" s="35"/>
-      <c r="AI17" s="202"/>
+      <c r="AI17" s="187"/>
       <c r="AJ17" s="176"/>
       <c r="AK17" s="176"/>
       <c r="AL17" s="176"/>
@@ -4151,12 +4151,12 @@
       <c r="Z18" s="153"/>
       <c r="AA18" s="161"/>
       <c r="AB18" s="161"/>
-      <c r="AD18" s="213"/>
-      <c r="AE18" s="216"/>
-      <c r="AF18" s="216"/>
-      <c r="AG18" s="216"/>
+      <c r="AD18" s="198"/>
+      <c r="AE18" s="201"/>
+      <c r="AF18" s="201"/>
+      <c r="AG18" s="201"/>
       <c r="AH18" s="150"/>
-      <c r="AI18" s="206"/>
+      <c r="AI18" s="191"/>
       <c r="AJ18" s="176"/>
       <c r="AK18" s="176"/>
       <c r="AL18" s="176"/>
@@ -4199,11 +4199,11 @@
       <c r="AB19" s="161"/>
       <c r="AC19" s="167"/>
       <c r="AD19" s="169"/>
-      <c r="AE19" s="216"/>
-      <c r="AF19" s="216"/>
-      <c r="AG19" s="216"/>
+      <c r="AE19" s="201"/>
+      <c r="AF19" s="201"/>
+      <c r="AG19" s="201"/>
       <c r="AH19" s="155"/>
-      <c r="AI19" s="206"/>
+      <c r="AI19" s="191"/>
       <c r="AJ19" s="176"/>
       <c r="AK19" s="176"/>
       <c r="AL19" s="176"/>
@@ -4245,12 +4245,12 @@
       <c r="AA20" s="161"/>
       <c r="AB20" s="161"/>
       <c r="AC20" s="71"/>
-      <c r="AD20" s="213"/>
-      <c r="AE20" s="211"/>
-      <c r="AF20" s="211"/>
-      <c r="AG20" s="211"/>
-      <c r="AH20" s="201"/>
-      <c r="AI20" s="207"/>
+      <c r="AD20" s="198"/>
+      <c r="AE20" s="196"/>
+      <c r="AF20" s="196"/>
+      <c r="AG20" s="196"/>
+      <c r="AH20" s="186"/>
+      <c r="AI20" s="192"/>
       <c r="AJ20" s="176"/>
       <c r="AK20" s="176"/>
       <c r="AL20" s="176"/>
@@ -4293,12 +4293,12 @@
       <c r="AA21" s="161"/>
       <c r="AB21" s="161"/>
       <c r="AC21" s="71"/>
-      <c r="AD21" s="213"/>
-      <c r="AE21" s="216"/>
-      <c r="AF21" s="216"/>
-      <c r="AG21" s="216"/>
+      <c r="AD21" s="198"/>
+      <c r="AE21" s="201"/>
+      <c r="AF21" s="201"/>
+      <c r="AG21" s="201"/>
       <c r="AH21" s="35"/>
-      <c r="AI21" s="202"/>
+      <c r="AI21" s="187"/>
       <c r="AJ21" s="176"/>
       <c r="AK21" s="176"/>
       <c r="AL21" s="176"/>
@@ -4341,12 +4341,12 @@
       <c r="AA22" s="161"/>
       <c r="AB22" s="161"/>
       <c r="AC22" s="42"/>
-      <c r="AD22" s="213"/>
-      <c r="AE22" s="216"/>
-      <c r="AF22" s="216"/>
-      <c r="AG22" s="216"/>
+      <c r="AD22" s="198"/>
+      <c r="AE22" s="201"/>
+      <c r="AF22" s="201"/>
+      <c r="AG22" s="201"/>
       <c r="AH22" s="35"/>
-      <c r="AI22" s="202"/>
+      <c r="AI22" s="187"/>
       <c r="AJ22" s="176"/>
       <c r="AK22" s="176"/>
       <c r="AL22" s="176"/>
@@ -4392,12 +4392,12 @@
       <c r="AA23" s="162"/>
       <c r="AB23" s="162"/>
       <c r="AC23" s="42"/>
-      <c r="AD23" s="213"/>
-      <c r="AE23" s="216"/>
-      <c r="AF23" s="216"/>
-      <c r="AG23" s="216"/>
+      <c r="AD23" s="198"/>
+      <c r="AE23" s="201"/>
+      <c r="AF23" s="201"/>
+      <c r="AG23" s="201"/>
       <c r="AH23" s="35"/>
-      <c r="AI23" s="202"/>
+      <c r="AI23" s="187"/>
       <c r="AJ23" s="176"/>
       <c r="AK23" s="176"/>
       <c r="AL23" s="176"/>
@@ -4442,12 +4442,12 @@
       <c r="AA24" s="162"/>
       <c r="AB24" s="162"/>
       <c r="AC24" s="42"/>
-      <c r="AD24" s="213"/>
-      <c r="AE24" s="216"/>
-      <c r="AF24" s="216"/>
-      <c r="AG24" s="216"/>
+      <c r="AD24" s="198"/>
+      <c r="AE24" s="201"/>
+      <c r="AF24" s="201"/>
+      <c r="AG24" s="201"/>
       <c r="AH24" s="35"/>
-      <c r="AI24" s="202"/>
+      <c r="AI24" s="187"/>
       <c r="AJ24" s="176"/>
       <c r="AK24" s="176"/>
       <c r="AL24" s="176"/>
@@ -4492,12 +4492,12 @@
       <c r="AA25" s="162"/>
       <c r="AB25" s="162"/>
       <c r="AC25" s="42"/>
-      <c r="AD25" s="213"/>
-      <c r="AE25" s="212"/>
-      <c r="AF25" s="212"/>
-      <c r="AG25" s="212"/>
+      <c r="AD25" s="198"/>
+      <c r="AE25" s="197"/>
+      <c r="AF25" s="197"/>
+      <c r="AG25" s="197"/>
       <c r="AH25" s="35"/>
-      <c r="AI25" s="202"/>
+      <c r="AI25" s="187"/>
       <c r="AJ25" s="176"/>
       <c r="AK25" s="176"/>
       <c r="AL25" s="176"/>
@@ -4543,11 +4543,11 @@
       <c r="AB26" s="183"/>
       <c r="AC26" s="178"/>
       <c r="AD26" s="178"/>
-      <c r="AE26" s="212"/>
-      <c r="AF26" s="212"/>
-      <c r="AG26" s="212"/>
+      <c r="AE26" s="197"/>
+      <c r="AF26" s="197"/>
+      <c r="AG26" s="197"/>
       <c r="AH26" s="35"/>
-      <c r="AI26" s="202"/>
+      <c r="AI26" s="187"/>
       <c r="AJ26" s="176"/>
       <c r="AK26" s="176"/>
       <c r="AL26" s="176"/>
@@ -4562,7 +4562,9 @@
       <c r="C27" s="79">
         <v>10</v>
       </c>
-      <c r="D27" s="71"/>
+      <c r="D27" s="71">
+        <v>7.5</v>
+      </c>
       <c r="E27" s="34">
         <v>1</v>
       </c>
@@ -4585,15 +4587,15 @@
       <c r="V27" s="183"/>
       <c r="W27" s="183"/>
       <c r="X27" s="78"/>
-      <c r="Y27" s="217"/>
+      <c r="Y27" s="202"/>
       <c r="Z27" s="41"/>
       <c r="AA27" s="183"/>
       <c r="AB27" s="183"/>
       <c r="AC27" s="42"/>
-      <c r="AD27" s="213"/>
-      <c r="AE27" s="212"/>
-      <c r="AF27" s="212"/>
-      <c r="AG27" s="212"/>
+      <c r="AD27" s="198"/>
+      <c r="AE27" s="197"/>
+      <c r="AF27" s="197"/>
+      <c r="AG27" s="197"/>
       <c r="AH27" s="178"/>
       <c r="AI27" s="178"/>
       <c r="AJ27" s="176"/>
@@ -4643,16 +4645,16 @@
       <c r="AB28" s="122"/>
       <c r="AC28" s="123"/>
       <c r="AD28" s="124"/>
-      <c r="AE28" s="215"/>
-      <c r="AF28" s="215"/>
-      <c r="AG28" s="215"/>
+      <c r="AE28" s="200"/>
+      <c r="AF28" s="200"/>
+      <c r="AG28" s="200"/>
       <c r="AH28" s="121"/>
       <c r="AI28" s="116"/>
-      <c r="AJ28" s="215"/>
-      <c r="AK28" s="215"/>
-      <c r="AL28" s="215"/>
-      <c r="AM28" s="215"/>
-      <c r="AN28" s="215"/>
+      <c r="AJ28" s="200"/>
+      <c r="AK28" s="200"/>
+      <c r="AL28" s="200"/>
+      <c r="AM28" s="200"/>
+      <c r="AN28" s="200"/>
     </row>
     <row r="29" spans="1:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="85">
@@ -4698,12 +4700,12 @@
       <c r="AF29" s="72"/>
       <c r="AG29" s="72"/>
       <c r="AH29" s="72"/>
-      <c r="AI29" s="202"/>
-      <c r="AJ29" s="218"/>
-      <c r="AK29" s="218"/>
-      <c r="AL29" s="218"/>
-      <c r="AM29" s="218"/>
-      <c r="AN29" s="218"/>
+      <c r="AI29" s="187"/>
+      <c r="AJ29" s="203"/>
+      <c r="AK29" s="203"/>
+      <c r="AL29" s="203"/>
+      <c r="AM29" s="203"/>
+      <c r="AN29" s="203"/>
     </row>
     <row r="30" spans="1:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="85">
@@ -4749,12 +4751,12 @@
       <c r="AF30" s="72"/>
       <c r="AG30" s="72"/>
       <c r="AH30" s="72"/>
-      <c r="AI30" s="202"/>
-      <c r="AJ30" s="218"/>
-      <c r="AK30" s="218"/>
-      <c r="AL30" s="218"/>
-      <c r="AM30" s="218"/>
-      <c r="AN30" s="218"/>
+      <c r="AI30" s="187"/>
+      <c r="AJ30" s="203"/>
+      <c r="AK30" s="203"/>
+      <c r="AL30" s="203"/>
+      <c r="AM30" s="203"/>
+      <c r="AN30" s="203"/>
     </row>
     <row r="31" spans="1:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="85">
@@ -4800,7 +4802,7 @@
       <c r="AF31" s="79"/>
       <c r="AG31" s="79"/>
       <c r="AH31" s="79"/>
-      <c r="AI31" s="209"/>
+      <c r="AI31" s="194"/>
       <c r="AJ31" s="176"/>
       <c r="AK31" s="176"/>
       <c r="AL31" s="176"/>
@@ -4851,12 +4853,12 @@
       <c r="AF32" s="64"/>
       <c r="AG32" s="64"/>
       <c r="AH32" s="64"/>
-      <c r="AI32" s="205"/>
-      <c r="AJ32" s="220"/>
-      <c r="AK32" s="220"/>
-      <c r="AL32" s="220"/>
-      <c r="AM32" s="220"/>
-      <c r="AN32" s="220"/>
+      <c r="AI32" s="190"/>
+      <c r="AJ32" s="205"/>
+      <c r="AK32" s="205"/>
+      <c r="AL32" s="205"/>
+      <c r="AM32" s="205"/>
+      <c r="AN32" s="205"/>
     </row>
     <row r="33" spans="1:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="111">
@@ -4957,7 +4959,7 @@
       <c r="AF34" s="79"/>
       <c r="AG34" s="79"/>
       <c r="AH34" s="79"/>
-      <c r="AI34" s="209"/>
+      <c r="AI34" s="194"/>
       <c r="AJ34" s="176"/>
       <c r="AK34" s="176"/>
       <c r="AL34" s="176"/>
@@ -5007,7 +5009,7 @@
       <c r="AF35" s="79"/>
       <c r="AG35" s="79"/>
       <c r="AH35" s="79"/>
-      <c r="AI35" s="208"/>
+      <c r="AI35" s="193"/>
       <c r="AJ35" s="176"/>
       <c r="AK35" s="176"/>
       <c r="AL35" s="176"/>
@@ -5055,7 +5057,7 @@
       <c r="AF36" s="64"/>
       <c r="AG36" s="64"/>
       <c r="AH36" s="64"/>
-      <c r="AI36" s="208"/>
+      <c r="AI36" s="193"/>
       <c r="AJ36" s="176"/>
       <c r="AK36" s="176"/>
       <c r="AL36" s="176"/>
@@ -5158,12 +5160,12 @@
       <c r="AF38" s="72"/>
       <c r="AG38" s="72"/>
       <c r="AH38" s="72"/>
-      <c r="AI38" s="202"/>
-      <c r="AJ38" s="218"/>
-      <c r="AK38" s="218"/>
-      <c r="AL38" s="218"/>
-      <c r="AM38" s="218"/>
-      <c r="AN38" s="218"/>
+      <c r="AI38" s="187"/>
+      <c r="AJ38" s="203"/>
+      <c r="AK38" s="203"/>
+      <c r="AL38" s="203"/>
+      <c r="AM38" s="203"/>
+      <c r="AN38" s="203"/>
     </row>
     <row r="39" spans="1:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="84">
@@ -5209,12 +5211,12 @@
       <c r="AF39" s="55"/>
       <c r="AG39" s="55"/>
       <c r="AH39" s="55"/>
-      <c r="AI39" s="203"/>
-      <c r="AJ39" s="218"/>
-      <c r="AK39" s="218"/>
-      <c r="AL39" s="218"/>
-      <c r="AM39" s="218"/>
-      <c r="AN39" s="218"/>
+      <c r="AI39" s="188"/>
+      <c r="AJ39" s="203"/>
+      <c r="AK39" s="203"/>
+      <c r="AL39" s="203"/>
+      <c r="AM39" s="203"/>
+      <c r="AN39" s="203"/>
     </row>
     <row r="40" spans="1:40" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="110"/>
@@ -5320,23 +5322,23 @@
       <c r="AG40" s="134"/>
       <c r="AH40" s="134"/>
       <c r="AI40" s="134"/>
-      <c r="AJ40" s="221"/>
-      <c r="AK40" s="221"/>
-      <c r="AL40" s="221"/>
-      <c r="AM40" s="221"/>
-      <c r="AN40" s="221"/>
+      <c r="AJ40" s="206"/>
+      <c r="AK40" s="206"/>
+      <c r="AL40" s="206"/>
+      <c r="AM40" s="206"/>
+      <c r="AN40" s="206"/>
     </row>
     <row r="41" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="136"/>
-      <c r="B41" s="189"/>
-      <c r="C41" s="189"/>
-      <c r="D41" s="189"/>
-      <c r="E41" s="189"/>
-      <c r="F41" s="189"/>
-      <c r="G41" s="189"/>
-      <c r="H41" s="189"/>
-      <c r="I41" s="189"/>
-      <c r="J41" s="189"/>
+      <c r="B41" s="210"/>
+      <c r="C41" s="210"/>
+      <c r="D41" s="210"/>
+      <c r="E41" s="210"/>
+      <c r="F41" s="210"/>
+      <c r="G41" s="210"/>
+      <c r="H41" s="210"/>
+      <c r="I41" s="210"/>
+      <c r="J41" s="210"/>
     </row>
     <row r="42" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="137"/>
@@ -5351,36 +5353,36 @@
       <c r="H42" s="15"/>
       <c r="I42" s="15"/>
       <c r="J42" s="15"/>
-      <c r="K42" s="187"/>
-      <c r="L42" s="188"/>
-      <c r="M42" s="188"/>
-      <c r="N42" s="188"/>
-      <c r="O42" s="188"/>
-      <c r="P42" s="188"/>
-      <c r="Q42" s="188"/>
-      <c r="R42" s="188"/>
-      <c r="S42" s="188"/>
-      <c r="T42" s="188"/>
-      <c r="U42" s="188"/>
-      <c r="V42" s="188"/>
-      <c r="W42" s="188"/>
-      <c r="X42" s="188"/>
-      <c r="Y42" s="188"/>
-      <c r="Z42" s="188"/>
-      <c r="AA42" s="188"/>
-      <c r="AB42" s="188"/>
-      <c r="AC42" s="188"/>
-      <c r="AD42" s="188"/>
-      <c r="AE42" s="188"/>
-      <c r="AF42" s="188"/>
-      <c r="AG42" s="188"/>
-      <c r="AH42" s="188"/>
-      <c r="AI42" s="188"/>
-      <c r="AJ42" s="188"/>
-      <c r="AK42" s="188"/>
-      <c r="AL42" s="188"/>
-      <c r="AM42" s="188"/>
-      <c r="AN42" s="188"/>
+      <c r="K42" s="208"/>
+      <c r="L42" s="209"/>
+      <c r="M42" s="209"/>
+      <c r="N42" s="209"/>
+      <c r="O42" s="209"/>
+      <c r="P42" s="209"/>
+      <c r="Q42" s="209"/>
+      <c r="R42" s="209"/>
+      <c r="S42" s="209"/>
+      <c r="T42" s="209"/>
+      <c r="U42" s="209"/>
+      <c r="V42" s="209"/>
+      <c r="W42" s="209"/>
+      <c r="X42" s="209"/>
+      <c r="Y42" s="209"/>
+      <c r="Z42" s="209"/>
+      <c r="AA42" s="209"/>
+      <c r="AB42" s="209"/>
+      <c r="AC42" s="209"/>
+      <c r="AD42" s="209"/>
+      <c r="AE42" s="209"/>
+      <c r="AF42" s="209"/>
+      <c r="AG42" s="209"/>
+      <c r="AH42" s="209"/>
+      <c r="AI42" s="209"/>
+      <c r="AJ42" s="209"/>
+      <c r="AK42" s="209"/>
+      <c r="AL42" s="209"/>
+      <c r="AM42" s="209"/>
+      <c r="AN42" s="209"/>
     </row>
     <row r="43" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="172"/>
@@ -5395,39 +5397,39 @@
       <c r="H43" s="17"/>
       <c r="I43" s="17"/>
       <c r="J43" s="17"/>
-      <c r="K43" s="186"/>
-      <c r="L43" s="186"/>
-      <c r="M43" s="186"/>
-      <c r="N43" s="186"/>
-      <c r="O43" s="186"/>
-      <c r="P43" s="186"/>
-      <c r="Q43" s="186"/>
-      <c r="R43" s="186"/>
-      <c r="S43" s="186"/>
-      <c r="T43" s="186"/>
-      <c r="U43" s="186"/>
-      <c r="V43" s="186"/>
-      <c r="W43" s="186"/>
-      <c r="X43" s="186"/>
-      <c r="Y43" s="186"/>
-      <c r="Z43" s="186"/>
-      <c r="AA43" s="186"/>
-      <c r="AB43" s="186"/>
-      <c r="AC43" s="186"/>
-      <c r="AD43" s="186"/>
-      <c r="AE43" s="186"/>
-      <c r="AF43" s="186"/>
-      <c r="AG43" s="186"/>
-      <c r="AH43" s="186"/>
-      <c r="AI43" s="186"/>
-      <c r="AJ43" s="186"/>
-      <c r="AK43" s="186"/>
-      <c r="AL43" s="186"/>
-      <c r="AM43" s="186"/>
-      <c r="AN43" s="186"/>
+      <c r="K43" s="207"/>
+      <c r="L43" s="207"/>
+      <c r="M43" s="207"/>
+      <c r="N43" s="207"/>
+      <c r="O43" s="207"/>
+      <c r="P43" s="207"/>
+      <c r="Q43" s="207"/>
+      <c r="R43" s="207"/>
+      <c r="S43" s="207"/>
+      <c r="T43" s="207"/>
+      <c r="U43" s="207"/>
+      <c r="V43" s="207"/>
+      <c r="W43" s="207"/>
+      <c r="X43" s="207"/>
+      <c r="Y43" s="207"/>
+      <c r="Z43" s="207"/>
+      <c r="AA43" s="207"/>
+      <c r="AB43" s="207"/>
+      <c r="AC43" s="207"/>
+      <c r="AD43" s="207"/>
+      <c r="AE43" s="207"/>
+      <c r="AF43" s="207"/>
+      <c r="AG43" s="207"/>
+      <c r="AH43" s="207"/>
+      <c r="AI43" s="207"/>
+      <c r="AJ43" s="207"/>
+      <c r="AK43" s="207"/>
+      <c r="AL43" s="207"/>
+      <c r="AM43" s="207"/>
+      <c r="AN43" s="207"/>
     </row>
     <row r="44" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="210"/>
+      <c r="A44" s="195"/>
       <c r="B44" s="14" t="s">
         <v>57</v>
       </c>
@@ -5439,36 +5441,36 @@
       <c r="H44" s="17"/>
       <c r="I44" s="17"/>
       <c r="J44" s="17"/>
-      <c r="K44" s="186"/>
-      <c r="L44" s="186"/>
-      <c r="M44" s="186"/>
-      <c r="N44" s="186"/>
-      <c r="O44" s="186"/>
-      <c r="P44" s="186"/>
-      <c r="Q44" s="186"/>
-      <c r="R44" s="186"/>
-      <c r="S44" s="186"/>
-      <c r="T44" s="186"/>
-      <c r="U44" s="186"/>
-      <c r="V44" s="186"/>
-      <c r="W44" s="186"/>
-      <c r="X44" s="186"/>
-      <c r="Y44" s="186"/>
-      <c r="Z44" s="186"/>
-      <c r="AA44" s="186"/>
-      <c r="AB44" s="186"/>
-      <c r="AC44" s="186"/>
-      <c r="AD44" s="186"/>
-      <c r="AE44" s="186"/>
-      <c r="AF44" s="186"/>
-      <c r="AG44" s="186"/>
-      <c r="AH44" s="186"/>
-      <c r="AI44" s="186"/>
-      <c r="AJ44" s="186"/>
-      <c r="AK44" s="186"/>
-      <c r="AL44" s="186"/>
-      <c r="AM44" s="186"/>
-      <c r="AN44" s="186"/>
+      <c r="K44" s="207"/>
+      <c r="L44" s="207"/>
+      <c r="M44" s="207"/>
+      <c r="N44" s="207"/>
+      <c r="O44" s="207"/>
+      <c r="P44" s="207"/>
+      <c r="Q44" s="207"/>
+      <c r="R44" s="207"/>
+      <c r="S44" s="207"/>
+      <c r="T44" s="207"/>
+      <c r="U44" s="207"/>
+      <c r="V44" s="207"/>
+      <c r="W44" s="207"/>
+      <c r="X44" s="207"/>
+      <c r="Y44" s="207"/>
+      <c r="Z44" s="207"/>
+      <c r="AA44" s="207"/>
+      <c r="AB44" s="207"/>
+      <c r="AC44" s="207"/>
+      <c r="AD44" s="207"/>
+      <c r="AE44" s="207"/>
+      <c r="AF44" s="207"/>
+      <c r="AG44" s="207"/>
+      <c r="AH44" s="207"/>
+      <c r="AI44" s="207"/>
+      <c r="AJ44" s="207"/>
+      <c r="AK44" s="207"/>
+      <c r="AL44" s="207"/>
+      <c r="AM44" s="207"/>
+      <c r="AN44" s="207"/>
     </row>
     <row r="45" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="19"/>
@@ -5612,21 +5614,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="196"/>
-      <c r="B1" s="196"/>
-      <c r="C1" s="196"/>
-      <c r="D1" s="196"/>
-      <c r="E1" s="196"/>
-      <c r="F1" s="196"/>
-      <c r="G1" s="196"/>
-      <c r="H1" s="196"/>
-      <c r="I1" s="196"/>
-      <c r="J1" s="196"/>
-      <c r="K1" s="196"/>
-      <c r="L1" s="196"/>
-      <c r="M1" s="196"/>
-      <c r="N1" s="196"/>
-      <c r="O1" s="196"/>
+      <c r="A1" s="217"/>
+      <c r="B1" s="217"/>
+      <c r="C1" s="217"/>
+      <c r="D1" s="217"/>
+      <c r="E1" s="217"/>
+      <c r="F1" s="217"/>
+      <c r="G1" s="217"/>
+      <c r="H1" s="217"/>
+      <c r="I1" s="217"/>
+      <c r="J1" s="217"/>
+      <c r="K1" s="217"/>
+      <c r="L1" s="217"/>
+      <c r="M1" s="217"/>
+      <c r="N1" s="217"/>
+      <c r="O1" s="217"/>
     </row>
     <row r="2" spans="1:15" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -5932,10 +5934,10 @@
     <row r="25" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="197" t="s">
+      <c r="A27" s="218" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="198"/>
+      <c r="B27" s="219"/>
       <c r="C27" s="4" t="s">
         <v>28</v>
       </c>
@@ -5944,10 +5946,10 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="194" t="s">
+      <c r="A28" s="215" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="195"/>
+      <c r="B28" s="216"/>
       <c r="C28" s="5">
         <f>'IPA Zeitplanung'!C5</f>
         <v>0</v>
@@ -5958,10 +5960,10 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="199" t="s">
+      <c r="A29" s="220" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="200"/>
+      <c r="B29" s="221"/>
       <c r="C29" s="5">
         <f>'IPA Zeitplanung'!C11</f>
         <v>0</v>
@@ -5972,10 +5974,10 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="194" t="s">
+      <c r="A30" s="215" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="195"/>
+      <c r="B30" s="216"/>
       <c r="C30" s="5">
         <f>'IPA Zeitplanung'!C15</f>
         <v>81</v>
@@ -5986,10 +5988,10 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="199" t="s">
+      <c r="A31" s="220" t="s">
         <v>8</v>
       </c>
-      <c r="B31" s="200"/>
+      <c r="B31" s="221"/>
       <c r="C31" s="5">
         <f>'IPA Zeitplanung'!C28</f>
         <v>0</v>
@@ -6000,10 +6002,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="194" t="s">
+      <c r="A32" s="215" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="195"/>
+      <c r="B32" s="216"/>
       <c r="C32" s="5">
         <f>'IPA Zeitplanung'!C33</f>
         <v>16.2</v>
@@ -6014,10 +6016,10 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="194" t="s">
+      <c r="A33" s="215" t="s">
         <v>9</v>
       </c>
-      <c r="B33" s="195"/>
+      <c r="B33" s="216"/>
       <c r="C33" s="5">
         <f>'IPA Zeitplanung'!C37</f>
         <v>0</v>

</xml_diff>